<commit_message>
Remove calc cells from data spreadsheet
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C39A857-1837-924B-BAB8-A681409083B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99701C60-4F47-5D47-82C6-9B551E33FF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1361,9 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A21B4A-A263-DF46-B91A-B4FADE2BF08E}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>

</xml_diff>

<commit_message>
Import license data to notebook
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99701C60-4F47-5D47-82C6-9B551E33FF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE1C0A-9CAF-8845-8523-58996860DE7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="149">
   <si>
     <r>
       <rPr>
@@ -918,6 +918,9 @@
   <si>
     <t>New England</t>
   </si>
+  <si>
+    <t>Resident vs Non-Resident Cost Data collected 2016-2018, not prior:</t>
+  </si>
 </sst>
 </file>
 
@@ -1361,7 +1364,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A21B4A-A263-DF46-B91A-B4FADE2BF08E}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -13145,7 +13150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3517F865-8CBE-3741-B22A-88376F7D2A2B}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13173,13 +13180,18 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -14362,3322 +14374,3475 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D88F12-E87E-FB45-A427-7B7D81090A77}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5">
         <v>2018</v>
       </c>
-      <c r="C1" s="5">
-        <f>B1-1</f>
+      <c r="D1" s="5">
+        <f>C1-1</f>
         <v>2017</v>
       </c>
-      <c r="D1" s="5">
-        <f t="shared" ref="D1:P1" si="0">C1-1</f>
+      <c r="E1" s="5">
+        <f t="shared" ref="E1:Q1" si="0">D1-1</f>
         <v>2016</v>
       </c>
-      <c r="E1" s="5">
+      <c r="F1" s="5">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="F1" s="5">
+      <c r="G1" s="5">
         <f t="shared" si="0"/>
         <v>2014</v>
       </c>
-      <c r="G1" s="5">
+      <c r="H1" s="5">
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-      <c r="H1" s="5">
+      <c r="I1" s="5">
         <f t="shared" si="0"/>
         <v>2012</v>
       </c>
-      <c r="I1" s="5">
+      <c r="J1" s="5">
         <f t="shared" si="0"/>
         <v>2011</v>
       </c>
-      <c r="J1" s="5">
+      <c r="K1" s="5">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
-      <c r="K1" s="5">
+      <c r="L1" s="5">
         <f t="shared" si="0"/>
         <v>2009</v>
       </c>
-      <c r="L1" s="5">
+      <c r="M1" s="5">
         <f t="shared" si="0"/>
         <v>2008</v>
       </c>
-      <c r="M1" s="5">
+      <c r="N1" s="5">
         <f t="shared" si="0"/>
         <v>2007</v>
       </c>
-      <c r="N1" s="5">
+      <c r="O1" s="5">
         <f t="shared" si="0"/>
         <v>2006</v>
       </c>
-      <c r="O1" s="5">
+      <c r="P1" s="5">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="P1" s="5">
+      <c r="Q1" s="5">
         <f t="shared" si="0"/>
         <v>2004</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="6">
         <f>'2018'!E2</f>
         <v>352780</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="6">
         <f>'2017'!E2</f>
         <v>402002</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <f>'2016'!E2</f>
         <v>362739</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="6">
         <f>'2015'!E2</f>
         <v>310644</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <f>'2014'!E2</f>
         <v>287352</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <f>'2013'!E2</f>
         <v>278400</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <f>'2012'!E2</f>
         <v>353266</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <f>'2011'!E2</f>
         <v>250073</v>
       </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <f>'2010'!E2</f>
         <v>239557</v>
       </c>
-      <c r="K2" s="6">
+      <c r="L2" s="6">
         <f>'2009'!E2</f>
         <v>227588</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
         <f>'2008'!E2</f>
         <v>227588</v>
       </c>
-      <c r="M2" s="6">
+      <c r="N2" s="6">
         <f>'2007'!E2</f>
         <v>227701</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2" s="6">
         <f>'2006'!E2</f>
         <v>223048</v>
       </c>
-      <c r="O2" s="6">
+      <c r="P2" s="6">
         <f>'2005'!E2</f>
         <v>223215</v>
       </c>
-      <c r="P2" s="6">
+      <c r="Q2" s="6">
         <f>'2004'!E2</f>
         <v>222544</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="6">
         <f>'2018'!E3</f>
         <v>579944</v>
       </c>
-      <c r="C3" s="6">
+      <c r="D3" s="6">
         <f>'2017'!E3</f>
         <v>587686</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <f>'2016'!E3</f>
         <v>604043</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <f>'2015'!E3</f>
         <v>599876</v>
       </c>
-      <c r="F3" s="6">
+      <c r="G3" s="6">
         <f>'2014'!E3</f>
         <v>597095</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <f>'2013'!E3</f>
         <v>609156</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <f>'2012'!E3</f>
         <v>607121</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <f>'2011'!E3</f>
         <v>625962</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <f>'2010'!E3</f>
         <v>287455</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <f>'2009'!E3</f>
         <v>291183</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <f>'2008'!E3</f>
         <v>283899</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <f>'2007'!E3</f>
         <v>289660</v>
       </c>
-      <c r="N3" s="6">
+      <c r="O3" s="6">
         <f>'2006'!E3</f>
         <v>302220</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="6">
         <f>'2005'!E3</f>
         <v>299224</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="6">
         <f>'2004'!E3</f>
         <v>303217</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="6">
         <f>'2018'!E4</f>
         <v>517046</v>
       </c>
-      <c r="C4" s="6">
+      <c r="D4" s="6">
         <f>'2017'!E4</f>
         <v>533585</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <f>'2016'!E4</f>
         <v>521098</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="6">
         <f>'2015'!E4</f>
         <v>498919</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="6">
         <f>'2014'!E4</f>
         <v>492479</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="6">
         <f>'2013'!E4</f>
         <v>475057</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <f>'2012'!E4</f>
         <v>468656</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <f>'2011'!E4</f>
         <v>481943</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <f>'2010'!E4</f>
         <v>434479</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <f>'2009'!E4</f>
         <v>424003</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <f>'2008'!E4</f>
         <v>388698</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <f>'2007'!E4</f>
         <v>421548</v>
       </c>
-      <c r="N4" s="6">
+      <c r="O4" s="6">
         <f>'2006'!E4</f>
         <v>422822</v>
       </c>
-      <c r="O4" s="6">
+      <c r="P4" s="6">
         <f>'2005'!E4</f>
         <v>438108</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <f>'2004'!E4</f>
         <v>464563</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="6">
         <f>'2018'!E5</f>
         <v>517747</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="6">
         <f>'2017'!E5</f>
         <v>540038</v>
       </c>
-      <c r="D5" s="6">
+      <c r="E5" s="6">
         <f>'2016'!E5</f>
         <v>446402</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="6">
         <f>'2015'!E5</f>
         <v>422136</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <f>'2014'!E5</f>
         <v>409672</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <f>'2013'!E5</f>
         <v>414623</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <f>'2012'!E5</f>
         <v>409680</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <f>'2011'!E5</f>
         <v>411617</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <f>'2010'!E5</f>
         <v>419161</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <f>'2009'!E5</f>
         <v>428669</v>
       </c>
-      <c r="L5" s="6">
+      <c r="M5" s="6">
         <f>'2008'!E5</f>
         <v>428669</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <f>'2007'!E5</f>
         <v>415432</v>
       </c>
-      <c r="N5" s="6">
+      <c r="O5" s="6">
         <f>'2006'!E5</f>
         <v>391973</v>
       </c>
-      <c r="O5" s="6">
+      <c r="P5" s="6">
         <f>'2005'!E5</f>
         <v>396299</v>
       </c>
-      <c r="P5" s="6">
+      <c r="Q5" s="6">
         <f>'2004'!E5</f>
         <v>406210</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="6">
         <f>'2018'!E6</f>
         <v>1030160</v>
       </c>
-      <c r="C6" s="6">
+      <c r="D6" s="6">
         <f>'2017'!E6</f>
         <v>1054000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <f>'2016'!E6</f>
         <v>1035351</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="6">
         <f>'2015'!E6</f>
         <v>847348</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="6">
         <f>'2014'!E6</f>
         <v>847348</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="6">
         <f>'2013'!E6</f>
         <v>834739</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <f>'2012'!E6</f>
         <v>875297</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <f>'2011'!E6</f>
         <v>828735</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <f>'2010'!E6</f>
         <v>836694</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <f>'2009'!E6</f>
         <v>841239</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <f>'2008'!E6</f>
         <v>830700</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <f>'2007'!E6</f>
         <v>831531</v>
       </c>
-      <c r="N6" s="6">
+      <c r="O6" s="6">
         <f>'2006'!E6</f>
         <v>833977</v>
       </c>
-      <c r="O6" s="6">
+      <c r="P6" s="6">
         <f>'2005'!E6</f>
         <v>858691</v>
       </c>
-      <c r="P6" s="6">
+      <c r="Q6" s="6">
         <f>'2004'!E6</f>
         <v>868209</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="6">
         <f>'2018'!E7</f>
         <v>568764</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="6">
         <f>'2017'!E7</f>
         <v>563870</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <f>'2016'!E7</f>
         <v>545216</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <f>'2015'!E7</f>
         <v>530736</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G7" s="6">
         <f>'2014'!E7</f>
         <v>528174</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <f>'2013'!E7</f>
         <v>537371</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <f>'2012'!E7</f>
         <v>535893</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <f>'2011'!E7</f>
         <v>538734</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <f>'2010'!E7</f>
         <v>538734</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <f>'2009'!E7</f>
         <v>566298</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <f>'2008'!E7</f>
         <v>566298</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <f>'2007'!E7</f>
         <v>581235</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="6">
         <f>'2006'!E7</f>
         <v>581733</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <f>'2005'!E7</f>
         <v>553899</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <f>'2004'!E7</f>
         <v>548011</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="6">
         <f>'2018'!E8</f>
         <v>128232</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D8" s="6">
         <f>'2017'!E8</f>
         <v>125402</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <f>'2016'!E8</f>
         <v>131331</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <f>'2015'!E8</f>
         <v>128666</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <f>'2014'!E8</f>
         <v>118798</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <f>'2013'!E8</f>
         <v>127612</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <f>'2012'!E8</f>
         <v>135711</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <f>'2011'!E8</f>
         <v>130361</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <f>'2010'!E8</f>
         <v>124647</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <f>'2009'!E8</f>
         <v>127746</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <f>'2008'!E8</f>
         <v>127746</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <f>'2007'!E8</f>
         <v>129443</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="6">
         <f>'2006'!E8</f>
         <v>133311</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <f>'2005'!E8</f>
         <v>134294</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <f>'2004'!E8</f>
         <v>143358</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="6">
         <f>'2018'!E9</f>
         <v>59440</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D9" s="6">
         <f>'2017'!E9</f>
         <v>60203</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <f>'2016'!E9</f>
         <v>58299</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <f>'2015'!E9</f>
         <v>57060</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <f>'2014'!E9</f>
         <v>29513</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <f>'2013'!E9</f>
         <v>42341</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <f>'2012'!E9</f>
         <v>44087</v>
       </c>
-      <c r="I9" s="6">
+      <c r="J9" s="6">
         <f>'2011'!E9</f>
         <v>45503</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <f>'2010'!E9</f>
         <v>47562</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <f>'2009'!E9</f>
         <v>44875</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <f>'2008'!E9</f>
         <v>44956</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <f>'2007'!E9</f>
         <v>30016</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="6">
         <f>'2006'!E9</f>
         <v>28968</v>
       </c>
-      <c r="O9" s="6">
+      <c r="P9" s="6">
         <f>'2005'!E9</f>
         <v>31847</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <f>'2004'!E9</f>
         <v>36000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="6">
         <f>'2018'!E10</f>
         <v>331709</v>
       </c>
-      <c r="C10" s="6">
+      <c r="D10" s="6">
         <f>'2017'!E10</f>
         <v>384611</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="6">
         <f>'2016'!E10</f>
         <v>353926</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="6">
         <f>'2015'!E10</f>
         <v>380398</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <f>'2014'!E10</f>
         <v>356262</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <f>'2013'!E10</f>
         <v>369998</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <f>'2012'!E10</f>
         <v>326835</v>
       </c>
-      <c r="I10" s="6">
+      <c r="J10" s="6">
         <f>'2011'!E10</f>
         <v>327973</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <f>'2010'!E10</f>
         <v>322445</v>
       </c>
-      <c r="K10" s="6">
+      <c r="L10" s="6">
         <f>'2009'!E10</f>
         <v>159070</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <f>'2008'!E10</f>
         <v>280643</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="6">
         <f>'2007'!E10</f>
         <v>294724</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="6">
         <f>'2006'!E10</f>
         <v>324353</v>
       </c>
-      <c r="O10" s="6">
+      <c r="P10" s="6">
         <f>'2005'!E10</f>
         <v>321179</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <f>'2004'!E10</f>
         <v>338769</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="6">
         <f>'2018'!E11</f>
         <v>1463441</v>
       </c>
-      <c r="C11" s="6">
+      <c r="D11" s="6">
         <f>'2017'!E11</f>
         <v>1458621</v>
       </c>
-      <c r="D11" s="6">
+      <c r="E11" s="6">
         <f>'2016'!E11</f>
         <v>1456426</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="6">
         <f>'2015'!E11</f>
         <v>1058503</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <f>'2014'!E11</f>
         <v>1028840</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <f>'2013'!E11</f>
         <v>964738</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <f>'2012'!E11</f>
         <v>1069502</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <f>'2011'!E11</f>
         <v>1185594</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <f>'2010'!E11</f>
         <v>1254371</v>
       </c>
-      <c r="K11" s="6">
+      <c r="L11" s="6">
         <f>'2009'!E11</f>
         <v>11235990</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="6">
         <f>'2008'!E11</f>
         <v>1235114</v>
       </c>
-      <c r="M11" s="6">
+      <c r="N11" s="6">
         <f>'2007'!E11</f>
         <v>989964</v>
       </c>
-      <c r="N11" s="6">
+      <c r="O11" s="6">
         <f>'2006'!E11</f>
         <v>989964</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <f>'2005'!E11</f>
         <v>954126</v>
       </c>
-      <c r="P11" s="6">
+      <c r="Q11" s="6">
         <f>'2004'!E11</f>
         <v>957739</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="6">
         <f>'2018'!E12</f>
         <v>11802</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="6">
         <f>'2017'!E12</f>
         <v>12521</v>
       </c>
-      <c r="D12" s="6">
+      <c r="E12" s="6">
         <f>'2016'!E12</f>
         <v>12202</v>
       </c>
-      <c r="E12" s="6">
+      <c r="F12" s="6">
         <f>'2015'!E12</f>
         <v>11486</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <f>'2014'!E12</f>
         <v>7970</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <f>'2013'!E12</f>
         <v>10653</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <f>'2012'!E12</f>
         <v>10421</v>
       </c>
-      <c r="I12" s="6">
+      <c r="J12" s="6">
         <f>'2011'!E12</f>
         <v>9653</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <f>'2010'!E12</f>
         <v>7803</v>
       </c>
-      <c r="K12" s="6">
+      <c r="L12" s="6">
         <f>'2009'!E12</f>
         <v>7812</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <f>'2008'!E12</f>
         <v>9372</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N12" s="6">
         <f>'2007'!E12</f>
         <v>8292</v>
       </c>
-      <c r="N12" s="6">
+      <c r="O12" s="6">
         <f>'2006'!E12</f>
         <v>8309</v>
       </c>
-      <c r="O12" s="6">
+      <c r="P12" s="6">
         <f>'2005'!E12</f>
         <v>8900</v>
       </c>
-      <c r="P12" s="6">
+      <c r="Q12" s="6">
         <f>'2004'!E12</f>
         <v>9540</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="6">
         <f>'2018'!E13</f>
         <v>583884</v>
       </c>
-      <c r="C13" s="6">
+      <c r="D13" s="6">
         <f>'2017'!E13</f>
         <v>606302</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="6">
         <f>'2016'!E13</f>
         <v>601508</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="6">
         <f>'2015'!E13</f>
         <v>841793</v>
       </c>
-      <c r="F13" s="6">
+      <c r="G13" s="6">
         <f>'2014'!E13</f>
         <v>860078</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <f>'2013'!E13</f>
         <v>876313</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <f>'2012'!E13</f>
         <v>943322</v>
       </c>
-      <c r="I13" s="6">
+      <c r="J13" s="6">
         <f>'2011'!E13</f>
         <v>965859</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <f>'2010'!E13</f>
         <v>971151</v>
       </c>
-      <c r="K13" s="6">
+      <c r="L13" s="6">
         <f>'2009'!E13</f>
         <v>990844</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <f>'2008'!E13</f>
         <v>1009364</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="6">
         <f>'2007'!E13</f>
         <v>980685</v>
       </c>
-      <c r="N13" s="6">
+      <c r="O13" s="6">
         <f>'2006'!E13</f>
         <v>962830</v>
       </c>
-      <c r="O13" s="6">
+      <c r="P13" s="6">
         <f>'2005'!E13</f>
         <v>871914</v>
       </c>
-      <c r="P13" s="6">
+      <c r="Q13" s="6">
         <f>'2004'!E13</f>
         <v>847182</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="6">
         <f>'2018'!E14</f>
         <v>1206997</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D14" s="6">
         <f>'2017'!E14</f>
         <v>1151159</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <f>'2016'!E14</f>
         <v>1081968</v>
       </c>
-      <c r="E14" s="6">
+      <c r="F14" s="6">
         <f>'2015'!E14</f>
         <v>1029816</v>
       </c>
-      <c r="F14" s="6">
+      <c r="G14" s="6">
         <f>'2014'!E14</f>
         <v>1015884</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <f>'2013'!E14</f>
         <v>958761</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <f>'2012'!E14</f>
         <v>978693</v>
       </c>
-      <c r="I14" s="6">
+      <c r="J14" s="6">
         <f>'2011'!E14</f>
         <v>946859</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <f>'2010'!E14</f>
         <v>959296</v>
       </c>
-      <c r="K14" s="6">
+      <c r="L14" s="6">
         <f>'2009'!E14</f>
         <v>913007</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <f>'2008'!E14</f>
         <v>913007</v>
       </c>
-      <c r="M14" s="6">
+      <c r="N14" s="6">
         <f>'2007'!E14</f>
         <v>902194</v>
       </c>
-      <c r="N14" s="6">
+      <c r="O14" s="6">
         <f>'2006'!E14</f>
         <v>846824</v>
       </c>
-      <c r="O14" s="6">
+      <c r="P14" s="6">
         <f>'2005'!E14</f>
         <v>824093</v>
       </c>
-      <c r="P14" s="6">
+      <c r="Q14" s="6">
         <f>'2004'!E14</f>
         <v>812609</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="6">
         <f>'2018'!E15</f>
         <v>1286532</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D15" s="6">
         <f>'2017'!E15</f>
         <v>1372038</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="6">
         <f>'2016'!E15</f>
         <v>1563709</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="6">
         <f>'2015'!E15</f>
         <v>1440993</v>
       </c>
-      <c r="F15" s="6">
+      <c r="G15" s="6">
         <f>'2014'!E15</f>
         <v>1436679</v>
       </c>
-      <c r="G15" s="6">
+      <c r="H15" s="6">
         <f>'2013'!E15</f>
         <v>1448776</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="6">
         <f>'2012'!E15</f>
         <v>1489893</v>
       </c>
-      <c r="I15" s="6">
+      <c r="J15" s="6">
         <f>'2011'!E15</f>
         <v>1520262</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <f>'2010'!E15</f>
         <v>1467858</v>
       </c>
-      <c r="K15" s="6">
+      <c r="L15" s="6">
         <f>'2009'!E15</f>
         <v>1431133</v>
       </c>
-      <c r="L15" s="6">
+      <c r="M15" s="6">
         <f>'2008'!E15</f>
         <v>1431133</v>
       </c>
-      <c r="M15" s="6">
+      <c r="N15" s="6">
         <f>'2007'!E15</f>
         <v>1279714</v>
       </c>
-      <c r="N15" s="6">
+      <c r="O15" s="6">
         <f>'2006'!E15</f>
         <v>1221932</v>
       </c>
-      <c r="O15" s="6">
+      <c r="P15" s="6">
         <f>'2005'!E15</f>
         <v>1102059</v>
       </c>
-      <c r="P15" s="6">
+      <c r="Q15" s="6">
         <f>'2004'!E15</f>
         <v>1159442</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="6">
         <f>'2018'!E16</f>
         <v>404739</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D16" s="6">
         <f>'2017'!E16</f>
         <v>417124</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <f>'2016'!E16</f>
         <v>426349</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="6">
         <f>'2015'!E16</f>
         <v>423318</v>
       </c>
-      <c r="F16" s="6">
+      <c r="G16" s="6">
         <f>'2014'!E16</f>
         <v>497715</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="6">
         <f>'2013'!E16</f>
         <v>491802</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <f>'2012'!E16</f>
         <v>489040</v>
       </c>
-      <c r="I16" s="6">
+      <c r="J16" s="6">
         <f>'2011'!E16</f>
         <v>472874</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <f>'2010'!E16</f>
         <v>451979</v>
       </c>
-      <c r="K16" s="6">
+      <c r="L16" s="6">
         <f>'2009'!E16</f>
         <v>460800</v>
       </c>
-      <c r="L16" s="6">
+      <c r="M16" s="6">
         <f>'2008'!E16</f>
         <v>460800</v>
       </c>
-      <c r="M16" s="6">
+      <c r="N16" s="6">
         <f>'2007'!E16</f>
         <v>445588</v>
       </c>
-      <c r="N16" s="6">
+      <c r="O16" s="6">
         <f>'2006'!E16</f>
         <v>552135</v>
       </c>
-      <c r="O16" s="6">
+      <c r="P16" s="6">
         <f>'2005'!E16</f>
         <v>436206</v>
       </c>
-      <c r="P16" s="6">
+      <c r="Q16" s="6">
         <f>'2004'!E16</f>
         <v>661769</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="6">
         <f>'2018'!E17</f>
         <v>519875</v>
       </c>
-      <c r="C17" s="6">
+      <c r="D17" s="6">
         <f>'2017'!E17</f>
         <v>517519</v>
       </c>
-      <c r="D17" s="6">
+      <c r="E17" s="6">
         <f>'2016'!E17</f>
         <v>520232</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="6">
         <f>'2015'!E17</f>
         <v>493665</v>
       </c>
-      <c r="F17" s="6">
+      <c r="G17" s="6">
         <f>'2014'!E17</f>
         <v>471678</v>
       </c>
-      <c r="G17" s="6">
+      <c r="H17" s="6">
         <f>'2013'!E17</f>
         <v>489223</v>
       </c>
-      <c r="H17" s="6">
+      <c r="I17" s="6">
         <f>'2012'!E17</f>
         <v>514090</v>
       </c>
-      <c r="I17" s="6">
+      <c r="J17" s="6">
         <f>'2011'!E17</f>
         <v>489728</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <f>'2010'!E17</f>
         <v>489728</v>
       </c>
-      <c r="K17" s="6">
+      <c r="L17" s="6">
         <f>'2009'!E17</f>
         <v>485091</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="6">
         <f>'2008'!E17</f>
         <v>481477</v>
       </c>
-      <c r="M17" s="6">
+      <c r="N17" s="6">
         <f>'2007'!E17</f>
         <v>470973</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="6">
         <f>'2006'!E17</f>
         <v>470884</v>
       </c>
-      <c r="O17" s="6">
+      <c r="P17" s="6">
         <f>'2005'!E17</f>
         <v>468946</v>
       </c>
-      <c r="P17" s="6">
+      <c r="Q17" s="6">
         <f>'2004'!E17</f>
         <v>471423</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="6">
         <f>'2018'!E18</f>
         <v>614742</v>
       </c>
-      <c r="C18" s="6">
+      <c r="D18" s="6">
         <f>'2017'!E18</f>
         <v>614120</v>
       </c>
-      <c r="D18" s="6">
+      <c r="E18" s="6">
         <f>'2016'!E18</f>
         <v>617129</v>
       </c>
-      <c r="E18" s="6">
+      <c r="F18" s="6">
         <f>'2015'!E18</f>
         <v>594389</v>
       </c>
-      <c r="F18" s="6">
+      <c r="G18" s="6">
         <f>'2014'!E18</f>
         <v>578862</v>
       </c>
-      <c r="G18" s="6">
+      <c r="H18" s="6">
         <f>'2013'!E18</f>
         <v>566072</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="6">
         <f>'2012'!E18</f>
         <v>579026</v>
       </c>
-      <c r="I18" s="6">
+      <c r="J18" s="6">
         <f>'2011'!E18</f>
         <v>537982</v>
       </c>
-      <c r="J18" s="6">
+      <c r="K18" s="6">
         <f>'2010'!E18</f>
         <v>562986</v>
       </c>
-      <c r="K18" s="6">
+      <c r="L18" s="6">
         <f>'2009'!E18</f>
         <v>615832</v>
       </c>
-      <c r="L18" s="6">
+      <c r="M18" s="6">
         <f>'2008'!E18</f>
         <v>615832</v>
       </c>
-      <c r="M18" s="6">
+      <c r="N18" s="6">
         <f>'2007'!E18</f>
         <v>599548</v>
       </c>
-      <c r="N18" s="6">
+      <c r="O18" s="6">
         <f>'2006'!E18</f>
         <v>654743</v>
       </c>
-      <c r="O18" s="6">
+      <c r="P18" s="6">
         <f>'2005'!E18</f>
         <v>666695</v>
       </c>
-      <c r="P18" s="6">
+      <c r="Q18" s="6">
         <f>'2004'!E18</f>
         <v>684768</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="6">
         <f>'2018'!E19</f>
         <v>658659</v>
       </c>
-      <c r="C19" s="6">
+      <c r="D19" s="6">
         <f>'2017'!E19</f>
         <v>676500</v>
       </c>
-      <c r="D19" s="6">
+      <c r="E19" s="6">
         <f>'2016'!E19</f>
         <v>677582</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="6">
         <f>'2015'!E19</f>
         <v>659165</v>
       </c>
-      <c r="F19" s="6">
+      <c r="G19" s="6">
         <f>'2014'!E19</f>
         <v>645912</v>
       </c>
-      <c r="G19" s="6">
+      <c r="H19" s="6">
         <f>'2013'!E19</f>
         <v>621388</v>
       </c>
-      <c r="H19" s="6">
+      <c r="I19" s="6">
         <f>'2012'!E19</f>
         <v>599516</v>
       </c>
-      <c r="I19" s="6">
+      <c r="J19" s="6">
         <f>'2011'!E19</f>
         <v>270713</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
         <f>'2010'!E19</f>
         <v>264939</v>
       </c>
-      <c r="K19" s="6">
+      <c r="L19" s="6">
         <f>'2009'!E19</f>
         <v>257134</v>
       </c>
-      <c r="L19" s="6">
+      <c r="M19" s="6">
         <f>'2008'!E19</f>
         <v>237618</v>
       </c>
-      <c r="M19" s="6">
+      <c r="N19" s="6">
         <f>'2007'!E19</f>
         <v>761795</v>
       </c>
-      <c r="N19" s="6">
+      <c r="O19" s="6">
         <f>'2006'!E19</f>
         <v>602229</v>
       </c>
-      <c r="O19" s="6">
+      <c r="P19" s="6">
         <f>'2005'!E19</f>
         <v>596557</v>
       </c>
-      <c r="P19" s="6">
+      <c r="Q19" s="6">
         <f>'2004'!E19</f>
         <v>623871</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="6">
         <f>'2018'!E20</f>
         <v>261556</v>
       </c>
-      <c r="C20" s="6">
+      <c r="D20" s="6">
         <f>'2017'!E20</f>
         <v>252212</v>
       </c>
-      <c r="D20" s="6">
+      <c r="E20" s="6">
         <f>'2016'!E20</f>
         <v>253725</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="6">
         <f>'2015'!E20</f>
         <v>246509</v>
       </c>
-      <c r="F20" s="6">
+      <c r="G20" s="6">
         <f>'2014'!E20</f>
         <v>250778</v>
       </c>
-      <c r="G20" s="6">
+      <c r="H20" s="6">
         <f>'2013'!E20</f>
         <v>227487</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="6">
         <f>'2012'!E20</f>
         <v>390013</v>
       </c>
-      <c r="I20" s="6">
+      <c r="J20" s="6">
         <f>'2011'!E20</f>
         <v>234851</v>
       </c>
-      <c r="J20" s="6">
+      <c r="K20" s="6">
         <f>'2010'!E20</f>
         <v>224446</v>
       </c>
-      <c r="K20" s="6">
+      <c r="L20" s="6">
         <f>'2009'!E20</f>
         <v>220645</v>
       </c>
-      <c r="L20" s="6">
+      <c r="M20" s="6">
         <f>'2008'!E20</f>
         <v>220015</v>
       </c>
-      <c r="M20" s="6">
+      <c r="N20" s="6">
         <f>'2007'!E20</f>
         <v>222513</v>
       </c>
-      <c r="N20" s="6">
+      <c r="O20" s="6">
         <f>'2006'!E20</f>
         <v>235117</v>
       </c>
-      <c r="O20" s="6">
+      <c r="P20" s="6">
         <f>'2005'!E20</f>
         <v>210350</v>
       </c>
-      <c r="P20" s="6">
+      <c r="Q20" s="6">
         <f>'2004'!E20</f>
         <v>224099</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="6">
         <f>'2018'!E21</f>
         <v>345211</v>
       </c>
-      <c r="C21" s="6">
+      <c r="D21" s="6">
         <f>'2017'!E21</f>
         <v>343495</v>
       </c>
-      <c r="D21" s="6">
+      <c r="E21" s="6">
         <f>'2016'!E21</f>
         <v>129376</v>
       </c>
-      <c r="E21" s="6">
+      <c r="F21" s="6">
         <f>'2015'!E21</f>
         <v>339319</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <f>'2014'!E21</f>
         <v>351004</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <f>'2013'!E21</f>
         <v>0</v>
       </c>
-      <c r="H21" s="6">
+      <c r="I21" s="6">
         <f>'2012'!E21</f>
         <v>323275</v>
       </c>
-      <c r="I21" s="6">
+      <c r="J21" s="6">
         <f>'2011'!E21</f>
         <v>326021</v>
       </c>
-      <c r="J21" s="6">
+      <c r="K21" s="6">
         <f>'2010'!E21</f>
         <v>321774</v>
       </c>
-      <c r="K21" s="6">
+      <c r="L21" s="6">
         <f>'2009'!E21</f>
         <v>338748</v>
       </c>
-      <c r="L21" s="6">
+      <c r="M21" s="6">
         <f>'2008'!E21</f>
         <v>303779</v>
       </c>
-      <c r="M21" s="6">
+      <c r="N21" s="6">
         <f>'2007'!E21</f>
         <v>310730</v>
       </c>
-      <c r="N21" s="6">
+      <c r="O21" s="6">
         <f>'2006'!E21</f>
         <v>168356</v>
       </c>
-      <c r="O21" s="6">
+      <c r="P21" s="6">
         <f>'2005'!E21</f>
         <v>293921</v>
       </c>
-      <c r="P21" s="6">
+      <c r="Q21" s="6">
         <f>'2004'!E21</f>
         <v>329707</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="6">
         <f>'2018'!E22</f>
         <v>249090</v>
       </c>
-      <c r="C22" s="6">
+      <c r="D22" s="6">
         <f>'2017'!E22</f>
         <v>252763</v>
       </c>
-      <c r="D22" s="6">
+      <c r="E22" s="6">
         <f>'2016'!E22</f>
         <v>259854</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="6">
         <f>'2015'!E22</f>
         <v>253477</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <f>'2014'!E22</f>
         <v>247098</v>
       </c>
-      <c r="G22" s="6">
+      <c r="H22" s="6">
         <f>'2013'!E22</f>
         <v>251988</v>
       </c>
-      <c r="H22" s="6">
+      <c r="I22" s="6">
         <f>'2012'!E22</f>
         <v>261404</v>
       </c>
-      <c r="I22" s="6">
+      <c r="J22" s="6">
         <f>'2011'!E22</f>
         <v>264067</v>
       </c>
-      <c r="J22" s="6">
+      <c r="K22" s="6">
         <f>'2010'!E22</f>
         <v>276493</v>
       </c>
-      <c r="K22" s="6">
+      <c r="L22" s="6">
         <f>'2009'!E22</f>
         <v>278775</v>
       </c>
-      <c r="L22" s="6">
+      <c r="M22" s="6">
         <f>'2008'!E22</f>
         <v>278775</v>
       </c>
-      <c r="M22" s="6">
+      <c r="N22" s="6">
         <f>'2007'!E22</f>
         <v>253863</v>
       </c>
-      <c r="N22" s="6">
+      <c r="O22" s="6">
         <f>'2006'!E22</f>
         <v>260362</v>
       </c>
-      <c r="O22" s="6">
+      <c r="P22" s="6">
         <f>'2005'!E22</f>
         <v>265605</v>
       </c>
-      <c r="P22" s="6">
+      <c r="Q22" s="6">
         <f>'2004'!E22</f>
         <v>259968</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="6">
         <f>'2018'!E23</f>
         <v>2224170</v>
       </c>
-      <c r="C23" s="6">
+      <c r="D23" s="6">
         <f>'2017'!E23</f>
         <v>2268341</v>
       </c>
-      <c r="D23" s="6">
+      <c r="E23" s="6">
         <f>'2016'!E23</f>
         <v>1884724</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="6">
         <f>'2015'!E23</f>
         <v>1896927</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <f>'2014'!E23</f>
         <v>1906410</v>
       </c>
-      <c r="G23" s="6">
+      <c r="H23" s="6">
         <f>'2013'!E23</f>
         <v>1946100</v>
       </c>
-      <c r="H23" s="6">
+      <c r="I23" s="6">
         <f>'2012'!E23</f>
         <v>2005244</v>
       </c>
-      <c r="I23" s="6">
+      <c r="J23" s="6">
         <f>'2011'!E23</f>
         <v>2009229</v>
       </c>
-      <c r="J23" s="6">
+      <c r="K23" s="6">
         <f>'2010'!E23</f>
         <v>1975715</v>
       </c>
-      <c r="K23" s="6">
+      <c r="L23" s="6">
         <f>'2009'!E23</f>
         <v>1986632</v>
       </c>
-      <c r="L23" s="6">
+      <c r="M23" s="6">
         <f>'2008'!E23</f>
         <v>2030036</v>
       </c>
-      <c r="M23" s="6">
+      <c r="N23" s="6">
         <f>'2007'!E23</f>
         <v>2018817</v>
       </c>
-      <c r="N23" s="6">
+      <c r="O23" s="6">
         <f>'2006'!E23</f>
         <v>2174714</v>
       </c>
-      <c r="O23" s="6">
+      <c r="P23" s="6">
         <f>'2005'!E23</f>
         <v>2266231</v>
       </c>
-      <c r="P23" s="6">
+      <c r="Q23" s="6">
         <f>'2004'!E23</f>
         <v>2272955</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="6">
         <f>'2018'!E24</f>
         <v>1421004</v>
       </c>
-      <c r="C24" s="6">
+      <c r="D24" s="6">
         <f>'2017'!E24</f>
         <v>1413430</v>
       </c>
-      <c r="D24" s="6">
+      <c r="E24" s="6">
         <f>'2016'!E24</f>
         <v>1486362</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="6">
         <f>'2015'!E24</f>
         <v>1571600</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <f>'2014'!E24</f>
         <v>1525137</v>
       </c>
-      <c r="G24" s="6">
+      <c r="H24" s="6">
         <f>'2013'!E24</f>
         <v>1553789</v>
       </c>
-      <c r="H24" s="6">
+      <c r="I24" s="6">
         <f>'2012'!E24</f>
         <v>1424718</v>
       </c>
-      <c r="I24" s="6">
+      <c r="J24" s="6">
         <f>'2011'!E24</f>
         <v>1471568</v>
       </c>
-      <c r="J24" s="6">
+      <c r="K24" s="6">
         <f>'2010'!E24</f>
         <v>1419876</v>
       </c>
-      <c r="K24" s="6">
+      <c r="L24" s="6">
         <f>'2009'!E24</f>
         <v>1456775</v>
       </c>
-      <c r="L24" s="6">
+      <c r="M24" s="6">
         <f>'2008'!E24</f>
         <v>1456775</v>
       </c>
-      <c r="M24" s="6">
+      <c r="N24" s="6">
         <f>'2007'!E24</f>
         <v>1377389</v>
       </c>
-      <c r="N24" s="6">
+      <c r="O24" s="6">
         <f>'2006'!E24</f>
         <v>1397641</v>
       </c>
-      <c r="O24" s="6">
+      <c r="P24" s="6">
         <f>'2005'!E24</f>
         <v>1413759</v>
       </c>
-      <c r="P24" s="6">
+      <c r="Q24" s="6">
         <f>'2004'!E24</f>
         <v>1594619</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="6">
         <f>'2018'!E25</f>
         <v>1782319</v>
       </c>
-      <c r="C25" s="6">
+      <c r="D25" s="6">
         <f>'2017'!E25</f>
         <v>1782319</v>
       </c>
-      <c r="D25" s="6">
+      <c r="E25" s="6">
         <f>'2016'!E25</f>
         <v>1827753</v>
       </c>
-      <c r="E25" s="6">
+      <c r="F25" s="6">
         <f>'2015'!E25</f>
         <v>1831083</v>
       </c>
-      <c r="F25" s="6">
+      <c r="G25" s="6">
         <f>'2014'!E25</f>
         <v>1787229</v>
       </c>
-      <c r="G25" s="6">
+      <c r="H25" s="6">
         <f>'2013'!E25</f>
         <v>1765901</v>
       </c>
-      <c r="H25" s="6">
+      <c r="I25" s="6">
         <f>'2012'!E25</f>
         <v>1776575</v>
       </c>
-      <c r="I25" s="6">
+      <c r="J25" s="6">
         <f>'2011'!E25</f>
         <v>1762735</v>
       </c>
-      <c r="J25" s="6">
+      <c r="K25" s="6">
         <f>'2010'!E25</f>
         <v>1728471</v>
       </c>
-      <c r="K25" s="6">
+      <c r="L25" s="6">
         <f>'2009'!E25</f>
         <v>1735761</v>
       </c>
-      <c r="L25" s="6">
+      <c r="M25" s="6">
         <f>'2008'!E25</f>
         <v>1736304</v>
       </c>
-      <c r="M25" s="6">
+      <c r="N25" s="6">
         <f>'2007'!E25</f>
         <v>1731058</v>
       </c>
-      <c r="N25" s="6">
+      <c r="O25" s="6">
         <f>'2006'!E25</f>
         <v>1742387</v>
       </c>
-      <c r="O25" s="6">
+      <c r="P25" s="6">
         <f>'2005'!E25</f>
         <v>1230036</v>
       </c>
-      <c r="P25" s="6">
+      <c r="Q25" s="6">
         <f>'2004'!E25</f>
         <v>1167886</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="6">
         <f>'2018'!E26</f>
         <v>426726</v>
       </c>
-      <c r="C26" s="6">
+      <c r="D26" s="6">
         <f>'2017'!E26</f>
         <v>428478</v>
       </c>
-      <c r="D26" s="6">
+      <c r="E26" s="6">
         <f>'2016'!E26</f>
         <v>433090</v>
       </c>
-      <c r="E26" s="6">
+      <c r="F26" s="6">
         <f>'2015'!E26</f>
         <v>418042</v>
       </c>
-      <c r="F26" s="6">
+      <c r="G26" s="6">
         <f>'2014'!E26</f>
         <v>340714</v>
       </c>
-      <c r="G26" s="6">
+      <c r="H26" s="6">
         <f>'2013'!E26</f>
         <v>245028</v>
       </c>
-      <c r="H26" s="6">
+      <c r="I26" s="6">
         <f>'2012'!E26</f>
         <v>249109</v>
       </c>
-      <c r="I26" s="6">
+      <c r="J26" s="6">
         <f>'2011'!E26</f>
         <v>259045</v>
       </c>
-      <c r="J26" s="6">
+      <c r="K26" s="6">
         <f>'2010'!E26</f>
         <v>362948</v>
       </c>
-      <c r="K26" s="6">
+      <c r="L26" s="6">
         <f>'2009'!E26</f>
         <v>333364</v>
       </c>
-      <c r="L26" s="6">
+      <c r="M26" s="6">
         <f>'2008'!E26</f>
         <v>314223</v>
       </c>
-      <c r="M26" s="6">
+      <c r="N26" s="6">
         <f>'2007'!E26</f>
         <v>274680</v>
       </c>
-      <c r="N26" s="6">
+      <c r="O26" s="6">
         <f>'2006'!E26</f>
         <v>279905</v>
       </c>
-      <c r="O26" s="6">
+      <c r="P26" s="6">
         <f>'2005'!E26</f>
         <v>278688</v>
       </c>
-      <c r="P26" s="6">
+      <c r="Q26" s="6">
         <f>'2004'!E26</f>
         <v>287272</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="6">
         <f>'2018'!E27</f>
         <v>1028981</v>
       </c>
-      <c r="C27" s="6">
+      <c r="D27" s="6">
         <f>'2017'!E27</f>
         <v>968295</v>
       </c>
-      <c r="D27" s="6">
+      <c r="E27" s="6">
         <f>'2016'!E27</f>
         <v>990082</v>
       </c>
-      <c r="E27" s="6">
+      <c r="F27" s="6">
         <f>'2015'!E27</f>
         <v>965823</v>
       </c>
-      <c r="F27" s="6">
+      <c r="G27" s="6">
         <f>'2014'!E27</f>
         <v>964200</v>
       </c>
-      <c r="G27" s="6">
+      <c r="H27" s="6">
         <f>'2013'!E27</f>
         <v>1005130</v>
       </c>
-      <c r="H27" s="6">
+      <c r="I27" s="6">
         <f>'2012'!E27</f>
         <v>1073594</v>
       </c>
-      <c r="I27" s="6">
+      <c r="J27" s="6">
         <f>'2011'!E27</f>
         <v>1065258</v>
       </c>
-      <c r="J27" s="6">
+      <c r="K27" s="6">
         <f>'2010'!E27</f>
         <v>1039982</v>
       </c>
-      <c r="K27" s="6">
+      <c r="L27" s="6">
         <f>'2009'!E27</f>
         <v>1044772</v>
       </c>
-      <c r="L27" s="6">
+      <c r="M27" s="6">
         <f>'2008'!E27</f>
         <v>1044772</v>
       </c>
-      <c r="M27" s="6">
+      <c r="N27" s="6">
         <f>'2007'!E27</f>
         <v>1000846</v>
       </c>
-      <c r="N27" s="6">
+      <c r="O27" s="6">
         <f>'2006'!E27</f>
         <v>1007542</v>
       </c>
-      <c r="O27" s="6">
+      <c r="P27" s="6">
         <f>'2005'!E27</f>
         <v>979429</v>
       </c>
-      <c r="P27" s="6">
+      <c r="Q27" s="6">
         <f>'2004'!E27</f>
         <v>935854</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="6">
         <f>'2018'!E28</f>
         <v>344762</v>
       </c>
-      <c r="C28" s="6">
+      <c r="D28" s="6">
         <f>'2017'!E28</f>
         <v>347124</v>
       </c>
-      <c r="D28" s="6">
+      <c r="E28" s="6">
         <f>'2016'!E28</f>
         <v>363336</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="6">
         <f>'2015'!E28</f>
         <v>347452</v>
       </c>
-      <c r="F28" s="6">
+      <c r="G28" s="6">
         <f>'2014'!E28</f>
         <v>352226</v>
       </c>
-      <c r="G28" s="6">
+      <c r="H28" s="6">
         <f>'2013'!E28</f>
         <v>358606</v>
       </c>
-      <c r="H28" s="6">
+      <c r="I28" s="6">
         <f>'2012'!E28</f>
         <v>352366</v>
       </c>
-      <c r="I28" s="6">
+      <c r="J28" s="6">
         <f>'2011'!E28</f>
         <v>372369</v>
       </c>
-      <c r="J28" s="6">
+      <c r="K28" s="6">
         <f>'2010'!E28</f>
         <v>373055</v>
       </c>
-      <c r="K28" s="6">
+      <c r="L28" s="6">
         <f>'2009'!E28</f>
         <v>547584</v>
       </c>
-      <c r="L28" s="6">
+      <c r="M28" s="6">
         <f>'2008'!E28</f>
         <v>522774</v>
       </c>
-      <c r="M28" s="6">
+      <c r="N28" s="6">
         <f>'2007'!E28</f>
         <v>488982</v>
       </c>
-      <c r="N28" s="6">
+      <c r="O28" s="6">
         <f>'2006'!E28</f>
         <v>497567</v>
       </c>
-      <c r="O28" s="6">
+      <c r="P28" s="6">
         <f>'2005'!E28</f>
         <v>493945</v>
       </c>
-      <c r="P28" s="6">
+      <c r="Q28" s="6">
         <f>'2004'!E28</f>
         <v>495908</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="6">
         <f>'2018'!E29</f>
         <v>520355</v>
       </c>
-      <c r="C29" s="6">
+      <c r="D29" s="6">
         <f>'2017'!E29</f>
         <v>517440</v>
       </c>
-      <c r="D29" s="6">
+      <c r="E29" s="6">
         <f>'2016'!E29</f>
         <v>543500</v>
       </c>
-      <c r="E29" s="6">
+      <c r="F29" s="6">
         <f>'2015'!E29</f>
         <v>549909</v>
       </c>
-      <c r="F29" s="6">
+      <c r="G29" s="6">
         <f>'2014'!E29</f>
         <v>587388</v>
       </c>
-      <c r="G29" s="6">
+      <c r="H29" s="6">
         <f>'2013'!E29</f>
         <v>625338</v>
       </c>
-      <c r="H29" s="6">
+      <c r="I29" s="6">
         <f>'2012'!E29</f>
         <v>646709</v>
       </c>
-      <c r="I29" s="6">
+      <c r="J29" s="6">
         <f>'2011'!E29</f>
         <v>656465</v>
       </c>
-      <c r="J29" s="6">
+      <c r="K29" s="6">
         <f>'2010'!E29</f>
         <v>677523</v>
       </c>
-      <c r="K29" s="6">
+      <c r="L29" s="6">
         <f>'2009'!E29</f>
         <v>649949</v>
       </c>
-      <c r="L29" s="6">
+      <c r="M29" s="6">
         <f>'2008'!E29</f>
         <v>636963</v>
       </c>
-      <c r="M29" s="6">
+      <c r="N29" s="6">
         <f>'2007'!E29</f>
         <v>620286</v>
       </c>
-      <c r="N29" s="6">
+      <c r="O29" s="6">
         <f>'2006'!E29</f>
         <v>592632</v>
       </c>
-      <c r="O29" s="6">
+      <c r="P29" s="6">
         <f>'2005'!E29</f>
         <v>603672</v>
       </c>
-      <c r="P29" s="6">
+      <c r="Q29" s="6">
         <f>'2004'!E29</f>
         <v>575486</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="6">
         <f>'2018'!E30</f>
         <v>429255</v>
       </c>
-      <c r="C30" s="6">
+      <c r="D30" s="6">
         <f>'2017'!E30</f>
         <v>417591</v>
       </c>
-      <c r="D30" s="6">
+      <c r="E30" s="6">
         <f>'2016'!E30</f>
         <v>417689</v>
       </c>
-      <c r="E30" s="6">
+      <c r="F30" s="6">
         <f>'2015'!E30</f>
         <v>419950</v>
       </c>
-      <c r="F30" s="6">
+      <c r="G30" s="6">
         <f>'2014'!E30</f>
         <v>447509</v>
       </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6">
         <f>'2013'!E30</f>
         <v>420893</v>
       </c>
-      <c r="H30" s="6">
+      <c r="I30" s="6">
         <f>'2012'!E30</f>
         <v>451121</v>
       </c>
-      <c r="I30" s="6">
+      <c r="J30" s="6">
         <f>'2011'!E30</f>
         <v>448366</v>
       </c>
-      <c r="J30" s="6">
+      <c r="K30" s="6">
         <f>'2010'!E30</f>
         <v>459212</v>
       </c>
-      <c r="K30" s="6">
+      <c r="L30" s="6">
         <f>'2009'!E30</f>
         <v>449663</v>
       </c>
-      <c r="L30" s="6">
+      <c r="M30" s="6">
         <f>'2008'!E30</f>
         <v>449663</v>
       </c>
-      <c r="M30" s="6">
+      <c r="N30" s="6">
         <f>'2007'!E30</f>
         <v>406359</v>
       </c>
-      <c r="N30" s="6">
+      <c r="O30" s="6">
         <f>'2006'!E30</f>
         <v>405644</v>
       </c>
-      <c r="O30" s="6">
+      <c r="P30" s="6">
         <f>'2005'!E30</f>
         <v>397069</v>
       </c>
-      <c r="P30" s="6">
+      <c r="Q30" s="6">
         <f>'2004'!E30</f>
         <v>394105</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="6">
         <f>'2018'!E31</f>
         <v>218342</v>
       </c>
-      <c r="C31" s="6">
+      <c r="D31" s="6">
         <f>'2017'!E31</f>
         <v>219698</v>
       </c>
-      <c r="D31" s="6">
+      <c r="E31" s="6">
         <f>'2016'!E31</f>
         <v>219741</v>
       </c>
-      <c r="E31" s="6">
+      <c r="F31" s="6">
         <f>'2015'!E31</f>
         <v>212046</v>
       </c>
-      <c r="F31" s="6">
+      <c r="G31" s="6">
         <f>'2014'!E31</f>
         <v>203793</v>
       </c>
-      <c r="G31" s="6">
+      <c r="H31" s="6">
         <f>'2013'!E31</f>
         <v>209194</v>
       </c>
-      <c r="H31" s="6">
+      <c r="I31" s="6">
         <f>'2012'!E31</f>
         <v>218346</v>
       </c>
-      <c r="I31" s="6">
+      <c r="J31" s="6">
         <f>'2011'!E31</f>
         <v>217306</v>
       </c>
-      <c r="J31" s="6">
+      <c r="K31" s="6">
         <f>'2010'!E31</f>
         <v>222364</v>
       </c>
-      <c r="K31" s="6">
+      <c r="L31" s="6">
         <f>'2009'!E31</f>
         <v>222164</v>
       </c>
-      <c r="L31" s="6">
+      <c r="M31" s="6">
         <f>'2008'!E31</f>
         <v>222164</v>
       </c>
-      <c r="M31" s="6">
+      <c r="N31" s="6">
         <f>'2007'!E31</f>
         <v>220561</v>
       </c>
-      <c r="N31" s="6">
+      <c r="O31" s="6">
         <f>'2006'!E31</f>
         <v>223430</v>
       </c>
-      <c r="O31" s="6">
+      <c r="P31" s="6">
         <f>'2005'!E31</f>
         <v>226252</v>
       </c>
-      <c r="P31" s="6">
+      <c r="Q31" s="6">
         <f>'2004'!E31</f>
         <v>233432</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="6">
         <f>'2018'!E32</f>
         <v>422237</v>
       </c>
-      <c r="C32" s="6">
+      <c r="D32" s="6">
         <f>'2017'!E32</f>
         <v>414662</v>
       </c>
-      <c r="D32" s="6">
+      <c r="E32" s="6">
         <f>'2016'!E32</f>
         <v>366625</v>
       </c>
-      <c r="E32" s="6">
+      <c r="F32" s="6">
         <f>'2015'!E32</f>
         <v>353652</v>
       </c>
-      <c r="F32" s="6">
+      <c r="G32" s="6">
         <f>'2014'!E32</f>
         <v>345727</v>
       </c>
-      <c r="G32" s="6">
+      <c r="H32" s="6">
         <f>'2013'!E32</f>
         <v>368420</v>
       </c>
-      <c r="H32" s="6">
+      <c r="I32" s="6">
         <f>'2012'!E32</f>
         <v>444884</v>
       </c>
-      <c r="I32" s="6">
+      <c r="J32" s="6">
         <f>'2011'!E32</f>
         <v>443704</v>
       </c>
-      <c r="J32" s="6">
+      <c r="K32" s="6">
         <f>'2010'!E32</f>
         <v>455066</v>
       </c>
-      <c r="K32" s="6">
+      <c r="L32" s="6">
         <f>'2009'!E32</f>
         <v>431715</v>
       </c>
-      <c r="L32" s="6">
+      <c r="M32" s="6">
         <f>'2008'!E32</f>
         <v>431715</v>
       </c>
-      <c r="M32" s="6">
+      <c r="N32" s="6">
         <f>'2007'!E32</f>
         <v>415802</v>
       </c>
-      <c r="N32" s="6">
+      <c r="O32" s="6">
         <f>'2006'!E32</f>
         <v>418089</v>
       </c>
-      <c r="O32" s="6">
+      <c r="P32" s="6">
         <f>'2005'!E32</f>
         <v>403563</v>
       </c>
-      <c r="P32" s="6">
+      <c r="Q32" s="6">
         <f>'2004'!E32</f>
         <v>429205</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="6">
         <f>'2018'!E33</f>
         <v>441906</v>
       </c>
-      <c r="C33" s="6">
+      <c r="D33" s="6">
         <f>'2017'!E33</f>
         <v>323624</v>
       </c>
-      <c r="D33" s="6">
+      <c r="E33" s="6">
         <f>'2016'!E33</f>
         <v>353760</v>
       </c>
-      <c r="E33" s="6">
+      <c r="F33" s="6">
         <f>'2015'!E33</f>
         <v>302504</v>
       </c>
-      <c r="F33" s="6">
+      <c r="G33" s="6">
         <f>'2014'!E33</f>
         <v>250163</v>
       </c>
-      <c r="G33" s="6">
+      <c r="H33" s="6">
         <f>'2013'!E33</f>
         <v>2648830</v>
       </c>
-      <c r="H33" s="6">
+      <c r="I33" s="6">
         <f>'2012'!E33</f>
         <v>269843</v>
       </c>
-      <c r="I33" s="6">
+      <c r="J33" s="6">
         <f>'2011'!E33</f>
         <v>267157</v>
       </c>
-      <c r="J33" s="6">
+      <c r="K33" s="6">
         <f>'2010'!E33</f>
         <v>296653</v>
       </c>
-      <c r="K33" s="6">
+      <c r="L33" s="6">
         <f>'2009'!E33</f>
         <v>231646</v>
       </c>
-      <c r="L33" s="6">
+      <c r="M33" s="6">
         <f>'2008'!E33</f>
         <v>212187</v>
       </c>
-      <c r="M33" s="6">
+      <c r="N33" s="6">
         <f>'2007'!E33</f>
         <v>324609</v>
       </c>
-      <c r="N33" s="6">
+      <c r="O33" s="6">
         <f>'2006'!E33</f>
         <v>338290</v>
       </c>
-      <c r="O33" s="6">
+      <c r="P33" s="6">
         <f>'2005'!E33</f>
         <v>338568</v>
       </c>
-      <c r="P33" s="6">
+      <c r="Q33" s="6">
         <f>'2004'!E33</f>
         <v>460545</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="6">
         <f>'2018'!E34</f>
         <v>150111</v>
       </c>
-      <c r="C34" s="6">
+      <c r="D34" s="6">
         <f>'2017'!E34</f>
         <v>149112</v>
       </c>
-      <c r="D34" s="6">
+      <c r="E34" s="6">
         <f>'2016'!E34</f>
         <v>146631</v>
       </c>
-      <c r="E34" s="6">
+      <c r="F34" s="6">
         <f>'2015'!E34</f>
         <v>143889</v>
       </c>
-      <c r="F34" s="6">
+      <c r="G34" s="6">
         <f>'2014'!E34</f>
         <v>129589</v>
       </c>
-      <c r="G34" s="6">
+      <c r="H34" s="6">
         <f>'2013'!E34</f>
         <v>128661</v>
       </c>
-      <c r="H34" s="6">
+      <c r="I34" s="6">
         <f>'2012'!E34</f>
         <v>130471</v>
       </c>
-      <c r="I34" s="6">
+      <c r="J34" s="6">
         <f>'2011'!E34</f>
         <v>126198</v>
       </c>
-      <c r="J34" s="6">
+      <c r="K34" s="6">
         <f>'2010'!E34</f>
         <v>127914</v>
       </c>
-      <c r="K34" s="6">
+      <c r="L34" s="6">
         <f>'2009'!E34</f>
         <v>135139</v>
       </c>
-      <c r="L34" s="6">
+      <c r="M34" s="6">
         <f>'2008'!E34</f>
         <v>135139</v>
       </c>
-      <c r="M34" s="6">
+      <c r="N34" s="6">
         <f>'2007'!E34</f>
         <v>120602</v>
       </c>
-      <c r="N34" s="6">
+      <c r="O34" s="6">
         <f>'2006'!E34</f>
         <v>110443</v>
       </c>
-      <c r="O34" s="6">
+      <c r="P34" s="6">
         <f>'2005'!E34</f>
         <v>89994</v>
       </c>
-      <c r="P34" s="6">
+      <c r="Q34" s="6">
         <f>'2004'!E34</f>
         <v>95545</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="6">
         <f>'2018'!E35</f>
         <v>1166349</v>
       </c>
-      <c r="C35" s="6">
+      <c r="D35" s="6">
         <f>'2017'!E35</f>
         <v>1145131</v>
       </c>
-      <c r="D35" s="6">
+      <c r="E35" s="6">
         <f>'2016'!E35</f>
         <v>1071806</v>
       </c>
-      <c r="E35" s="6">
+      <c r="F35" s="6">
         <f>'2015'!E35</f>
         <v>1114904</v>
       </c>
-      <c r="F35" s="6">
+      <c r="G35" s="6">
         <f>'2014'!E35</f>
         <v>1077625</v>
       </c>
-      <c r="G35" s="6">
+      <c r="H35" s="6">
         <f>'2013'!E35</f>
         <v>1065247</v>
       </c>
-      <c r="H35" s="6">
+      <c r="I35" s="6">
         <f>'2012'!E35</f>
         <v>1091187</v>
       </c>
-      <c r="I35" s="6">
+      <c r="J35" s="6">
         <f>'2011'!E35</f>
         <v>732654</v>
       </c>
-      <c r="J35" s="6">
+      <c r="K35" s="6">
         <f>'2010'!E35</f>
         <v>899036</v>
       </c>
-      <c r="K35" s="6">
+      <c r="L35" s="6">
         <f>'2009'!E35</f>
         <v>901313</v>
       </c>
-      <c r="L35" s="6">
+      <c r="M35" s="6">
         <f>'2008'!E35</f>
         <v>922855</v>
       </c>
-      <c r="M35" s="6">
+      <c r="N35" s="6">
         <f>'2007'!E35</f>
         <v>936592</v>
       </c>
-      <c r="N35" s="6">
+      <c r="O35" s="6">
         <f>'2006'!E35</f>
         <v>1375917</v>
       </c>
-      <c r="O35" s="6">
+      <c r="P35" s="6">
         <f>'2005'!E35</f>
         <v>1454229</v>
       </c>
-      <c r="P35" s="6">
+      <c r="Q35" s="6">
         <f>'2004'!E35</f>
         <v>754189</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="6">
         <f>'2018'!E36</f>
         <v>995164</v>
       </c>
-      <c r="C36" s="6">
+      <c r="D36" s="6">
         <f>'2017'!E36</f>
         <v>1037841</v>
       </c>
-      <c r="D36" s="6">
+      <c r="E36" s="6">
         <f>'2016'!E36</f>
         <v>1098675</v>
       </c>
-      <c r="E36" s="6">
+      <c r="F36" s="6">
         <f>'2015'!E36</f>
         <v>1151515</v>
       </c>
-      <c r="F36" s="6">
+      <c r="G36" s="6">
         <f>'2014'!E36</f>
         <v>1174147</v>
       </c>
-      <c r="G36" s="6">
+      <c r="H36" s="6">
         <f>'2013'!E36</f>
         <v>416101</v>
       </c>
-      <c r="H36" s="6">
+      <c r="I36" s="6">
         <f>'2012'!E36</f>
         <v>423715</v>
       </c>
-      <c r="I36" s="6">
+      <c r="J36" s="6">
         <f>'2011'!E36</f>
         <v>417491</v>
       </c>
-      <c r="J36" s="6">
+      <c r="K36" s="6">
         <f>'2010'!E36</f>
         <v>1084277</v>
       </c>
-      <c r="K36" s="6">
+      <c r="L36" s="6">
         <f>'2009'!E36</f>
         <v>1164034</v>
       </c>
-      <c r="L36" s="6">
+      <c r="M36" s="6">
         <f>'2008'!E36</f>
         <v>1121921</v>
       </c>
-      <c r="M36" s="6">
+      <c r="N36" s="6">
         <f>'2007'!E36</f>
         <v>1104617</v>
       </c>
-      <c r="N36" s="6">
+      <c r="O36" s="6">
         <f>'2006'!E36</f>
         <v>1179515</v>
       </c>
-      <c r="O36" s="6">
+      <c r="P36" s="6">
         <f>'2005'!E36</f>
         <v>1128842</v>
       </c>
-      <c r="P36" s="6">
+      <c r="Q36" s="6">
         <f>'2004'!E36</f>
         <v>1086640</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="6">
         <f>'2018'!E37</f>
         <v>400238</v>
       </c>
-      <c r="C37" s="6">
+      <c r="D37" s="6">
         <f>'2017'!E37</f>
         <v>321534</v>
       </c>
-      <c r="D37" s="6">
+      <c r="E37" s="6">
         <f>'2016'!E37</f>
         <v>312573</v>
       </c>
-      <c r="E37" s="6">
+      <c r="F37" s="6">
         <f>'2015'!E37</f>
         <v>311776</v>
       </c>
-      <c r="F37" s="6">
+      <c r="G37" s="6">
         <f>'2014'!E37</f>
         <v>290577</v>
       </c>
-      <c r="G37" s="6">
+      <c r="H37" s="6">
         <f>'2013'!E37</f>
         <v>289240</v>
       </c>
-      <c r="H37" s="6">
+      <c r="I37" s="6">
         <f>'2012'!E37</f>
         <v>301441</v>
       </c>
-      <c r="I37" s="6">
+      <c r="J37" s="6">
         <f>'2011'!E37</f>
         <v>305787</v>
       </c>
-      <c r="J37" s="6">
+      <c r="K37" s="6">
         <f>'2010'!E37</f>
         <v>292514</v>
       </c>
-      <c r="K37" s="6">
+      <c r="L37" s="6">
         <f>'2009'!E37</f>
         <v>281390</v>
       </c>
-      <c r="L37" s="6">
+      <c r="M37" s="6">
         <f>'2008'!E37</f>
         <v>277600</v>
       </c>
-      <c r="M37" s="6">
+      <c r="N37" s="6">
         <f>'2007'!E37</f>
         <v>288373</v>
       </c>
-      <c r="N37" s="6">
+      <c r="O37" s="6">
         <f>'2006'!E37</f>
         <v>307589</v>
       </c>
-      <c r="O37" s="6">
+      <c r="P37" s="6">
         <f>'2005'!E37</f>
         <v>328993</v>
       </c>
-      <c r="P37" s="6">
+      <c r="Q37" s="6">
         <f>'2004'!E37</f>
         <v>348924</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="6">
         <f>'2018'!E38</f>
         <v>1222670</v>
       </c>
-      <c r="C38" s="6">
+      <c r="D38" s="6">
         <f>'2017'!E38</f>
         <v>1238680</v>
       </c>
-      <c r="D38" s="6">
+      <c r="E38" s="6">
         <f>'2016'!E38</f>
         <v>1253956</v>
       </c>
-      <c r="E38" s="6">
+      <c r="F38" s="6">
         <f>'2015'!E38</f>
         <v>1291430</v>
       </c>
-      <c r="F38" s="6">
+      <c r="G38" s="6">
         <f>'2014'!E38</f>
         <v>1240155</v>
       </c>
-      <c r="G38" s="6">
+      <c r="H38" s="6">
         <f>'2013'!E38</f>
         <v>1255439</v>
       </c>
-      <c r="H38" s="6">
+      <c r="I38" s="6">
         <f>'2012'!E38</f>
         <v>1289930</v>
       </c>
-      <c r="I38" s="6">
+      <c r="J38" s="6">
         <f>'2011'!E38</f>
         <v>1318164</v>
       </c>
-      <c r="J38" s="6">
+      <c r="K38" s="6">
         <f>'2010'!E38</f>
         <v>279893</v>
       </c>
-      <c r="K38" s="6">
+      <c r="L38" s="6">
         <f>'2009'!E38</f>
         <v>1322269</v>
       </c>
-      <c r="L38" s="6">
+      <c r="M38" s="6">
         <f>'2008'!E38</f>
         <v>1322269</v>
       </c>
-      <c r="M38" s="6">
+      <c r="N38" s="6">
         <f>'2007'!E38</f>
         <v>1329338</v>
       </c>
-      <c r="N38" s="6">
+      <c r="O38" s="6">
         <f>'2006'!E38</f>
         <v>1331894</v>
       </c>
-      <c r="O38" s="6">
+      <c r="P38" s="6">
         <f>'2005'!E38</f>
         <v>1381167</v>
       </c>
-      <c r="P38" s="6">
+      <c r="Q38" s="6">
         <f>'2004'!E38</f>
         <v>1409238</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="6">
         <f>'2018'!E39</f>
         <v>2569930</v>
       </c>
-      <c r="C39" s="6">
+      <c r="D39" s="6">
         <f>'2017'!E39</f>
         <v>2378225</v>
       </c>
-      <c r="D39" s="6">
+      <c r="E39" s="6">
         <f>'2016'!E39</f>
         <v>2664373</v>
       </c>
-      <c r="E39" s="6">
+      <c r="F39" s="6">
         <f>'2015'!E39</f>
         <v>2642943</v>
       </c>
-      <c r="F39" s="6">
+      <c r="G39" s="6">
         <f>'2014'!E39</f>
         <v>2668942</v>
       </c>
-      <c r="G39" s="6">
+      <c r="H39" s="6">
         <f>'2013'!E39</f>
         <v>2427886</v>
       </c>
-      <c r="H39" s="6">
+      <c r="I39" s="6">
         <f>'2012'!E39</f>
         <v>2668549</v>
       </c>
-      <c r="I39" s="6">
+      <c r="J39" s="6">
         <f>'2011'!E39</f>
         <v>2526585</v>
       </c>
-      <c r="J39" s="6">
+      <c r="K39" s="6">
         <f>'2010'!E39</f>
         <v>2536376</v>
       </c>
-      <c r="K39" s="6">
+      <c r="L39" s="6">
         <f>'2009'!E39</f>
         <v>2562760</v>
       </c>
-      <c r="L39" s="6">
+      <c r="M39" s="6">
         <f>'2008'!E39</f>
         <v>2622327</v>
       </c>
-      <c r="M39" s="6">
+      <c r="N39" s="6">
         <f>'2007'!E39</f>
         <v>2828198</v>
       </c>
-      <c r="N39" s="6">
+      <c r="O39" s="6">
         <f>'2006'!E39</f>
         <v>2718624</v>
       </c>
-      <c r="O39" s="6">
+      <c r="P39" s="6">
         <f>'2005'!E39</f>
         <v>2791423</v>
       </c>
-      <c r="P39" s="6">
+      <c r="Q39" s="6">
         <f>'2004'!E39</f>
         <v>2520673</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="6">
         <f>'2018'!E40</f>
         <v>30903</v>
       </c>
-      <c r="C40" s="6">
+      <c r="D40" s="6">
         <f>'2017'!E40</f>
         <v>33200</v>
       </c>
-      <c r="D40" s="6">
+      <c r="E40" s="6">
         <f>'2016'!E40</f>
         <v>8978</v>
       </c>
-      <c r="E40" s="6">
+      <c r="F40" s="6">
         <f>'2015'!E40</f>
         <v>33872</v>
       </c>
-      <c r="F40" s="6">
+      <c r="G40" s="6">
         <f>'2014'!E40</f>
         <v>9025</v>
       </c>
-      <c r="G40" s="6">
+      <c r="H40" s="6">
         <f>'2013'!E40</f>
         <v>8605</v>
       </c>
-      <c r="H40" s="6">
+      <c r="I40" s="6">
         <f>'2012'!E40</f>
         <v>8798</v>
       </c>
-      <c r="I40" s="6">
+      <c r="J40" s="6">
         <f>'2011'!E40</f>
         <v>0</v>
       </c>
-      <c r="J40" s="6">
+      <c r="K40" s="6">
         <f>'2010'!E40</f>
         <v>34628</v>
       </c>
-      <c r="K40" s="6">
+      <c r="L40" s="6">
         <f>'2009'!E40</f>
         <v>34628</v>
       </c>
-      <c r="L40" s="6">
+      <c r="M40" s="6">
         <f>'2008'!E40</f>
         <v>34628</v>
       </c>
-      <c r="M40" s="6">
+      <c r="N40" s="6">
         <f>'2007'!E40</f>
         <v>31639</v>
       </c>
-      <c r="N40" s="6">
+      <c r="O40" s="6">
         <f>'2006'!E40</f>
         <v>33988</v>
       </c>
-      <c r="O40" s="6">
+      <c r="P40" s="6">
         <f>'2005'!E40</f>
         <v>33876</v>
       </c>
-      <c r="P40" s="6">
+      <c r="Q40" s="6">
         <f>'2004'!E40</f>
         <v>32823</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="6">
         <f>'2018'!E41</f>
         <v>814285</v>
       </c>
-      <c r="C41" s="6">
+      <c r="D41" s="6">
         <f>'2017'!E41</f>
         <v>802737</v>
       </c>
-      <c r="D41" s="6">
+      <c r="E41" s="6">
         <f>'2016'!E41</f>
         <v>434043</v>
       </c>
-      <c r="E41" s="6">
+      <c r="F41" s="6">
         <f>'2015'!E41</f>
         <v>423437</v>
       </c>
-      <c r="F41" s="6">
+      <c r="G41" s="6">
         <f>'2014'!E41</f>
         <v>428526</v>
       </c>
-      <c r="G41" s="6">
+      <c r="H41" s="6">
         <f>'2013'!E41</f>
         <v>399386</v>
       </c>
-      <c r="H41" s="6">
+      <c r="I41" s="6">
         <f>'2012'!E41</f>
         <v>638166</v>
       </c>
-      <c r="I41" s="6">
+      <c r="J41" s="6">
         <f>'2011'!E41</f>
         <v>567796</v>
       </c>
-      <c r="J41" s="6">
+      <c r="K41" s="6">
         <f>'2010'!E41</f>
         <v>558532</v>
       </c>
-      <c r="K41" s="6">
+      <c r="L41" s="6">
         <f>'2009'!E41</f>
         <v>535360</v>
       </c>
-      <c r="L41" s="6">
+      <c r="M41" s="6">
         <f>'2008'!E41</f>
         <v>517773</v>
       </c>
-      <c r="M41" s="6">
+      <c r="N41" s="6">
         <f>'2007'!E41</f>
         <v>479965</v>
       </c>
-      <c r="N41" s="6">
+      <c r="O41" s="6">
         <f>'2006'!E41</f>
         <v>457410</v>
       </c>
-      <c r="O41" s="6">
+      <c r="P41" s="6">
         <f>'2005'!E41</f>
         <v>259343</v>
       </c>
-      <c r="P41" s="6">
+      <c r="Q41" s="6">
         <f>'2004'!E41</f>
         <v>265906</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="6">
         <f>'2018'!E42</f>
         <v>373976</v>
       </c>
-      <c r="C42" s="6">
+      <c r="D42" s="6">
         <f>'2017'!E42</f>
         <v>362804</v>
       </c>
-      <c r="D42" s="6">
+      <c r="E42" s="6">
         <f>'2016'!E42</f>
         <v>400704</v>
       </c>
-      <c r="E42" s="6">
+      <c r="F42" s="6">
         <f>'2015'!E42</f>
         <v>402372</v>
       </c>
-      <c r="F42" s="6">
+      <c r="G42" s="6">
         <f>'2014'!E42</f>
         <v>414924</v>
       </c>
-      <c r="G42" s="6">
+      <c r="H42" s="6">
         <f>'2013'!E42</f>
         <v>430552</v>
       </c>
-      <c r="H42" s="6">
+      <c r="I42" s="6">
         <f>'2012'!E42</f>
         <v>432327</v>
       </c>
-      <c r="I42" s="6">
+      <c r="J42" s="6">
         <f>'2011'!E42</f>
         <v>441264</v>
       </c>
-      <c r="J42" s="6">
+      <c r="K42" s="6">
         <f>'2010'!E42</f>
         <v>439537</v>
       </c>
-      <c r="K42" s="6">
+      <c r="L42" s="6">
         <f>'2009'!E42</f>
         <v>418141</v>
       </c>
-      <c r="L42" s="6">
+      <c r="M42" s="6">
         <f>'2008'!E42</f>
         <v>397779</v>
       </c>
-      <c r="M42" s="6">
+      <c r="N42" s="6">
         <f>'2007'!E42</f>
         <v>387164</v>
       </c>
-      <c r="N42" s="6">
+      <c r="O42" s="6">
         <f>'2006'!E42</f>
         <v>370227</v>
       </c>
-      <c r="O42" s="6">
+      <c r="P42" s="6">
         <f>'2005'!E42</f>
         <v>348703</v>
       </c>
-      <c r="P42" s="6">
+      <c r="Q42" s="6">
         <f>'2004'!E42</f>
         <v>347928</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="6">
         <f>'2018'!E43</f>
         <v>737173</v>
       </c>
-      <c r="C43" s="6">
+      <c r="D43" s="6">
         <f>'2017'!E43</f>
         <v>785026</v>
       </c>
-      <c r="D43" s="6">
+      <c r="E43" s="6">
         <f>'2016'!E43</f>
         <v>785761</v>
       </c>
-      <c r="E43" s="6">
+      <c r="F43" s="6">
         <f>'2015'!E43</f>
         <v>757359</v>
       </c>
-      <c r="F43" s="6">
+      <c r="G43" s="6">
         <f>'2014'!E43</f>
         <v>720420</v>
       </c>
-      <c r="G43" s="6">
+      <c r="H43" s="6">
         <f>'2013'!E43</f>
         <v>697018</v>
       </c>
-      <c r="H43" s="6">
+      <c r="I43" s="6">
         <f>'2012'!E43</f>
         <v>731401</v>
       </c>
-      <c r="I43" s="6">
+      <c r="J43" s="6">
         <f>'2011'!E43</f>
         <v>756236</v>
       </c>
-      <c r="J43" s="6">
+      <c r="K43" s="6">
         <f>'2010'!E43</f>
         <v>783115</v>
       </c>
-      <c r="K43" s="6">
+      <c r="L43" s="6">
         <f>'2009'!E43</f>
         <v>832944</v>
       </c>
-      <c r="L43" s="6">
+      <c r="M43" s="6">
         <f>'2008'!E43</f>
         <v>725238</v>
       </c>
-      <c r="M43" s="6">
+      <c r="N43" s="6">
         <f>'2007'!E43</f>
         <v>1093825</v>
       </c>
-      <c r="N43" s="6">
+      <c r="O43" s="6">
         <f>'2006'!E43</f>
         <v>1302277</v>
       </c>
-      <c r="O43" s="6">
+      <c r="P43" s="6">
         <f>'2005'!E43</f>
         <v>983990</v>
       </c>
-      <c r="P43" s="6">
+      <c r="Q43" s="6">
         <f>'2004'!E43</f>
         <v>1131450</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="6">
         <f>'2018'!E44</f>
         <v>1655343</v>
       </c>
-      <c r="C44" s="6">
+      <c r="D44" s="6">
         <f>'2017'!E44</f>
         <v>1641604</v>
       </c>
-      <c r="D44" s="6">
+      <c r="E44" s="6">
         <f>'2016'!E44</f>
         <v>1611342</v>
       </c>
-      <c r="E44" s="6">
+      <c r="F44" s="6">
         <f>'2015'!E44</f>
         <v>1537431</v>
       </c>
-      <c r="F44" s="6">
+      <c r="G44" s="6">
         <f>'2014'!E44</f>
         <v>1450212</v>
       </c>
-      <c r="G44" s="6">
+      <c r="H44" s="6">
         <f>'2013'!E44</f>
         <v>1473996</v>
       </c>
-      <c r="H44" s="6">
+      <c r="I44" s="6">
         <f>'2012'!E44</f>
         <v>1442357</v>
       </c>
-      <c r="I44" s="6">
+      <c r="J44" s="6">
         <f>'2011'!E44</f>
         <v>1473969</v>
       </c>
-      <c r="J44" s="6">
+      <c r="K44" s="6">
         <f>'2010'!E44</f>
         <v>1596084</v>
       </c>
-      <c r="K44" s="6">
+      <c r="L44" s="6">
         <f>'2009'!E44</f>
         <v>1539111</v>
       </c>
-      <c r="L44" s="6">
+      <c r="M44" s="6">
         <f>'2008'!E44</f>
         <v>1512583</v>
       </c>
-      <c r="M44" s="6">
+      <c r="N44" s="6">
         <f>'2007'!E44</f>
         <v>1444364</v>
       </c>
-      <c r="N44" s="6">
+      <c r="O44" s="6">
         <f>'2006'!E44</f>
         <v>1294660</v>
       </c>
-      <c r="O44" s="6">
+      <c r="P44" s="6">
         <f>'2005'!E44</f>
         <v>1290716</v>
       </c>
-      <c r="P44" s="6">
+      <c r="Q44" s="6">
         <f>'2004'!E44</f>
         <v>1266103</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="6">
         <f>'2018'!E45</f>
         <v>420841</v>
       </c>
-      <c r="C45" s="6">
+      <c r="D45" s="6">
         <f>'2017'!E45</f>
         <v>410468</v>
       </c>
-      <c r="D45" s="6">
+      <c r="E45" s="6">
         <f>'2016'!E45</f>
         <v>386403</v>
       </c>
-      <c r="E45" s="6">
+      <c r="F45" s="6">
         <f>'2015'!E45</f>
         <v>367527</v>
       </c>
-      <c r="F45" s="6">
+      <c r="G45" s="6">
         <f>'2014'!E45</f>
         <v>370250</v>
       </c>
-      <c r="G45" s="6">
+      <c r="H45" s="6">
         <f>'2013'!E45</f>
         <v>385032</v>
       </c>
-      <c r="H45" s="6">
+      <c r="I45" s="6">
         <f>'2012'!E45</f>
         <v>386191</v>
       </c>
-      <c r="I45" s="6">
+      <c r="J45" s="6">
         <f>'2011'!E45</f>
         <v>374210</v>
       </c>
-      <c r="J45" s="6">
+      <c r="K45" s="6">
         <f>'2010'!E45</f>
         <v>292695</v>
       </c>
-      <c r="K45" s="6">
+      <c r="L45" s="6">
         <f>'2009'!E45</f>
         <v>267512</v>
       </c>
-      <c r="L45" s="6">
+      <c r="M45" s="6">
         <f>'2008'!E45</f>
         <v>267512</v>
       </c>
-      <c r="M45" s="6">
+      <c r="N45" s="6">
         <f>'2007'!E45</f>
         <v>231901</v>
       </c>
-      <c r="N45" s="6">
+      <c r="O45" s="6">
         <f>'2006'!E45</f>
         <v>242701</v>
       </c>
-      <c r="O45" s="6">
+      <c r="P45" s="6">
         <f>'2005'!E45</f>
         <v>238073</v>
       </c>
-      <c r="P45" s="6">
+      <c r="Q45" s="6">
         <f>'2004'!E45</f>
         <v>230153</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="6">
         <f>'2018'!E46</f>
         <v>860075</v>
       </c>
-      <c r="C46" s="6">
+      <c r="D46" s="6">
         <f>'2017'!E46</f>
         <v>839898</v>
       </c>
-      <c r="D46" s="6">
+      <c r="E46" s="6">
         <f>'2016'!E46</f>
         <v>843423</v>
       </c>
-      <c r="E46" s="6">
+      <c r="F46" s="6">
         <f>'2015'!E46</f>
         <v>830192</v>
       </c>
-      <c r="F46" s="6">
+      <c r="G46" s="6">
         <f>'2014'!E46</f>
         <v>818851</v>
       </c>
-      <c r="G46" s="6">
+      <c r="H46" s="6">
         <f>'2013'!E46</f>
         <v>816776</v>
       </c>
-      <c r="H46" s="6">
+      <c r="I46" s="6">
         <f>'2012'!E46</f>
         <v>789834</v>
       </c>
-      <c r="I46" s="6">
+      <c r="J46" s="6">
         <f>'2011'!E46</f>
         <v>810659</v>
       </c>
-      <c r="J46" s="6">
+      <c r="K46" s="6">
         <f>'2010'!E46</f>
         <v>802526</v>
       </c>
-      <c r="K46" s="6">
+      <c r="L46" s="6">
         <f>'2009'!E46</f>
         <v>795015</v>
       </c>
-      <c r="L46" s="6">
+      <c r="M46" s="6">
         <f>'2008'!E46</f>
         <v>794827</v>
       </c>
-      <c r="M46" s="6">
+      <c r="N46" s="6">
         <f>'2007'!E46</f>
         <v>791509</v>
       </c>
-      <c r="N46" s="6">
+      <c r="O46" s="6">
         <f>'2006'!E46</f>
         <v>817220</v>
       </c>
-      <c r="O46" s="6">
+      <c r="P46" s="6">
         <f>'2005'!E46</f>
         <v>813880</v>
       </c>
-      <c r="P46" s="6">
+      <c r="Q46" s="6">
         <f>'2004'!E46</f>
         <v>823123</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="6">
         <f>'2018'!E47</f>
         <v>169328</v>
       </c>
-      <c r="C47" s="6">
+      <c r="D47" s="6">
         <f>'2017'!E47</f>
         <v>177428</v>
       </c>
-      <c r="D47" s="6">
+      <c r="E47" s="6">
         <f>'2016'!E47</f>
         <v>178743</v>
       </c>
-      <c r="E47" s="6">
+      <c r="F47" s="6">
         <f>'2015'!E47</f>
         <v>183780</v>
       </c>
-      <c r="F47" s="6">
+      <c r="G47" s="6">
         <f>'2014'!E47</f>
         <v>172351</v>
       </c>
-      <c r="G47" s="6">
+      <c r="H47" s="6">
         <f>'2013'!E47</f>
         <v>189241</v>
       </c>
-      <c r="H47" s="6">
+      <c r="I47" s="6">
         <f>'2012'!E47</f>
         <v>191735</v>
       </c>
-      <c r="I47" s="6">
+      <c r="J47" s="6">
         <f>'2011'!E47</f>
         <v>188068</v>
       </c>
-      <c r="J47" s="6">
+      <c r="K47" s="6">
         <f>'2010'!E47</f>
         <v>172964</v>
       </c>
-      <c r="K47" s="6">
+      <c r="L47" s="6">
         <f>'2009'!E47</f>
         <v>172964</v>
       </c>
-      <c r="L47" s="6">
+      <c r="M47" s="6">
         <f>'2008'!E47</f>
         <v>165583</v>
       </c>
-      <c r="M47" s="6">
+      <c r="N47" s="6">
         <f>'2007'!E47</f>
         <v>154596</v>
       </c>
-      <c r="N47" s="6">
+      <c r="O47" s="6">
         <f>'2006'!E47</f>
         <v>170680</v>
       </c>
-      <c r="O47" s="6">
+      <c r="P47" s="6">
         <f>'2005'!E47</f>
         <v>186789</v>
       </c>
-      <c r="P47" s="6">
+      <c r="Q47" s="6">
         <f>'2004'!E47</f>
         <v>192308</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="6">
         <f>'2018'!E48</f>
         <v>691732</v>
       </c>
-      <c r="C48" s="6">
+      <c r="D48" s="6">
         <f>'2017'!E48</f>
         <v>685166</v>
       </c>
-      <c r="D48" s="6">
+      <c r="E48" s="6">
         <f>'2016'!E48</f>
         <v>674196</v>
       </c>
-      <c r="E48" s="6">
+      <c r="F48" s="6">
         <f>'2015'!E48</f>
         <v>676025</v>
       </c>
-      <c r="F48" s="6">
+      <c r="G48" s="6">
         <f>'2014'!E48</f>
         <v>666678</v>
       </c>
-      <c r="G48" s="6">
+      <c r="H48" s="6">
         <f>'2013'!E48</f>
         <v>738385</v>
       </c>
-      <c r="H48" s="6">
+      <c r="I48" s="6">
         <f>'2012'!E48</f>
         <v>770206</v>
       </c>
-      <c r="I48" s="6">
+      <c r="J48" s="6">
         <f>'2011'!E48</f>
         <v>775028</v>
       </c>
-      <c r="J48" s="6">
+      <c r="K48" s="6">
         <f>'2010'!E48</f>
         <v>763171</v>
       </c>
-      <c r="K48" s="6">
+      <c r="L48" s="6">
         <f>'2009'!E48</f>
         <v>782009</v>
       </c>
-      <c r="L48" s="6">
+      <c r="M48" s="6">
         <f>'2008'!E48</f>
         <v>837738</v>
       </c>
-      <c r="M48" s="6">
+      <c r="N48" s="6">
         <f>'2007'!E48</f>
         <v>929616</v>
       </c>
-      <c r="N48" s="6">
+      <c r="O48" s="6">
         <f>'2006'!E48</f>
         <v>902485</v>
       </c>
-      <c r="O48" s="6">
+      <c r="P48" s="6">
         <f>'2005'!E48</f>
         <v>883616</v>
       </c>
-      <c r="P48" s="6">
+      <c r="Q48" s="6">
         <f>'2004'!E48</f>
         <v>791512</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="6">
         <f>'2018'!E49</f>
         <v>2863676</v>
       </c>
-      <c r="C49" s="6">
+      <c r="D49" s="6">
         <f>'2017'!E49</f>
         <v>2836703</v>
       </c>
-      <c r="D49" s="6">
+      <c r="E49" s="6">
         <f>'2016'!E49</f>
         <v>2941239</v>
       </c>
-      <c r="E49" s="6">
+      <c r="F49" s="6">
         <f>'2015'!E49</f>
         <v>2968341</v>
       </c>
-      <c r="F49" s="6">
+      <c r="G49" s="6">
         <f>'2014'!E49</f>
         <v>2880270</v>
       </c>
-      <c r="G49" s="6">
+      <c r="H49" s="6">
         <f>'2013'!E49</f>
         <v>2941549</v>
       </c>
-      <c r="H49" s="6">
+      <c r="I49" s="6">
         <f>'2012'!E49</f>
         <v>3041084</v>
       </c>
-      <c r="I49" s="6">
+      <c r="J49" s="6">
         <f>'2011'!E49</f>
         <v>2972072</v>
       </c>
-      <c r="J49" s="6">
+      <c r="K49" s="6">
         <f>'2010'!E49</f>
         <v>2887881</v>
       </c>
-      <c r="K49" s="6">
+      <c r="L49" s="6">
         <f>'2009'!E49</f>
         <v>3072436</v>
       </c>
-      <c r="L49" s="6">
+      <c r="M49" s="6">
         <f>'2008'!E49</f>
         <v>3072436</v>
       </c>
-      <c r="M49" s="6">
+      <c r="N49" s="6">
         <f>'2007'!E49</f>
         <v>3143230</v>
       </c>
-      <c r="N49" s="6">
+      <c r="O49" s="6">
         <f>'2006'!E49</f>
         <v>3030609</v>
       </c>
-      <c r="O49" s="6">
+      <c r="P49" s="6">
         <f>'2005'!E49</f>
         <v>2717877</v>
       </c>
-      <c r="P49" s="6">
+      <c r="Q49" s="6">
         <f>'2004'!E49</f>
         <v>2599506</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="6">
         <f>'2018'!E50</f>
         <v>677710</v>
       </c>
-      <c r="C50" s="6">
+      <c r="D50" s="6">
         <f>'2017'!E50</f>
         <v>705072</v>
       </c>
-      <c r="D50" s="6">
+      <c r="E50" s="6">
         <f>'2016'!E50</f>
         <v>719105</v>
       </c>
-      <c r="E50" s="6">
+      <c r="F50" s="6">
         <f>'2015'!E50</f>
         <v>704055</v>
       </c>
-      <c r="F50" s="6">
+      <c r="G50" s="6">
         <f>'2014'!E50</f>
         <v>684738</v>
       </c>
-      <c r="G50" s="6">
+      <c r="H50" s="6">
         <f>'2013'!E50</f>
         <v>710174</v>
       </c>
-      <c r="H50" s="6">
+      <c r="I50" s="6">
         <f>'2012'!E50</f>
         <v>778357</v>
       </c>
-      <c r="I50" s="6">
+      <c r="J50" s="6">
         <f>'2011'!E50</f>
         <v>767999</v>
       </c>
-      <c r="J50" s="6">
+      <c r="K50" s="6">
         <f>'2010'!E50</f>
         <v>736383</v>
       </c>
-      <c r="K50" s="6">
+      <c r="L50" s="6">
         <f>'2009'!E50</f>
         <v>753449</v>
       </c>
-      <c r="L50" s="6">
+      <c r="M50" s="6">
         <f>'2008'!E50</f>
         <v>753449</v>
       </c>
-      <c r="M50" s="6">
+      <c r="N50" s="6">
         <f>'2007'!E50</f>
         <v>738049</v>
       </c>
-      <c r="N50" s="6">
+      <c r="O50" s="6">
         <f>'2006'!E50</f>
         <v>949284</v>
       </c>
-      <c r="O50" s="6">
+      <c r="P50" s="6">
         <f>'2005'!E50</f>
         <v>926177</v>
       </c>
-      <c r="P50" s="6">
+      <c r="Q50" s="6">
         <f>'2004'!E50</f>
         <v>830748</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="6">
         <f>'2018'!E51</f>
         <v>247914</v>
       </c>
-      <c r="C51" s="6">
+      <c r="D51" s="6">
         <f>'2017'!E51</f>
         <v>240862</v>
       </c>
-      <c r="D51" s="6">
+      <c r="E51" s="6">
         <f>'2016'!E51</f>
         <v>249478</v>
       </c>
-      <c r="E51" s="6">
+      <c r="F51" s="6">
         <f>'2015'!E51</f>
         <v>261991</v>
       </c>
-      <c r="F51" s="6">
+      <c r="G51" s="6">
         <f>'2014'!E51</f>
         <v>264957</v>
       </c>
-      <c r="G51" s="6">
+      <c r="H51" s="6">
         <f>'2013'!E51</f>
         <v>269424</v>
       </c>
-      <c r="H51" s="6">
+      <c r="I51" s="6">
         <f>'2012'!E51</f>
         <v>265887</v>
       </c>
-      <c r="I51" s="6">
+      <c r="J51" s="6">
         <f>'2011'!E51</f>
         <v>260973</v>
       </c>
-      <c r="J51" s="6">
+      <c r="K51" s="6">
         <f>'2010'!E51</f>
         <v>278632</v>
       </c>
-      <c r="K51" s="6">
+      <c r="L51" s="6">
         <f>'2009'!E51</f>
         <v>266483</v>
       </c>
-      <c r="L51" s="6">
+      <c r="M51" s="6">
         <f>'2008'!E51</f>
         <v>266483</v>
       </c>
-      <c r="M51" s="6">
+      <c r="N51" s="6">
         <f>'2007'!E51</f>
         <v>249489</v>
       </c>
-      <c r="N51" s="6">
+      <c r="O51" s="6">
         <f>'2006'!E51</f>
         <v>242143</v>
       </c>
-      <c r="O51" s="6">
+      <c r="P51" s="6">
         <f>'2005'!E51</f>
         <v>228394</v>
       </c>
-      <c r="P51" s="6">
+      <c r="Q51" s="6">
         <f>'2004'!E51</f>
         <v>240898</v>
       </c>

</xml_diff>

<commit_message>
Fix 2018 links in hunting license spreadsheet
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="12" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="19" r:id="rId1"/>
@@ -1044,9 +1044,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1098,17 +1106,25 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -12085,8 +12101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -12128,31 +12144,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <f>'2018'!B2</f>
         <v>108921</v>
       </c>
       <c r="C2" s="6">
-        <f>'2018'!C2</f>
         <v>278248</v>
       </c>
       <c r="D2" s="6">
-        <f>'2018'!D2</f>
         <v>74532</v>
       </c>
       <c r="E2" s="6">
-        <f>'2018'!E2</f>
         <v>352780</v>
       </c>
       <c r="F2" s="6">
-        <f>Notes!B9</f>
         <v>2922692</v>
       </c>
       <c r="G2" s="6">
-        <f>Notes!C9</f>
         <v>5568901</v>
       </c>
       <c r="H2" s="7">
-        <f>'2018'!F2</f>
         <v>8491593</v>
       </c>
       <c r="I2" s="17">
@@ -12166,31 +12175,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <f>'2018'!B3</f>
         <v>547905</v>
       </c>
       <c r="C3" s="6">
-        <f>'2018'!C3</f>
         <v>542838</v>
       </c>
       <c r="D3" s="6">
-        <f>'2018'!D3</f>
         <v>37106</v>
       </c>
       <c r="E3" s="6">
-        <f>'2018'!E3</f>
         <v>579944</v>
       </c>
       <c r="F3" s="6">
-        <f>Notes!B10</f>
         <v>5693734</v>
       </c>
       <c r="G3" s="6">
-        <f>Notes!C10</f>
         <v>6107717</v>
       </c>
       <c r="H3" s="7">
-        <f>'2018'!F3</f>
         <v>11801451</v>
       </c>
       <c r="I3" s="17">
@@ -12204,31 +12206,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="6">
-        <f>'2018'!B4</f>
         <v>326559</v>
       </c>
       <c r="C4" s="6">
-        <f>'2018'!C4</f>
         <v>380102</v>
       </c>
       <c r="D4" s="6">
-        <f>'2018'!D4</f>
         <v>136944</v>
       </c>
       <c r="E4" s="6">
-        <f>'2018'!E4</f>
         <v>517046</v>
       </c>
       <c r="F4" s="6">
-        <f>Notes!B11</f>
         <v>8186097</v>
       </c>
       <c r="G4" s="6">
-        <f>Notes!C11</f>
         <v>10579420</v>
       </c>
       <c r="H4" s="7">
-        <f>'2018'!F4</f>
         <v>18765517</v>
       </c>
       <c r="I4" s="17">
@@ -12242,31 +12237,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <f>'2018'!B5</f>
         <v>305214</v>
       </c>
       <c r="C5" s="6">
-        <f>'2018'!C5</f>
         <v>456140</v>
       </c>
       <c r="D5" s="6">
-        <f>'2018'!D5</f>
         <v>61607</v>
       </c>
       <c r="E5" s="6">
-        <f>'2018'!E5</f>
         <v>517747</v>
       </c>
       <c r="F5" s="6">
-        <f>Notes!B12</f>
         <v>13358303</v>
       </c>
       <c r="G5" s="6">
-        <f>Notes!C12</f>
         <v>4515780</v>
       </c>
       <c r="H5" s="7">
-        <f>'2018'!F5</f>
         <v>17874083</v>
       </c>
       <c r="I5" s="17">
@@ -12279,31 +12267,24 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <f>'2018'!B6</f>
         <v>280967</v>
       </c>
       <c r="C6" s="6">
-        <f>'2018'!C6</f>
         <v>1007422</v>
       </c>
       <c r="D6" s="6">
-        <f>'2018'!D6</f>
         <v>22738</v>
       </c>
       <c r="E6" s="6">
-        <f>'2018'!E6</f>
         <v>1030160</v>
       </c>
       <c r="F6" s="6">
-        <f>Notes!B13</f>
         <v>20609712</v>
       </c>
       <c r="G6" s="6">
-        <f>Notes!C13</f>
         <v>1006282</v>
       </c>
       <c r="H6" s="7">
-        <f>'2018'!F6</f>
         <v>21615994</v>
       </c>
       <c r="I6" s="17">
@@ -12316,31 +12297,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <f>'2018'!B7</f>
         <v>294319</v>
       </c>
       <c r="C7" s="6">
-        <f>'2018'!C7</f>
         <v>459518</v>
       </c>
       <c r="D7" s="6">
-        <f>'2018'!D7</f>
         <v>109246</v>
       </c>
       <c r="E7" s="6">
-        <f>'2018'!E7</f>
         <v>568764</v>
       </c>
       <c r="F7" s="6">
-        <f>Notes!B14</f>
         <v>12751122</v>
       </c>
       <c r="G7" s="6">
-        <f>Notes!C14</f>
         <v>44305473</v>
       </c>
       <c r="H7" s="7">
-        <f>'2018'!F7</f>
         <v>57056595</v>
       </c>
       <c r="I7" s="17">
@@ -12353,31 +12327,24 @@
         <v>7</v>
       </c>
       <c r="B8" s="6">
-        <f>'2018'!B8</f>
         <v>37489</v>
       </c>
       <c r="C8" s="6">
-        <f>'2018'!C8</f>
         <v>124169</v>
       </c>
       <c r="D8" s="6">
-        <f>'2018'!D8</f>
         <v>4063</v>
       </c>
       <c r="E8" s="6">
-        <f>'2018'!E8</f>
         <v>128232</v>
       </c>
       <c r="F8" s="6">
-        <f>Notes!B15</f>
         <v>2085367</v>
       </c>
       <c r="G8" s="6">
-        <f>Notes!C15</f>
         <v>394950</v>
       </c>
       <c r="H8" s="7">
-        <f>'2018'!F8</f>
         <v>2480317</v>
       </c>
       <c r="I8" s="17">
@@ -12390,31 +12357,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <f>'2018'!B9</f>
         <v>17847</v>
       </c>
       <c r="C9" s="6">
-        <f>'2018'!C9</f>
         <v>52315</v>
       </c>
       <c r="D9" s="6">
-        <f>'2018'!D9</f>
         <v>7125</v>
       </c>
       <c r="E9" s="6">
-        <f>'2018'!E9</f>
         <v>59440</v>
       </c>
       <c r="F9" s="6">
-        <f>Notes!B16</f>
         <v>632742</v>
       </c>
       <c r="G9" s="6">
-        <f>Notes!C16</f>
         <v>372462</v>
       </c>
       <c r="H9" s="7">
-        <f>'2018'!F9</f>
         <v>1005204</v>
       </c>
       <c r="I9" s="17">
@@ -12427,31 +12387,24 @@
         <v>9</v>
       </c>
       <c r="B10" s="6">
-        <f>'2018'!B10</f>
         <v>190232</v>
       </c>
       <c r="C10" s="6">
-        <f>'2018'!C10</f>
         <v>313554</v>
       </c>
       <c r="D10" s="6">
-        <f>'2018'!D10</f>
         <v>18155</v>
       </c>
       <c r="E10" s="6">
-        <f>'2018'!E10</f>
         <v>331709</v>
       </c>
       <c r="F10" s="6">
-        <f>Notes!B17</f>
         <v>7890888</v>
       </c>
       <c r="G10" s="6">
-        <f>Notes!C17</f>
         <v>984031</v>
       </c>
       <c r="H10" s="7">
-        <f>'2018'!F10</f>
         <v>8874919</v>
       </c>
       <c r="I10" s="17">
@@ -12464,31 +12417,24 @@
         <v>10</v>
       </c>
       <c r="B11" s="6">
-        <f>'2018'!B11</f>
         <v>651910</v>
       </c>
       <c r="C11" s="6">
-        <f>'2018'!C11</f>
         <v>1297350</v>
       </c>
       <c r="D11" s="6">
-        <f>'2018'!D11</f>
         <v>166091</v>
       </c>
       <c r="E11" s="6">
-        <f>'2018'!E11</f>
         <v>1463441</v>
       </c>
       <c r="F11" s="6">
-        <f>Notes!B18</f>
         <v>6627327</v>
       </c>
       <c r="G11" s="6">
-        <f>Notes!C18</f>
         <v>7132438</v>
       </c>
       <c r="H11" s="7">
-        <f>'2018'!F11</f>
         <v>13759765</v>
       </c>
       <c r="I11" s="17">
@@ -12501,31 +12447,24 @@
         <v>11</v>
       </c>
       <c r="B12" s="6">
-        <f>'2018'!B12</f>
         <v>10617</v>
       </c>
       <c r="C12" s="6">
-        <f>'2018'!C12</f>
         <v>11068</v>
       </c>
       <c r="D12" s="1">
-        <f>'2018'!D12</f>
         <v>734</v>
       </c>
       <c r="E12" s="6">
-        <f>'2018'!E12</f>
         <v>11802</v>
       </c>
       <c r="F12" s="6">
-        <f>Notes!B19</f>
         <v>501285</v>
       </c>
       <c r="G12" s="6">
-        <f>Notes!C19</f>
         <v>77070</v>
       </c>
       <c r="H12" s="7">
-        <f>'2018'!F12</f>
         <v>578355</v>
       </c>
       <c r="I12" s="17">
@@ -12538,31 +12477,24 @@
         <v>12</v>
       </c>
       <c r="B13" s="6">
-        <f>'2018'!B13</f>
         <v>223232</v>
       </c>
       <c r="C13" s="6">
-        <f>'2018'!C13</f>
         <v>516446</v>
       </c>
       <c r="D13" s="6">
-        <f>'2018'!D13</f>
         <v>67438</v>
       </c>
       <c r="E13" s="6">
-        <f>'2018'!E13</f>
         <v>583884</v>
       </c>
       <c r="F13" s="6">
-        <f>Notes!B20</f>
         <v>10772431</v>
       </c>
       <c r="G13" s="6">
-        <f>Notes!C20</f>
         <v>6940825</v>
       </c>
       <c r="H13" s="7">
-        <f>'2018'!F13</f>
         <v>17713256</v>
       </c>
       <c r="I13" s="17">
@@ -12575,31 +12507,24 @@
         <v>13</v>
       </c>
       <c r="B14" s="6">
-        <f>'2018'!B14</f>
         <v>286947</v>
       </c>
       <c r="C14" s="6">
-        <f>'2018'!C14</f>
         <v>1047773</v>
       </c>
       <c r="D14" s="6">
-        <f>'2018'!D14</f>
         <v>159224</v>
       </c>
       <c r="E14" s="6">
-        <f>'2018'!E14</f>
         <v>1206997</v>
       </c>
       <c r="F14" s="6">
-        <f>Notes!B21</f>
         <v>10454861</v>
       </c>
       <c r="G14" s="6">
-        <f>Notes!C21</f>
         <v>15200880</v>
       </c>
       <c r="H14" s="7">
-        <f>'2018'!F14</f>
         <v>25655741</v>
       </c>
       <c r="I14" s="17">
@@ -12612,31 +12537,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="6">
-        <f>'2018'!B15</f>
         <v>306024</v>
       </c>
       <c r="C15" s="6">
-        <f>'2018'!C15</f>
         <v>1203507</v>
       </c>
       <c r="D15" s="6">
-        <f>'2018'!D15</f>
         <v>83025</v>
       </c>
       <c r="E15" s="6">
-        <f>'2018'!E15</f>
         <v>1286532</v>
       </c>
       <c r="F15" s="6">
-        <f>Notes!B22</f>
         <v>16424426</v>
       </c>
       <c r="G15" s="6">
-        <f>Notes!C22</f>
         <v>15520789</v>
       </c>
       <c r="H15" s="7">
-        <f>'2018'!F15</f>
         <v>31945215</v>
       </c>
       <c r="I15" s="17">
@@ -12649,31 +12567,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="6">
-        <f>'2018'!B16</f>
         <v>267447</v>
       </c>
       <c r="C16" s="6">
-        <f>'2018'!C16</f>
         <v>383958</v>
       </c>
       <c r="D16" s="6">
-        <f>'2018'!D16</f>
         <v>20781</v>
       </c>
       <c r="E16" s="6">
-        <f>'2018'!E16</f>
         <v>404739</v>
       </c>
       <c r="F16" s="6">
-        <f>Notes!B23</f>
         <v>9358292</v>
       </c>
       <c r="G16" s="6">
-        <f>Notes!C23</f>
         <v>2300953</v>
       </c>
       <c r="H16" s="7">
-        <f>'2018'!F16</f>
         <v>11659245</v>
       </c>
       <c r="I16" s="17">
@@ -12686,31 +12597,24 @@
         <v>16</v>
       </c>
       <c r="B17" s="6">
-        <f>'2018'!B17</f>
         <v>251390</v>
       </c>
       <c r="C17" s="6">
-        <f>'2018'!C17</f>
         <v>349199</v>
       </c>
       <c r="D17" s="6">
-        <f>'2018'!D17</f>
         <v>170676</v>
       </c>
       <c r="E17" s="6">
-        <f>'2018'!E17</f>
         <v>519875</v>
       </c>
       <c r="F17" s="6">
-        <f>Notes!B24</f>
         <v>6732462</v>
       </c>
       <c r="G17" s="6">
-        <f>Notes!C24</f>
         <v>12704150</v>
       </c>
       <c r="H17" s="7">
-        <f>'2018'!F17</f>
         <v>19436612</v>
       </c>
       <c r="I17" s="17">
@@ -12723,31 +12627,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="6">
-        <f>'2018'!B18</f>
         <v>352408</v>
       </c>
       <c r="C18" s="6">
-        <f>'2018'!C18</f>
         <v>512113</v>
       </c>
       <c r="D18" s="6">
-        <f>'2018'!D18</f>
         <v>102629</v>
       </c>
       <c r="E18" s="6">
-        <f>'2018'!E18</f>
         <v>614742</v>
       </c>
       <c r="F18" s="6">
-        <f>Notes!B25</f>
         <v>12059992</v>
       </c>
       <c r="G18" s="6">
-        <f>Notes!C25</f>
         <v>7727579</v>
       </c>
       <c r="H18" s="7">
-        <f>'2018'!F18</f>
         <v>19787571</v>
       </c>
       <c r="I18" s="17">
@@ -12760,31 +12657,24 @@
         <v>18</v>
       </c>
       <c r="B19" s="6">
-        <f>'2018'!B19</f>
         <v>398808</v>
       </c>
       <c r="C19" s="6">
-        <f>'2018'!C19</f>
         <v>605336</v>
       </c>
       <c r="D19" s="6">
-        <f>'2018'!D19</f>
         <v>53323</v>
       </c>
       <c r="E19" s="6">
-        <f>'2018'!E19</f>
         <v>658659</v>
       </c>
       <c r="F19" s="6">
-        <f>Notes!B26</f>
         <v>7954155</v>
       </c>
       <c r="G19" s="6">
-        <f>Notes!C26</f>
         <v>2043839</v>
       </c>
       <c r="H19" s="7">
-        <f>'2018'!F19</f>
         <v>9997994</v>
       </c>
       <c r="I19" s="17">
@@ -12797,31 +12687,24 @@
         <v>19</v>
       </c>
       <c r="B20" s="6">
-        <f>'2018'!B20</f>
         <v>57921</v>
       </c>
       <c r="C20" s="6">
-        <f>'2018'!C20</f>
         <v>246052</v>
       </c>
       <c r="D20" s="6">
-        <f>'2018'!D20</f>
         <v>15504</v>
       </c>
       <c r="E20" s="6">
-        <f>'2018'!E20</f>
         <v>261556</v>
       </c>
       <c r="F20" s="6">
-        <f>Notes!B27</f>
         <v>2009739</v>
       </c>
       <c r="G20" s="6">
-        <f>Notes!C27</f>
         <v>396357</v>
       </c>
       <c r="H20" s="7">
-        <f>'2018'!F20</f>
         <v>2406096</v>
       </c>
       <c r="I20" s="17">
@@ -12834,31 +12717,24 @@
         <v>20</v>
       </c>
       <c r="B21" s="6">
-        <f>'2018'!B21</f>
         <v>120334</v>
       </c>
       <c r="C21" s="6">
-        <f>'2018'!C21</f>
         <v>284941</v>
       </c>
       <c r="D21" s="6">
-        <f>'2018'!D21</f>
         <v>60270</v>
       </c>
       <c r="E21" s="6">
-        <f>'2018'!E21</f>
         <v>345211</v>
       </c>
       <c r="F21" s="6">
-        <f>Notes!B28</f>
         <v>3394548</v>
       </c>
       <c r="G21" s="6">
-        <f>Notes!C28</f>
         <v>2974503</v>
       </c>
       <c r="H21" s="7">
-        <f>'2018'!F21</f>
         <v>6369051</v>
       </c>
       <c r="I21" s="17">
@@ -12871,31 +12747,24 @@
         <v>21</v>
       </c>
       <c r="B22" s="6">
-        <f>'2018'!B22</f>
         <v>163191</v>
       </c>
       <c r="C22" s="6">
-        <f>'2018'!C22</f>
         <v>214767</v>
       </c>
       <c r="D22" s="6">
-        <f>'2018'!D22</f>
         <v>34323</v>
       </c>
       <c r="E22" s="6">
-        <f>'2018'!E22</f>
         <v>249090</v>
       </c>
       <c r="F22" s="6">
-        <f>Notes!B29</f>
         <v>4635181</v>
       </c>
       <c r="G22" s="6">
-        <f>Notes!C29</f>
         <v>3236598</v>
       </c>
       <c r="H22" s="7">
-        <f>'2018'!F22</f>
         <v>7871779</v>
       </c>
       <c r="I22" s="17">
@@ -12908,31 +12777,24 @@
         <v>22</v>
       </c>
       <c r="B23" s="6">
-        <f>'2018'!B23</f>
         <v>706101</v>
       </c>
       <c r="C23" s="6">
-        <f>'2018'!C23</f>
         <v>2171384</v>
       </c>
       <c r="D23" s="6">
-        <f>'2018'!D23</f>
         <v>52786</v>
       </c>
       <c r="E23" s="6">
-        <f>'2018'!E23</f>
         <v>2224170</v>
       </c>
       <c r="F23" s="6">
-        <f>Notes!B30</f>
         <v>33009073</v>
       </c>
       <c r="G23" s="6">
-        <f>Notes!C30</f>
         <v>4045709</v>
       </c>
       <c r="H23" s="7">
-        <f>'2018'!F23</f>
         <v>37054782</v>
       </c>
       <c r="I23" s="17">
@@ -12945,31 +12807,24 @@
         <v>23</v>
       </c>
       <c r="B24" s="6">
-        <f>'2018'!B24</f>
         <v>568057</v>
       </c>
       <c r="C24" s="6">
-        <f>'2018'!C24</f>
         <v>1376759</v>
       </c>
       <c r="D24" s="6">
-        <f>'2018'!D24</f>
         <v>44245</v>
       </c>
       <c r="E24" s="6">
-        <f>'2018'!E24</f>
         <v>1421004</v>
       </c>
       <c r="F24" s="6">
-        <f>Notes!B31</f>
         <v>27229500</v>
       </c>
       <c r="G24" s="6">
-        <f>Notes!C31</f>
         <v>3495674</v>
       </c>
       <c r="H24" s="7">
-        <f>'2018'!F24</f>
         <v>30725174</v>
       </c>
       <c r="I24" s="17">
@@ -12982,31 +12837,24 @@
         <v>24</v>
       </c>
       <c r="B25" s="6">
-        <f>'2018'!B25</f>
         <v>498319</v>
       </c>
       <c r="C25" s="6">
-        <f>'2018'!C25</f>
         <v>1702400</v>
       </c>
       <c r="D25" s="6">
-        <f>'2018'!D25</f>
         <v>79919</v>
       </c>
       <c r="E25" s="6">
-        <f>'2018'!E25</f>
         <v>1782319</v>
       </c>
       <c r="F25" s="6">
-        <f>Notes!B32</f>
         <v>12585185</v>
       </c>
       <c r="G25" s="6">
-        <f>Notes!C32</f>
         <v>8708655</v>
       </c>
       <c r="H25" s="7">
-        <f>'2018'!F25</f>
         <v>21293840</v>
       </c>
       <c r="I25" s="17">
@@ -13019,31 +12867,24 @@
         <v>25</v>
       </c>
       <c r="B26" s="6">
-        <f>'2018'!B26</f>
         <v>300146</v>
       </c>
       <c r="C26" s="6">
-        <f>'2018'!C26</f>
         <v>335324</v>
       </c>
       <c r="D26" s="6">
-        <f>'2018'!D26</f>
         <v>91402</v>
       </c>
       <c r="E26" s="6">
-        <f>'2018'!E26</f>
         <v>426726</v>
       </c>
       <c r="F26" s="6">
-        <f>Notes!B33</f>
         <v>4023594</v>
       </c>
       <c r="G26" s="6">
-        <f>Notes!C33</f>
         <v>8249067</v>
       </c>
       <c r="H26" s="7">
-        <f>'2018'!F26</f>
         <v>12272661</v>
       </c>
       <c r="I26" s="17">
@@ -13056,31 +12897,24 @@
         <v>26</v>
       </c>
       <c r="B27" s="6">
-        <f>'2018'!B27</f>
         <v>253412</v>
       </c>
       <c r="C27" s="6">
-        <f>'2018'!C27</f>
         <v>873323</v>
       </c>
       <c r="D27" s="6">
-        <f>'2018'!D27</f>
         <v>155658</v>
       </c>
       <c r="E27" s="6">
-        <f>'2018'!E27</f>
         <v>1028981</v>
       </c>
       <c r="F27" s="6">
-        <f>Notes!B34</f>
         <v>9459094</v>
       </c>
       <c r="G27" s="6">
-        <f>Notes!C34</f>
         <v>23458615</v>
       </c>
       <c r="H27" s="7">
-        <f>'2018'!F27</f>
         <v>32917709</v>
       </c>
       <c r="I27" s="17">
@@ -13093,31 +12927,24 @@
         <v>27</v>
       </c>
       <c r="B28" s="6">
-        <f>'2018'!B28</f>
         <v>585766</v>
       </c>
       <c r="C28" s="6">
-        <f>'2018'!C28</f>
         <v>319136</v>
       </c>
       <c r="D28" s="6">
-        <f>'2018'!D28</f>
         <v>25626</v>
       </c>
       <c r="E28" s="6">
-        <f>'2018'!E28</f>
         <v>344762</v>
       </c>
       <c r="F28" s="6">
-        <f>Notes!B35</f>
         <v>8629779</v>
       </c>
       <c r="G28" s="6">
-        <f>Notes!C35</f>
         <v>2127935</v>
       </c>
       <c r="H28" s="7">
-        <f>'2018'!F28</f>
         <v>10757714</v>
       </c>
       <c r="I28" s="17">
@@ -13130,31 +12957,24 @@
         <v>28</v>
       </c>
       <c r="B29" s="6">
-        <f>'2018'!B29</f>
         <v>141553</v>
       </c>
       <c r="C29" s="6">
-        <f>'2018'!C29</f>
         <v>362554</v>
       </c>
       <c r="D29" s="6">
-        <f>'2018'!D29</f>
         <v>157801</v>
       </c>
       <c r="E29" s="6">
-        <f>'2018'!E29</f>
         <v>520355</v>
       </c>
       <c r="F29" s="6">
-        <f>Notes!B36</f>
         <v>4257890</v>
       </c>
       <c r="G29" s="6">
-        <f>Notes!C36</f>
         <v>7553355</v>
       </c>
       <c r="H29" s="7">
-        <f>'2018'!F29</f>
         <v>11811245</v>
       </c>
       <c r="I29" s="17">
@@ -13167,31 +12987,24 @@
         <v>29</v>
       </c>
       <c r="B30" s="6">
-        <f>'2018'!B30</f>
         <v>183056</v>
       </c>
       <c r="C30" s="6">
-        <f>'2018'!C30</f>
         <v>339053</v>
       </c>
       <c r="D30" s="6">
-        <f>'2018'!D30</f>
         <v>90202</v>
       </c>
       <c r="E30" s="6">
-        <f>'2018'!E30</f>
         <v>429255</v>
       </c>
       <c r="F30" s="6">
-        <f>Notes!B37</f>
         <v>7565754</v>
       </c>
       <c r="G30" s="6">
-        <f>Notes!C37</f>
         <v>5935707</v>
       </c>
       <c r="H30" s="7">
-        <f>'2018'!F30</f>
         <v>13501461</v>
       </c>
       <c r="I30" s="17">
@@ -13204,31 +13017,24 @@
         <v>30</v>
       </c>
       <c r="B31" s="6">
-        <f>'2018'!B31</f>
         <v>58099</v>
       </c>
       <c r="C31" s="6">
-        <f>'2018'!C31</f>
         <v>186931</v>
       </c>
       <c r="D31" s="6">
-        <f>'2018'!D31</f>
         <v>31411</v>
       </c>
       <c r="E31" s="6">
-        <f>'2018'!E31</f>
         <v>218342</v>
       </c>
       <c r="F31" s="6">
-        <f>Notes!B38</f>
         <v>2646432</v>
       </c>
       <c r="G31" s="6">
-        <f>Notes!C38</f>
         <v>1370915</v>
       </c>
       <c r="H31" s="7">
-        <f>'2018'!F31</f>
         <v>4017347</v>
       </c>
       <c r="I31" s="17">
@@ -13241,31 +13047,24 @@
         <v>31</v>
       </c>
       <c r="B32" s="6">
-        <f>'2018'!B32</f>
         <v>74794</v>
       </c>
       <c r="C32" s="6">
-        <f>'2018'!C32</f>
         <v>303795</v>
       </c>
       <c r="D32" s="6">
-        <f>'2018'!D32</f>
         <v>118442</v>
       </c>
       <c r="E32" s="6">
-        <f>'2018'!E32</f>
         <v>422237</v>
       </c>
       <c r="F32" s="6">
-        <f>Notes!B39</f>
         <v>6981229</v>
       </c>
       <c r="G32" s="6">
-        <f>Notes!C39</f>
         <v>1147736</v>
       </c>
       <c r="H32" s="7">
-        <f>'2018'!F32</f>
         <v>8128965</v>
       </c>
       <c r="I32" s="17">
@@ -13278,31 +13077,24 @@
         <v>32</v>
       </c>
       <c r="B33" s="6">
-        <f>'2018'!B33</f>
         <v>107331</v>
       </c>
       <c r="C33" s="6">
-        <f>'2018'!C33</f>
         <v>329423</v>
       </c>
       <c r="D33" s="6">
-        <f>'2018'!D33</f>
         <v>112483</v>
       </c>
       <c r="E33" s="6">
-        <f>'2018'!E33</f>
         <v>441906</v>
       </c>
       <c r="F33" s="6">
-        <f>Notes!B40</f>
         <v>5866269</v>
       </c>
       <c r="G33" s="6">
-        <f>Notes!C40</f>
         <v>10319383</v>
       </c>
       <c r="H33" s="7">
-        <f>'2018'!F33</f>
         <v>16185652</v>
       </c>
       <c r="I33" s="17">
@@ -13315,31 +13107,24 @@
         <v>33</v>
       </c>
       <c r="B34" s="6">
-        <f>'2018'!B34</f>
         <v>68744</v>
       </c>
       <c r="C34" s="6">
-        <f>'2018'!C34</f>
         <v>123271</v>
       </c>
       <c r="D34" s="6">
-        <f>'2018'!D34</f>
         <v>26840</v>
       </c>
       <c r="E34" s="6">
-        <f>'2018'!E34</f>
         <v>150111</v>
       </c>
       <c r="F34" s="6">
-        <f>Notes!B41</f>
         <v>3920404</v>
       </c>
       <c r="G34" s="6">
-        <f>Notes!C41</f>
         <v>3829980</v>
       </c>
       <c r="H34" s="7">
-        <f>'2018'!F34</f>
         <v>7750384</v>
       </c>
       <c r="I34" s="17">
@@ -13352,31 +13137,24 @@
         <v>34</v>
       </c>
       <c r="B35" s="6">
-        <f>'2018'!B35</f>
         <v>579043</v>
       </c>
       <c r="C35" s="6">
-        <f>'2018'!C35</f>
         <v>1117576</v>
       </c>
       <c r="D35" s="6">
-        <f>'2018'!D35</f>
         <v>48773</v>
       </c>
       <c r="E35" s="6">
-        <f>'2018'!E35</f>
         <v>1166349</v>
       </c>
       <c r="F35" s="6">
-        <f>Notes!B42</f>
         <v>17441081</v>
       </c>
       <c r="G35" s="6">
-        <f>Notes!C42</f>
         <v>4177215</v>
       </c>
       <c r="H35" s="7">
-        <f>'2018'!F35</f>
         <v>21618296</v>
       </c>
       <c r="I35" s="17">
@@ -13389,31 +13167,24 @@
         <v>35</v>
       </c>
       <c r="B36" s="6">
-        <f>'2018'!B36</f>
         <v>390268</v>
       </c>
       <c r="C36" s="6">
-        <f>'2018'!C36</f>
         <v>895099</v>
       </c>
       <c r="D36" s="6">
-        <f>'2018'!D36</f>
         <v>100065</v>
       </c>
       <c r="E36" s="6">
-        <f>'2018'!E36</f>
         <v>995164</v>
       </c>
       <c r="F36" s="6">
-        <f>Notes!B43</f>
         <v>16259079</v>
       </c>
       <c r="G36" s="6">
-        <f>Notes!C43</f>
         <v>6378876</v>
       </c>
       <c r="H36" s="7">
-        <f>'2018'!F36</f>
         <v>22637955</v>
       </c>
       <c r="I36" s="17">
@@ -13426,31 +13197,24 @@
         <v>36</v>
       </c>
       <c r="B37" s="6">
-        <f>'2018'!B37</f>
         <v>529651</v>
       </c>
       <c r="C37" s="6">
-        <f>'2018'!C37</f>
         <v>377498</v>
       </c>
       <c r="D37" s="6">
-        <f>'2018'!D37</f>
         <v>22740</v>
       </c>
       <c r="E37" s="6">
-        <f>'2018'!E37</f>
         <v>400238</v>
       </c>
       <c r="F37" s="6">
-        <f>Notes!B44</f>
         <v>5735625</v>
       </c>
       <c r="G37" s="6">
-        <f>Notes!C44</f>
         <v>3870723</v>
       </c>
       <c r="H37" s="7">
-        <f>'2018'!F37</f>
         <v>9606348</v>
       </c>
       <c r="I37" s="17">
@@ -13463,31 +13227,24 @@
         <v>37</v>
       </c>
       <c r="B38" s="6">
-        <f>'2018'!B38</f>
         <v>264684</v>
       </c>
       <c r="C38" s="6">
-        <f>'2018'!C38</f>
         <v>1173427</v>
       </c>
       <c r="D38" s="6">
-        <f>'2018'!D38</f>
         <v>49243</v>
       </c>
       <c r="E38" s="6">
-        <f>'2018'!E38</f>
         <v>1222670</v>
       </c>
       <c r="F38" s="6">
-        <f>Notes!B45</f>
         <v>20982703</v>
       </c>
       <c r="G38" s="6">
-        <f>Notes!C45</f>
         <v>5416770</v>
       </c>
       <c r="H38" s="7">
-        <f>'2018'!F38</f>
         <v>26399473</v>
       </c>
       <c r="I38" s="17">
@@ -13500,31 +13257,24 @@
         <v>38</v>
       </c>
       <c r="B39" s="6">
-        <f>'2018'!B39</f>
         <v>975650</v>
       </c>
       <c r="C39" s="6">
-        <f>'2018'!C39</f>
         <v>2468652</v>
       </c>
       <c r="D39" s="6">
-        <f>'2018'!D39</f>
         <v>101278</v>
       </c>
       <c r="E39" s="6">
-        <f>'2018'!E39</f>
         <v>2569930</v>
       </c>
       <c r="F39" s="6">
-        <f>Notes!B46</f>
         <v>30352406</v>
       </c>
       <c r="G39" s="6">
-        <f>Notes!C46</f>
         <v>6079410</v>
       </c>
       <c r="H39" s="7">
-        <f>'2018'!F39</f>
         <v>36431816</v>
       </c>
       <c r="I39" s="17">
@@ -13537,31 +13287,24 @@
         <v>39</v>
       </c>
       <c r="B40" s="6">
-        <f>'2018'!B40</f>
         <v>8209</v>
       </c>
       <c r="C40" s="6">
-        <f>'2018'!C40</f>
         <v>26515</v>
       </c>
       <c r="D40" s="6">
-        <f>'2018'!D40</f>
         <v>4388</v>
       </c>
       <c r="E40" s="6">
-        <f>'2018'!E40</f>
         <v>30903</v>
       </c>
       <c r="F40" s="6">
-        <f>Notes!B47</f>
         <v>362093</v>
       </c>
       <c r="G40" s="6">
-        <f>Notes!C47</f>
         <v>121483</v>
       </c>
       <c r="H40" s="7">
-        <f>'2018'!F40</f>
         <v>483576</v>
       </c>
       <c r="I40" s="17">
@@ -13574,31 +13317,24 @@
         <v>40</v>
       </c>
       <c r="B41" s="6">
-        <f>'2018'!B41</f>
         <v>210369</v>
       </c>
       <c r="C41" s="6">
-        <f>'2018'!C41</f>
         <v>722055</v>
       </c>
       <c r="D41" s="6">
-        <f>'2018'!D41</f>
         <v>92230</v>
       </c>
       <c r="E41" s="6">
-        <f>'2018'!E41</f>
         <v>814285</v>
       </c>
       <c r="F41" s="6">
-        <f>Notes!B48</f>
         <v>5434146</v>
       </c>
       <c r="G41" s="6">
-        <f>Notes!C48</f>
         <v>4283172</v>
       </c>
       <c r="H41" s="7">
-        <f>'2018'!F41</f>
         <v>9717318</v>
       </c>
       <c r="I41" s="17">
@@ -13611,31 +13347,24 @@
         <v>41</v>
       </c>
       <c r="B42" s="6">
-        <f>'2018'!B42</f>
         <v>233215</v>
       </c>
       <c r="C42" s="6">
-        <f>'2018'!C42</f>
         <v>245474</v>
       </c>
       <c r="D42" s="6">
-        <f>'2018'!D42</f>
         <v>128502</v>
       </c>
       <c r="E42" s="6">
-        <f>'2018'!E42</f>
         <v>373976</v>
       </c>
       <c r="F42" s="6">
-        <f>Notes!B49</f>
         <v>7186745</v>
       </c>
       <c r="G42" s="6">
-        <f>Notes!C49</f>
         <v>14874974</v>
       </c>
       <c r="H42" s="7">
-        <f>'2018'!F42</f>
         <v>22061719</v>
       </c>
       <c r="I42" s="17">
@@ -13648,31 +13377,24 @@
         <v>42</v>
       </c>
       <c r="B43" s="6">
-        <f>'2018'!B43</f>
         <v>700600</v>
       </c>
       <c r="C43" s="6">
-        <f>'2018'!C43</f>
         <v>696906</v>
       </c>
       <c r="D43" s="6">
-        <f>'2018'!D43</f>
         <v>40267</v>
       </c>
       <c r="E43" s="6">
-        <f>'2018'!E43</f>
         <v>737173</v>
       </c>
       <c r="F43" s="6">
-        <f>Notes!B50</f>
         <v>17016820</v>
       </c>
       <c r="G43" s="6">
-        <f>Notes!C50</f>
         <v>3703363</v>
       </c>
       <c r="H43" s="7">
-        <f>'2018'!F43</f>
         <v>20720183</v>
       </c>
       <c r="I43" s="17">
@@ -13685,31 +13407,24 @@
         <v>43</v>
       </c>
       <c r="B44" s="6">
-        <f>'2018'!B44</f>
         <v>1157779</v>
       </c>
       <c r="C44" s="6">
-        <f>'2018'!C44</f>
         <v>1575985</v>
       </c>
       <c r="D44" s="6">
-        <f>'2018'!D44</f>
         <v>79358</v>
       </c>
       <c r="E44" s="6">
-        <f>'2018'!E44</f>
         <v>1655343</v>
       </c>
       <c r="F44" s="6">
-        <f>Notes!B51</f>
         <v>35200343</v>
       </c>
       <c r="G44" s="6">
-        <f>Notes!C51</f>
         <v>11017420</v>
       </c>
       <c r="H44" s="7">
-        <f>'2018'!F44</f>
         <v>46217763</v>
       </c>
       <c r="I44" s="17">
@@ -13722,31 +13437,24 @@
         <v>44</v>
       </c>
       <c r="B45" s="6">
-        <f>'2018'!B45</f>
         <v>236656</v>
       </c>
       <c r="C45" s="6">
-        <f>'2018'!C45</f>
         <v>379805</v>
       </c>
       <c r="D45" s="6">
-        <f>'2018'!D45</f>
         <v>41036</v>
       </c>
       <c r="E45" s="6">
-        <f>'2018'!E45</f>
         <v>420841</v>
       </c>
       <c r="F45" s="6">
-        <f>Notes!B52</f>
         <v>11216469</v>
       </c>
       <c r="G45" s="6">
-        <f>Notes!C52</f>
         <v>5545567</v>
       </c>
       <c r="H45" s="7">
-        <f>'2018'!F45</f>
         <v>16762036</v>
       </c>
       <c r="I45" s="17">
@@ -13759,31 +13467,24 @@
         <v>45</v>
       </c>
       <c r="B46" s="6">
-        <f>'2018'!B46</f>
         <v>276019</v>
       </c>
       <c r="C46" s="6">
-        <f>'2018'!C46</f>
         <v>815464</v>
       </c>
       <c r="D46" s="6">
-        <f>'2018'!D46</f>
         <v>44611</v>
       </c>
       <c r="E46" s="6">
-        <f>'2018'!E46</f>
         <v>860075</v>
       </c>
       <c r="F46" s="6">
-        <f>Notes!B53</f>
         <v>17488685</v>
       </c>
       <c r="G46" s="6">
-        <f>Notes!C53</f>
         <v>3815542</v>
       </c>
       <c r="H46" s="7">
-        <f>'2018'!F46</f>
         <v>21304227</v>
       </c>
       <c r="I46" s="17">
@@ -13796,31 +13497,24 @@
         <v>46</v>
       </c>
       <c r="B47" s="6">
-        <f>'2018'!B47</f>
         <v>69943</v>
       </c>
       <c r="C47" s="6">
-        <f>'2018'!C47</f>
         <v>153476</v>
       </c>
       <c r="D47" s="6">
-        <f>'2018'!D47</f>
         <v>15852</v>
       </c>
       <c r="E47" s="6">
-        <f>'2018'!E47</f>
         <v>169328</v>
       </c>
       <c r="F47" s="6">
-        <f>Notes!B54</f>
         <v>2975620</v>
       </c>
       <c r="G47" s="6">
-        <f>Notes!C54</f>
         <v>989935</v>
       </c>
       <c r="H47" s="7">
-        <f>'2018'!F47</f>
         <v>3965555</v>
       </c>
       <c r="I47" s="17">
@@ -13833,31 +13527,24 @@
         <v>47</v>
       </c>
       <c r="B48" s="6">
-        <f>'2018'!B48</f>
         <v>183063</v>
       </c>
       <c r="C48" s="6">
-        <f>'2018'!C48</f>
         <v>681049</v>
       </c>
       <c r="D48" s="6">
-        <f>'2018'!D48</f>
         <v>10683</v>
       </c>
       <c r="E48" s="6">
-        <f>'2018'!E48</f>
         <v>691732</v>
       </c>
       <c r="F48" s="6">
-        <f>Notes!B55</f>
         <v>16129772</v>
       </c>
       <c r="G48" s="6">
-        <f>Notes!C55</f>
         <v>1062087</v>
       </c>
       <c r="H48" s="7">
-        <f>'2018'!F48</f>
         <v>17191859</v>
       </c>
       <c r="I48" s="17">
@@ -13870,31 +13557,24 @@
         <v>48</v>
       </c>
       <c r="B49" s="6">
-        <f>'2018'!B49</f>
         <v>706400</v>
       </c>
       <c r="C49" s="6">
-        <f>'2018'!C49</f>
         <v>2716899</v>
       </c>
       <c r="D49" s="6">
-        <f>'2018'!D49</f>
         <v>146777</v>
       </c>
       <c r="E49" s="6">
-        <f>'2018'!E49</f>
         <v>2863676</v>
       </c>
       <c r="F49" s="6">
-        <f>Notes!B56</f>
         <v>33771619</v>
       </c>
       <c r="G49" s="6">
-        <f>Notes!C56</f>
         <v>7609753</v>
       </c>
       <c r="H49" s="7">
-        <f>'2018'!F49</f>
         <v>41381372</v>
       </c>
       <c r="I49" s="17">
@@ -13907,31 +13587,24 @@
         <v>49</v>
       </c>
       <c r="B50" s="6">
-        <f>'2018'!B50</f>
         <v>217123</v>
       </c>
       <c r="C50" s="6">
-        <f>'2018'!C50</f>
         <v>537767</v>
       </c>
       <c r="D50" s="6">
-        <f>'2018'!D50</f>
         <v>139943</v>
       </c>
       <c r="E50" s="6">
-        <f>'2018'!E50</f>
         <v>677710</v>
       </c>
       <c r="F50" s="6">
-        <f>Notes!B57</f>
         <v>4354126</v>
       </c>
       <c r="G50" s="6">
-        <f>Notes!C57</f>
         <v>4868774</v>
       </c>
       <c r="H50" s="7">
-        <f>'2018'!F50</f>
         <v>9222900</v>
       </c>
       <c r="I50" s="17">
@@ -13944,31 +13617,24 @@
         <v>50</v>
       </c>
       <c r="B51" s="6">
-        <f>'2018'!B51</f>
         <v>130304</v>
       </c>
       <c r="C51" s="6">
-        <f>'2018'!C51</f>
         <v>176549</v>
       </c>
       <c r="D51" s="6">
-        <f>'2018'!D51</f>
         <v>71365</v>
       </c>
       <c r="E51" s="6">
-        <f>'2018'!E51</f>
         <v>247914</v>
       </c>
       <c r="F51" s="6">
-        <f>Notes!B58</f>
         <v>6484947</v>
       </c>
       <c r="G51" s="6">
-        <f>Notes!C58</f>
         <v>18388025</v>
       </c>
       <c r="H51" s="7">
-        <f>'2018'!F51</f>
         <v>24872972</v>
       </c>
       <c r="I51" s="17">
@@ -17476,7 +17142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -17546,9 +17214,11 @@
         <v>1</v>
       </c>
       <c r="B9" s="7">
+        <f>'2018-Full'!F2</f>
         <v>2922692</v>
       </c>
       <c r="C9" s="7">
+        <f>'2018-Full'!G2</f>
         <v>5568901</v>
       </c>
       <c r="D9" s="9">
@@ -17569,9 +17239,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="7">
+        <f>'2018-Full'!F3</f>
         <v>5693734</v>
       </c>
       <c r="C10" s="7">
+        <f>'2018-Full'!G3</f>
         <v>6107717</v>
       </c>
       <c r="D10" s="9">
@@ -17592,9 +17264,11 @@
         <v>3</v>
       </c>
       <c r="B11" s="7">
+        <f>'2018-Full'!F4</f>
         <v>8186097</v>
       </c>
       <c r="C11" s="7">
+        <f>'2018-Full'!G4</f>
         <v>10579420</v>
       </c>
       <c r="D11" s="9">
@@ -17615,9 +17289,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="7">
+        <f>'2018-Full'!F5</f>
         <v>13358303</v>
       </c>
       <c r="C12" s="7">
+        <f>'2018-Full'!G5</f>
         <v>4515780</v>
       </c>
       <c r="D12" s="9">
@@ -17638,9 +17314,11 @@
         <v>5</v>
       </c>
       <c r="B13" s="7">
+        <f>'2018-Full'!F6</f>
         <v>20609712</v>
       </c>
       <c r="C13" s="7">
+        <f>'2018-Full'!G6</f>
         <v>1006282</v>
       </c>
       <c r="D13" s="9">
@@ -17661,9 +17339,11 @@
         <v>6</v>
       </c>
       <c r="B14" s="7">
+        <f>'2018-Full'!F7</f>
         <v>12751122</v>
       </c>
       <c r="C14" s="7">
+        <f>'2018-Full'!G7</f>
         <v>44305473</v>
       </c>
       <c r="D14" s="9">
@@ -17684,9 +17364,11 @@
         <v>7</v>
       </c>
       <c r="B15" s="7">
+        <f>'2018-Full'!F8</f>
         <v>2085367</v>
       </c>
       <c r="C15" s="7">
+        <f>'2018-Full'!G8</f>
         <v>394950</v>
       </c>
       <c r="D15" s="9">
@@ -17707,9 +17389,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="7">
+        <f>'2018-Full'!F9</f>
         <v>632742</v>
       </c>
       <c r="C16" s="7">
+        <f>'2018-Full'!G9</f>
         <v>372462</v>
       </c>
       <c r="D16" s="9">
@@ -17730,9 +17414,11 @@
         <v>9</v>
       </c>
       <c r="B17" s="7">
+        <f>'2018-Full'!F10</f>
         <v>7890888</v>
       </c>
       <c r="C17" s="7">
+        <f>'2018-Full'!G10</f>
         <v>984031</v>
       </c>
       <c r="D17" s="9">
@@ -17753,9 +17439,11 @@
         <v>10</v>
       </c>
       <c r="B18" s="7">
+        <f>'2018-Full'!F11</f>
         <v>6627327</v>
       </c>
       <c r="C18" s="7">
+        <f>'2018-Full'!G11</f>
         <v>7132438</v>
       </c>
       <c r="D18" s="9">
@@ -17776,9 +17464,11 @@
         <v>11</v>
       </c>
       <c r="B19" s="7">
+        <f>'2018-Full'!F12</f>
         <v>501285</v>
       </c>
       <c r="C19" s="7">
+        <f>'2018-Full'!G12</f>
         <v>77070</v>
       </c>
       <c r="D19" s="9">
@@ -17799,9 +17489,11 @@
         <v>12</v>
       </c>
       <c r="B20" s="7">
+        <f>'2018-Full'!F13</f>
         <v>10772431</v>
       </c>
       <c r="C20" s="7">
+        <f>'2018-Full'!G13</f>
         <v>6940825</v>
       </c>
       <c r="D20" s="9">
@@ -17822,9 +17514,11 @@
         <v>13</v>
       </c>
       <c r="B21" s="7">
+        <f>'2018-Full'!F14</f>
         <v>10454861</v>
       </c>
       <c r="C21" s="7">
+        <f>'2018-Full'!G14</f>
         <v>15200880</v>
       </c>
       <c r="D21" s="9">
@@ -17845,9 +17539,11 @@
         <v>14</v>
       </c>
       <c r="B22" s="7">
+        <f>'2018-Full'!F15</f>
         <v>16424426</v>
       </c>
       <c r="C22" s="7">
+        <f>'2018-Full'!G15</f>
         <v>15520789</v>
       </c>
       <c r="D22" s="9">
@@ -17868,9 +17564,11 @@
         <v>15</v>
       </c>
       <c r="B23" s="7">
+        <f>'2018-Full'!F16</f>
         <v>9358292</v>
       </c>
       <c r="C23" s="7">
+        <f>'2018-Full'!G16</f>
         <v>2300953</v>
       </c>
       <c r="D23" s="9">
@@ -17891,9 +17589,11 @@
         <v>16</v>
       </c>
       <c r="B24" s="7">
+        <f>'2018-Full'!F17</f>
         <v>6732462</v>
       </c>
       <c r="C24" s="7">
+        <f>'2018-Full'!G17</f>
         <v>12704150</v>
       </c>
       <c r="D24" s="9">
@@ -17914,9 +17614,11 @@
         <v>17</v>
       </c>
       <c r="B25" s="7">
+        <f>'2018-Full'!F18</f>
         <v>12059992</v>
       </c>
       <c r="C25" s="7">
+        <f>'2018-Full'!G18</f>
         <v>7727579</v>
       </c>
       <c r="D25" s="9">
@@ -17937,9 +17639,11 @@
         <v>18</v>
       </c>
       <c r="B26" s="7">
+        <f>'2018-Full'!F19</f>
         <v>7954155</v>
       </c>
       <c r="C26" s="7">
+        <f>'2018-Full'!G19</f>
         <v>2043839</v>
       </c>
       <c r="D26" s="9">
@@ -17960,9 +17664,11 @@
         <v>19</v>
       </c>
       <c r="B27" s="7">
+        <f>'2018-Full'!F20</f>
         <v>2009739</v>
       </c>
       <c r="C27" s="7">
+        <f>'2018-Full'!G20</f>
         <v>396357</v>
       </c>
       <c r="D27" s="9">
@@ -17983,9 +17689,11 @@
         <v>20</v>
       </c>
       <c r="B28" s="7">
+        <f>'2018-Full'!F21</f>
         <v>3394548</v>
       </c>
       <c r="C28" s="7">
+        <f>'2018-Full'!G21</f>
         <v>2974503</v>
       </c>
       <c r="D28" s="9">
@@ -18006,9 +17714,11 @@
         <v>21</v>
       </c>
       <c r="B29" s="7">
+        <f>'2018-Full'!F22</f>
         <v>4635181</v>
       </c>
       <c r="C29" s="7">
+        <f>'2018-Full'!G22</f>
         <v>3236598</v>
       </c>
       <c r="D29" s="9">
@@ -18029,9 +17739,11 @@
         <v>22</v>
       </c>
       <c r="B30" s="7">
+        <f>'2018-Full'!F23</f>
         <v>33009073</v>
       </c>
       <c r="C30" s="7">
+        <f>'2018-Full'!G23</f>
         <v>4045709</v>
       </c>
       <c r="D30" s="9">
@@ -18052,9 +17764,11 @@
         <v>23</v>
       </c>
       <c r="B31" s="7">
+        <f>'2018-Full'!F24</f>
         <v>27229500</v>
       </c>
       <c r="C31" s="7">
+        <f>'2018-Full'!G24</f>
         <v>3495674</v>
       </c>
       <c r="D31" s="9">
@@ -18075,9 +17789,11 @@
         <v>24</v>
       </c>
       <c r="B32" s="7">
+        <f>'2018-Full'!F25</f>
         <v>12585185</v>
       </c>
       <c r="C32" s="7">
+        <f>'2018-Full'!G25</f>
         <v>8708655</v>
       </c>
       <c r="D32" s="9">
@@ -18098,9 +17814,11 @@
         <v>25</v>
       </c>
       <c r="B33" s="7">
+        <f>'2018-Full'!F26</f>
         <v>4023594</v>
       </c>
       <c r="C33" s="7">
+        <f>'2018-Full'!G26</f>
         <v>8249067</v>
       </c>
       <c r="D33" s="9">
@@ -18121,9 +17839,11 @@
         <v>26</v>
       </c>
       <c r="B34" s="7">
+        <f>'2018-Full'!F27</f>
         <v>9459094</v>
       </c>
       <c r="C34" s="7">
+        <f>'2018-Full'!G27</f>
         <v>23458615</v>
       </c>
       <c r="D34" s="9">
@@ -18144,9 +17864,11 @@
         <v>27</v>
       </c>
       <c r="B35" s="7">
+        <f>'2018-Full'!F28</f>
         <v>8629779</v>
       </c>
       <c r="C35" s="7">
+        <f>'2018-Full'!G28</f>
         <v>2127935</v>
       </c>
       <c r="D35" s="9">
@@ -18167,9 +17889,11 @@
         <v>28</v>
       </c>
       <c r="B36" s="7">
+        <f>'2018-Full'!F29</f>
         <v>4257890</v>
       </c>
       <c r="C36" s="7">
+        <f>'2018-Full'!G29</f>
         <v>7553355</v>
       </c>
       <c r="D36" s="9">
@@ -18190,9 +17914,11 @@
         <v>29</v>
       </c>
       <c r="B37" s="7">
+        <f>'2018-Full'!F30</f>
         <v>7565754</v>
       </c>
       <c r="C37" s="7">
+        <f>'2018-Full'!G30</f>
         <v>5935707</v>
       </c>
       <c r="D37" s="9">
@@ -18213,9 +17939,11 @@
         <v>30</v>
       </c>
       <c r="B38" s="7">
+        <f>'2018-Full'!F31</f>
         <v>2646432</v>
       </c>
       <c r="C38" s="7">
+        <f>'2018-Full'!G31</f>
         <v>1370915</v>
       </c>
       <c r="D38" s="9">
@@ -18236,9 +17964,11 @@
         <v>31</v>
       </c>
       <c r="B39" s="7">
+        <f>'2018-Full'!F32</f>
         <v>6981229</v>
       </c>
       <c r="C39" s="7">
+        <f>'2018-Full'!G32</f>
         <v>1147736</v>
       </c>
       <c r="D39" s="9">
@@ -18259,9 +17989,11 @@
         <v>32</v>
       </c>
       <c r="B40" s="7">
+        <f>'2018-Full'!F33</f>
         <v>5866269</v>
       </c>
       <c r="C40" s="7">
+        <f>'2018-Full'!G33</f>
         <v>10319383</v>
       </c>
       <c r="D40" s="9">
@@ -18282,9 +18014,11 @@
         <v>33</v>
       </c>
       <c r="B41" s="7">
+        <f>'2018-Full'!F34</f>
         <v>3920404</v>
       </c>
       <c r="C41" s="7">
+        <f>'2018-Full'!G34</f>
         <v>3829980</v>
       </c>
       <c r="D41" s="9">
@@ -18305,9 +18039,11 @@
         <v>34</v>
       </c>
       <c r="B42" s="7">
+        <f>'2018-Full'!F35</f>
         <v>17441081</v>
       </c>
       <c r="C42" s="7">
+        <f>'2018-Full'!G35</f>
         <v>4177215</v>
       </c>
       <c r="D42" s="9">
@@ -18328,9 +18064,11 @@
         <v>35</v>
       </c>
       <c r="B43" s="7">
+        <f>'2018-Full'!F36</f>
         <v>16259079</v>
       </c>
       <c r="C43" s="7">
+        <f>'2018-Full'!G36</f>
         <v>6378876</v>
       </c>
       <c r="D43" s="9">
@@ -18351,9 +18089,11 @@
         <v>36</v>
       </c>
       <c r="B44" s="7">
+        <f>'2018-Full'!F37</f>
         <v>5735625</v>
       </c>
       <c r="C44" s="7">
+        <f>'2018-Full'!G37</f>
         <v>3870723</v>
       </c>
       <c r="D44" s="9">
@@ -18374,9 +18114,11 @@
         <v>37</v>
       </c>
       <c r="B45" s="7">
+        <f>'2018-Full'!F38</f>
         <v>20982703</v>
       </c>
       <c r="C45" s="7">
+        <f>'2018-Full'!G38</f>
         <v>5416770</v>
       </c>
       <c r="D45" s="9">
@@ -18397,9 +18139,11 @@
         <v>38</v>
       </c>
       <c r="B46" s="7">
+        <f>'2018-Full'!F39</f>
         <v>30352406</v>
       </c>
       <c r="C46" s="7">
+        <f>'2018-Full'!G39</f>
         <v>6079410</v>
       </c>
       <c r="D46" s="9">
@@ -18420,9 +18164,11 @@
         <v>39</v>
       </c>
       <c r="B47" s="7">
+        <f>'2018-Full'!F40</f>
         <v>362093</v>
       </c>
       <c r="C47" s="7">
+        <f>'2018-Full'!G40</f>
         <v>121483</v>
       </c>
       <c r="D47" s="9">
@@ -18443,9 +18189,11 @@
         <v>40</v>
       </c>
       <c r="B48" s="7">
+        <f>'2018-Full'!F41</f>
         <v>5434146</v>
       </c>
       <c r="C48" s="7">
+        <f>'2018-Full'!G41</f>
         <v>4283172</v>
       </c>
       <c r="D48" s="9">
@@ -18466,9 +18214,11 @@
         <v>41</v>
       </c>
       <c r="B49" s="7">
+        <f>'2018-Full'!F42</f>
         <v>7186745</v>
       </c>
       <c r="C49" s="7">
+        <f>'2018-Full'!G42</f>
         <v>14874974</v>
       </c>
       <c r="D49" s="9">
@@ -18489,9 +18239,11 @@
         <v>42</v>
       </c>
       <c r="B50" s="7">
+        <f>'2018-Full'!F43</f>
         <v>17016820</v>
       </c>
       <c r="C50" s="7">
+        <f>'2018-Full'!G43</f>
         <v>3703363</v>
       </c>
       <c r="D50" s="9">
@@ -18512,9 +18264,11 @@
         <v>43</v>
       </c>
       <c r="B51" s="7">
+        <f>'2018-Full'!F44</f>
         <v>35200343</v>
       </c>
       <c r="C51" s="7">
+        <f>'2018-Full'!G44</f>
         <v>11017420</v>
       </c>
       <c r="D51" s="9">
@@ -18535,9 +18289,11 @@
         <v>44</v>
       </c>
       <c r="B52" s="7">
+        <f>'2018-Full'!F45</f>
         <v>11216469</v>
       </c>
       <c r="C52" s="7">
+        <f>'2018-Full'!G45</f>
         <v>5545567</v>
       </c>
       <c r="D52" s="9">
@@ -18558,9 +18314,11 @@
         <v>45</v>
       </c>
       <c r="B53" s="7">
+        <f>'2018-Full'!F46</f>
         <v>17488685</v>
       </c>
       <c r="C53" s="7">
+        <f>'2018-Full'!G46</f>
         <v>3815542</v>
       </c>
       <c r="D53" s="9">
@@ -18581,9 +18339,11 @@
         <v>46</v>
       </c>
       <c r="B54" s="7">
+        <f>'2018-Full'!F47</f>
         <v>2975620</v>
       </c>
       <c r="C54" s="7">
+        <f>'2018-Full'!G47</f>
         <v>989935</v>
       </c>
       <c r="D54" s="9">
@@ -18604,9 +18364,11 @@
         <v>47</v>
       </c>
       <c r="B55" s="7">
+        <f>'2018-Full'!F48</f>
         <v>16129772</v>
       </c>
       <c r="C55" s="7">
+        <f>'2018-Full'!G48</f>
         <v>1062087</v>
       </c>
       <c r="D55" s="9">
@@ -18627,9 +18389,11 @@
         <v>48</v>
       </c>
       <c r="B56" s="7">
+        <f>'2018-Full'!F49</f>
         <v>33771619</v>
       </c>
       <c r="C56" s="7">
+        <f>'2018-Full'!G49</f>
         <v>7609753</v>
       </c>
       <c r="D56" s="9">
@@ -18650,9 +18414,11 @@
         <v>49</v>
       </c>
       <c r="B57" s="7">
+        <f>'2018-Full'!F50</f>
         <v>4354126</v>
       </c>
       <c r="C57" s="7">
+        <f>'2018-Full'!G50</f>
         <v>4868774</v>
       </c>
       <c r="D57" s="9">
@@ -18673,9 +18439,11 @@
         <v>50</v>
       </c>
       <c r="B58" s="7">
+        <f>'2018-Full'!F51</f>
         <v>6484947</v>
       </c>
       <c r="C58" s="7">
+        <f>'2018-Full'!G51</f>
         <v>18388025</v>
       </c>
       <c r="D58" s="9">
@@ -22191,7 +21959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -22223,18 +21991,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
+        <f>'2018-Full'!B2</f>
         <v>108921</v>
       </c>
       <c r="C2" s="6">
+        <f>'2018-Full'!C2</f>
         <v>278248</v>
       </c>
       <c r="D2" s="6">
+        <f>'2018-Full'!D2</f>
         <v>74532</v>
       </c>
       <c r="E2" s="6">
+        <f>'2018-Full'!E2</f>
         <v>352780</v>
       </c>
       <c r="F2" s="7">
+        <f>'2018-Full'!H2</f>
         <v>8491593</v>
       </c>
       <c r="G2" s="11"/>
@@ -22245,18 +22018,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
+        <f>'2018-Full'!B3</f>
         <v>547905</v>
       </c>
       <c r="C3" s="6">
+        <f>'2018-Full'!C3</f>
         <v>542838</v>
       </c>
       <c r="D3" s="6">
+        <f>'2018-Full'!D3</f>
         <v>37106</v>
       </c>
       <c r="E3" s="6">
+        <f>'2018-Full'!E3</f>
         <v>579944</v>
       </c>
       <c r="F3" s="7">
+        <f>'2018-Full'!H3</f>
         <v>11801451</v>
       </c>
       <c r="G3" s="11"/>
@@ -22267,18 +22045,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="6">
+        <f>'2018-Full'!B4</f>
         <v>326559</v>
       </c>
       <c r="C4" s="6">
+        <f>'2018-Full'!C4</f>
         <v>380102</v>
       </c>
       <c r="D4" s="6">
+        <f>'2018-Full'!D4</f>
         <v>136944</v>
       </c>
       <c r="E4" s="6">
+        <f>'2018-Full'!E4</f>
         <v>517046</v>
       </c>
       <c r="F4" s="7">
+        <f>'2018-Full'!H4</f>
         <v>18765517</v>
       </c>
       <c r="G4" s="11"/>
@@ -22289,18 +22072,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="6">
+        <f>'2018-Full'!B5</f>
         <v>305214</v>
       </c>
       <c r="C5" s="6">
+        <f>'2018-Full'!C5</f>
         <v>456140</v>
       </c>
       <c r="D5" s="6">
+        <f>'2018-Full'!D5</f>
         <v>61607</v>
       </c>
       <c r="E5" s="6">
+        <f>'2018-Full'!E5</f>
         <v>517747</v>
       </c>
       <c r="F5" s="7">
+        <f>'2018-Full'!H5</f>
         <v>17874083</v>
       </c>
     </row>
@@ -22309,18 +22097,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
+        <f>'2018-Full'!B6</f>
         <v>280967</v>
       </c>
       <c r="C6" s="6">
+        <f>'2018-Full'!C6</f>
         <v>1007422</v>
       </c>
       <c r="D6" s="6">
+        <f>'2018-Full'!D6</f>
         <v>22738</v>
       </c>
       <c r="E6" s="6">
+        <f>'2018-Full'!E6</f>
         <v>1030160</v>
       </c>
       <c r="F6" s="7">
+        <f>'2018-Full'!H6</f>
         <v>21615994</v>
       </c>
     </row>
@@ -22329,18 +22122,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
+        <f>'2018-Full'!B7</f>
         <v>294319</v>
       </c>
       <c r="C7" s="6">
+        <f>'2018-Full'!C7</f>
         <v>459518</v>
       </c>
       <c r="D7" s="6">
+        <f>'2018-Full'!D7</f>
         <v>109246</v>
       </c>
       <c r="E7" s="6">
+        <f>'2018-Full'!E7</f>
         <v>568764</v>
       </c>
       <c r="F7" s="7">
+        <f>'2018-Full'!H7</f>
         <v>57056595</v>
       </c>
     </row>
@@ -22349,18 +22147,23 @@
         <v>7</v>
       </c>
       <c r="B8" s="6">
+        <f>'2018-Full'!B8</f>
         <v>37489</v>
       </c>
       <c r="C8" s="6">
+        <f>'2018-Full'!C8</f>
         <v>124169</v>
       </c>
       <c r="D8" s="6">
+        <f>'2018-Full'!D8</f>
         <v>4063</v>
       </c>
       <c r="E8" s="6">
+        <f>'2018-Full'!E8</f>
         <v>128232</v>
       </c>
       <c r="F8" s="7">
+        <f>'2018-Full'!H8</f>
         <v>2480317</v>
       </c>
     </row>
@@ -22369,18 +22172,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="6">
+        <f>'2018-Full'!B9</f>
         <v>17847</v>
       </c>
       <c r="C9" s="6">
+        <f>'2018-Full'!C9</f>
         <v>52315</v>
       </c>
       <c r="D9" s="6">
+        <f>'2018-Full'!D9</f>
         <v>7125</v>
       </c>
       <c r="E9" s="6">
+        <f>'2018-Full'!E9</f>
         <v>59440</v>
       </c>
       <c r="F9" s="7">
+        <f>'2018-Full'!H9</f>
         <v>1005204</v>
       </c>
     </row>
@@ -22389,18 +22197,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="6">
+        <f>'2018-Full'!B10</f>
         <v>190232</v>
       </c>
       <c r="C10" s="6">
+        <f>'2018-Full'!C10</f>
         <v>313554</v>
       </c>
       <c r="D10" s="6">
+        <f>'2018-Full'!D10</f>
         <v>18155</v>
       </c>
       <c r="E10" s="6">
+        <f>'2018-Full'!E10</f>
         <v>331709</v>
       </c>
       <c r="F10" s="7">
+        <f>'2018-Full'!H10</f>
         <v>8874919</v>
       </c>
     </row>
@@ -22409,18 +22222,23 @@
         <v>10</v>
       </c>
       <c r="B11" s="6">
+        <f>'2018-Full'!B11</f>
         <v>651910</v>
       </c>
       <c r="C11" s="6">
+        <f>'2018-Full'!C11</f>
         <v>1297350</v>
       </c>
       <c r="D11" s="6">
+        <f>'2018-Full'!D11</f>
         <v>166091</v>
       </c>
       <c r="E11" s="6">
+        <f>'2018-Full'!E11</f>
         <v>1463441</v>
       </c>
       <c r="F11" s="7">
+        <f>'2018-Full'!H11</f>
         <v>13759765</v>
       </c>
     </row>
@@ -22429,18 +22247,23 @@
         <v>11</v>
       </c>
       <c r="B12" s="6">
+        <f>'2018-Full'!B12</f>
         <v>10617</v>
       </c>
       <c r="C12" s="6">
+        <f>'2018-Full'!C12</f>
         <v>11068</v>
       </c>
       <c r="D12" s="1">
+        <f>'2018-Full'!D12</f>
         <v>734</v>
       </c>
       <c r="E12" s="6">
+        <f>'2018-Full'!E12</f>
         <v>11802</v>
       </c>
       <c r="F12" s="7">
+        <f>'2018-Full'!H12</f>
         <v>578355</v>
       </c>
     </row>
@@ -22449,18 +22272,23 @@
         <v>12</v>
       </c>
       <c r="B13" s="6">
+        <f>'2018-Full'!B13</f>
         <v>223232</v>
       </c>
       <c r="C13" s="6">
+        <f>'2018-Full'!C13</f>
         <v>516446</v>
       </c>
       <c r="D13" s="6">
+        <f>'2018-Full'!D13</f>
         <v>67438</v>
       </c>
       <c r="E13" s="6">
+        <f>'2018-Full'!E13</f>
         <v>583884</v>
       </c>
       <c r="F13" s="7">
+        <f>'2018-Full'!H13</f>
         <v>17713256</v>
       </c>
     </row>
@@ -22469,18 +22297,23 @@
         <v>13</v>
       </c>
       <c r="B14" s="6">
+        <f>'2018-Full'!B14</f>
         <v>286947</v>
       </c>
       <c r="C14" s="6">
+        <f>'2018-Full'!C14</f>
         <v>1047773</v>
       </c>
       <c r="D14" s="6">
+        <f>'2018-Full'!D14</f>
         <v>159224</v>
       </c>
       <c r="E14" s="6">
+        <f>'2018-Full'!E14</f>
         <v>1206997</v>
       </c>
       <c r="F14" s="7">
+        <f>'2018-Full'!H14</f>
         <v>25655741</v>
       </c>
     </row>
@@ -22489,18 +22322,23 @@
         <v>14</v>
       </c>
       <c r="B15" s="6">
+        <f>'2018-Full'!B15</f>
         <v>306024</v>
       </c>
       <c r="C15" s="6">
+        <f>'2018-Full'!C15</f>
         <v>1203507</v>
       </c>
       <c r="D15" s="6">
+        <f>'2018-Full'!D15</f>
         <v>83025</v>
       </c>
       <c r="E15" s="6">
+        <f>'2018-Full'!E15</f>
         <v>1286532</v>
       </c>
       <c r="F15" s="7">
+        <f>'2018-Full'!H15</f>
         <v>31945215</v>
       </c>
     </row>
@@ -22509,18 +22347,23 @@
         <v>15</v>
       </c>
       <c r="B16" s="6">
+        <f>'2018-Full'!B16</f>
         <v>267447</v>
       </c>
       <c r="C16" s="6">
+        <f>'2018-Full'!C16</f>
         <v>383958</v>
       </c>
       <c r="D16" s="6">
+        <f>'2018-Full'!D16</f>
         <v>20781</v>
       </c>
       <c r="E16" s="6">
+        <f>'2018-Full'!E16</f>
         <v>404739</v>
       </c>
       <c r="F16" s="7">
+        <f>'2018-Full'!H16</f>
         <v>11659245</v>
       </c>
     </row>
@@ -22529,18 +22372,23 @@
         <v>16</v>
       </c>
       <c r="B17" s="6">
+        <f>'2018-Full'!B17</f>
         <v>251390</v>
       </c>
       <c r="C17" s="6">
+        <f>'2018-Full'!C17</f>
         <v>349199</v>
       </c>
       <c r="D17" s="6">
+        <f>'2018-Full'!D17</f>
         <v>170676</v>
       </c>
       <c r="E17" s="6">
+        <f>'2018-Full'!E17</f>
         <v>519875</v>
       </c>
       <c r="F17" s="7">
+        <f>'2018-Full'!H17</f>
         <v>19436612</v>
       </c>
     </row>
@@ -22549,18 +22397,23 @@
         <v>17</v>
       </c>
       <c r="B18" s="6">
+        <f>'2018-Full'!B18</f>
         <v>352408</v>
       </c>
       <c r="C18" s="6">
+        <f>'2018-Full'!C18</f>
         <v>512113</v>
       </c>
       <c r="D18" s="6">
+        <f>'2018-Full'!D18</f>
         <v>102629</v>
       </c>
       <c r="E18" s="6">
+        <f>'2018-Full'!E18</f>
         <v>614742</v>
       </c>
       <c r="F18" s="7">
+        <f>'2018-Full'!H18</f>
         <v>19787571</v>
       </c>
     </row>
@@ -22569,18 +22422,23 @@
         <v>18</v>
       </c>
       <c r="B19" s="6">
+        <f>'2018-Full'!B19</f>
         <v>398808</v>
       </c>
       <c r="C19" s="6">
+        <f>'2018-Full'!C19</f>
         <v>605336</v>
       </c>
       <c r="D19" s="6">
+        <f>'2018-Full'!D19</f>
         <v>53323</v>
       </c>
       <c r="E19" s="6">
+        <f>'2018-Full'!E19</f>
         <v>658659</v>
       </c>
       <c r="F19" s="7">
+        <f>'2018-Full'!H19</f>
         <v>9997994</v>
       </c>
     </row>
@@ -22589,18 +22447,23 @@
         <v>19</v>
       </c>
       <c r="B20" s="6">
+        <f>'2018-Full'!B20</f>
         <v>57921</v>
       </c>
       <c r="C20" s="6">
+        <f>'2018-Full'!C20</f>
         <v>246052</v>
       </c>
       <c r="D20" s="6">
+        <f>'2018-Full'!D20</f>
         <v>15504</v>
       </c>
       <c r="E20" s="6">
+        <f>'2018-Full'!E20</f>
         <v>261556</v>
       </c>
       <c r="F20" s="7">
+        <f>'2018-Full'!H20</f>
         <v>2406096</v>
       </c>
     </row>
@@ -22609,18 +22472,23 @@
         <v>20</v>
       </c>
       <c r="B21" s="6">
+        <f>'2018-Full'!B21</f>
         <v>120334</v>
       </c>
       <c r="C21" s="6">
+        <f>'2018-Full'!C21</f>
         <v>284941</v>
       </c>
       <c r="D21" s="6">
+        <f>'2018-Full'!D21</f>
         <v>60270</v>
       </c>
       <c r="E21" s="6">
+        <f>'2018-Full'!E21</f>
         <v>345211</v>
       </c>
       <c r="F21" s="7">
+        <f>'2018-Full'!H21</f>
         <v>6369051</v>
       </c>
     </row>
@@ -22629,18 +22497,23 @@
         <v>21</v>
       </c>
       <c r="B22" s="6">
+        <f>'2018-Full'!B22</f>
         <v>163191</v>
       </c>
       <c r="C22" s="6">
+        <f>'2018-Full'!C22</f>
         <v>214767</v>
       </c>
       <c r="D22" s="6">
+        <f>'2018-Full'!D22</f>
         <v>34323</v>
       </c>
       <c r="E22" s="6">
+        <f>'2018-Full'!E22</f>
         <v>249090</v>
       </c>
       <c r="F22" s="7">
+        <f>'2018-Full'!H22</f>
         <v>7871779</v>
       </c>
     </row>
@@ -22649,18 +22522,23 @@
         <v>22</v>
       </c>
       <c r="B23" s="6">
+        <f>'2018-Full'!B23</f>
         <v>706101</v>
       </c>
       <c r="C23" s="6">
+        <f>'2018-Full'!C23</f>
         <v>2171384</v>
       </c>
       <c r="D23" s="6">
+        <f>'2018-Full'!D23</f>
         <v>52786</v>
       </c>
       <c r="E23" s="6">
+        <f>'2018-Full'!E23</f>
         <v>2224170</v>
       </c>
       <c r="F23" s="7">
+        <f>'2018-Full'!H23</f>
         <v>37054782</v>
       </c>
     </row>
@@ -22669,18 +22547,23 @@
         <v>23</v>
       </c>
       <c r="B24" s="6">
+        <f>'2018-Full'!B24</f>
         <v>568057</v>
       </c>
       <c r="C24" s="6">
+        <f>'2018-Full'!C24</f>
         <v>1376759</v>
       </c>
       <c r="D24" s="6">
+        <f>'2018-Full'!D24</f>
         <v>44245</v>
       </c>
       <c r="E24" s="6">
+        <f>'2018-Full'!E24</f>
         <v>1421004</v>
       </c>
       <c r="F24" s="7">
+        <f>'2018-Full'!H24</f>
         <v>30725174</v>
       </c>
     </row>
@@ -22689,18 +22572,23 @@
         <v>24</v>
       </c>
       <c r="B25" s="6">
+        <f>'2018-Full'!B25</f>
         <v>498319</v>
       </c>
       <c r="C25" s="6">
+        <f>'2018-Full'!C25</f>
         <v>1702400</v>
       </c>
       <c r="D25" s="6">
+        <f>'2018-Full'!D25</f>
         <v>79919</v>
       </c>
       <c r="E25" s="6">
+        <f>'2018-Full'!E25</f>
         <v>1782319</v>
       </c>
       <c r="F25" s="7">
+        <f>'2018-Full'!H25</f>
         <v>21293840</v>
       </c>
     </row>
@@ -22709,18 +22597,23 @@
         <v>25</v>
       </c>
       <c r="B26" s="6">
+        <f>'2018-Full'!B26</f>
         <v>300146</v>
       </c>
       <c r="C26" s="6">
+        <f>'2018-Full'!C26</f>
         <v>335324</v>
       </c>
       <c r="D26" s="6">
+        <f>'2018-Full'!D26</f>
         <v>91402</v>
       </c>
       <c r="E26" s="6">
+        <f>'2018-Full'!E26</f>
         <v>426726</v>
       </c>
       <c r="F26" s="7">
+        <f>'2018-Full'!H26</f>
         <v>12272661</v>
       </c>
     </row>
@@ -22729,18 +22622,23 @@
         <v>26</v>
       </c>
       <c r="B27" s="6">
+        <f>'2018-Full'!B27</f>
         <v>253412</v>
       </c>
       <c r="C27" s="6">
+        <f>'2018-Full'!C27</f>
         <v>873323</v>
       </c>
       <c r="D27" s="6">
+        <f>'2018-Full'!D27</f>
         <v>155658</v>
       </c>
       <c r="E27" s="6">
+        <f>'2018-Full'!E27</f>
         <v>1028981</v>
       </c>
       <c r="F27" s="7">
+        <f>'2018-Full'!H27</f>
         <v>32917709</v>
       </c>
     </row>
@@ -22749,18 +22647,23 @@
         <v>27</v>
       </c>
       <c r="B28" s="6">
+        <f>'2018-Full'!B28</f>
         <v>585766</v>
       </c>
       <c r="C28" s="6">
+        <f>'2018-Full'!C28</f>
         <v>319136</v>
       </c>
       <c r="D28" s="6">
+        <f>'2018-Full'!D28</f>
         <v>25626</v>
       </c>
       <c r="E28" s="6">
+        <f>'2018-Full'!E28</f>
         <v>344762</v>
       </c>
       <c r="F28" s="7">
+        <f>'2018-Full'!H28</f>
         <v>10757714</v>
       </c>
     </row>
@@ -22769,18 +22672,23 @@
         <v>28</v>
       </c>
       <c r="B29" s="6">
+        <f>'2018-Full'!B29</f>
         <v>141553</v>
       </c>
       <c r="C29" s="6">
+        <f>'2018-Full'!C29</f>
         <v>362554</v>
       </c>
       <c r="D29" s="6">
+        <f>'2018-Full'!D29</f>
         <v>157801</v>
       </c>
       <c r="E29" s="6">
+        <f>'2018-Full'!E29</f>
         <v>520355</v>
       </c>
       <c r="F29" s="7">
+        <f>'2018-Full'!H29</f>
         <v>11811245</v>
       </c>
     </row>
@@ -22789,18 +22697,23 @@
         <v>29</v>
       </c>
       <c r="B30" s="6">
+        <f>'2018-Full'!B30</f>
         <v>183056</v>
       </c>
       <c r="C30" s="6">
+        <f>'2018-Full'!C30</f>
         <v>339053</v>
       </c>
       <c r="D30" s="6">
+        <f>'2018-Full'!D30</f>
         <v>90202</v>
       </c>
       <c r="E30" s="6">
+        <f>'2018-Full'!E30</f>
         <v>429255</v>
       </c>
       <c r="F30" s="7">
+        <f>'2018-Full'!H30</f>
         <v>13501461</v>
       </c>
     </row>
@@ -22809,18 +22722,23 @@
         <v>30</v>
       </c>
       <c r="B31" s="6">
+        <f>'2018-Full'!B31</f>
         <v>58099</v>
       </c>
       <c r="C31" s="6">
+        <f>'2018-Full'!C31</f>
         <v>186931</v>
       </c>
       <c r="D31" s="6">
+        <f>'2018-Full'!D31</f>
         <v>31411</v>
       </c>
       <c r="E31" s="6">
+        <f>'2018-Full'!E31</f>
         <v>218342</v>
       </c>
       <c r="F31" s="7">
+        <f>'2018-Full'!H31</f>
         <v>4017347</v>
       </c>
     </row>
@@ -22829,18 +22747,23 @@
         <v>31</v>
       </c>
       <c r="B32" s="6">
+        <f>'2018-Full'!B32</f>
         <v>74794</v>
       </c>
       <c r="C32" s="6">
+        <f>'2018-Full'!C32</f>
         <v>303795</v>
       </c>
       <c r="D32" s="6">
+        <f>'2018-Full'!D32</f>
         <v>118442</v>
       </c>
       <c r="E32" s="6">
+        <f>'2018-Full'!E32</f>
         <v>422237</v>
       </c>
       <c r="F32" s="7">
+        <f>'2018-Full'!H32</f>
         <v>8128965</v>
       </c>
     </row>
@@ -22849,18 +22772,23 @@
         <v>32</v>
       </c>
       <c r="B33" s="6">
+        <f>'2018-Full'!B33</f>
         <v>107331</v>
       </c>
       <c r="C33" s="6">
+        <f>'2018-Full'!C33</f>
         <v>329423</v>
       </c>
       <c r="D33" s="6">
+        <f>'2018-Full'!D33</f>
         <v>112483</v>
       </c>
       <c r="E33" s="6">
+        <f>'2018-Full'!E33</f>
         <v>441906</v>
       </c>
       <c r="F33" s="7">
+        <f>'2018-Full'!H33</f>
         <v>16185652</v>
       </c>
     </row>
@@ -22869,18 +22797,23 @@
         <v>33</v>
       </c>
       <c r="B34" s="6">
+        <f>'2018-Full'!B34</f>
         <v>68744</v>
       </c>
       <c r="C34" s="6">
+        <f>'2018-Full'!C34</f>
         <v>123271</v>
       </c>
       <c r="D34" s="6">
+        <f>'2018-Full'!D34</f>
         <v>26840</v>
       </c>
       <c r="E34" s="6">
+        <f>'2018-Full'!E34</f>
         <v>150111</v>
       </c>
       <c r="F34" s="7">
+        <f>'2018-Full'!H34</f>
         <v>7750384</v>
       </c>
     </row>
@@ -22889,18 +22822,23 @@
         <v>34</v>
       </c>
       <c r="B35" s="6">
+        <f>'2018-Full'!B35</f>
         <v>579043</v>
       </c>
       <c r="C35" s="6">
+        <f>'2018-Full'!C35</f>
         <v>1117576</v>
       </c>
       <c r="D35" s="6">
+        <f>'2018-Full'!D35</f>
         <v>48773</v>
       </c>
       <c r="E35" s="6">
+        <f>'2018-Full'!E35</f>
         <v>1166349</v>
       </c>
       <c r="F35" s="7">
+        <f>'2018-Full'!H35</f>
         <v>21618296</v>
       </c>
     </row>
@@ -22909,18 +22847,23 @@
         <v>35</v>
       </c>
       <c r="B36" s="6">
+        <f>'2018-Full'!B36</f>
         <v>390268</v>
       </c>
       <c r="C36" s="6">
+        <f>'2018-Full'!C36</f>
         <v>895099</v>
       </c>
       <c r="D36" s="6">
+        <f>'2018-Full'!D36</f>
         <v>100065</v>
       </c>
       <c r="E36" s="6">
+        <f>'2018-Full'!E36</f>
         <v>995164</v>
       </c>
       <c r="F36" s="7">
+        <f>'2018-Full'!H36</f>
         <v>22637955</v>
       </c>
     </row>
@@ -22929,18 +22872,23 @@
         <v>36</v>
       </c>
       <c r="B37" s="6">
+        <f>'2018-Full'!B37</f>
         <v>529651</v>
       </c>
       <c r="C37" s="6">
+        <f>'2018-Full'!C37</f>
         <v>377498</v>
       </c>
       <c r="D37" s="6">
+        <f>'2018-Full'!D37</f>
         <v>22740</v>
       </c>
       <c r="E37" s="6">
+        <f>'2018-Full'!E37</f>
         <v>400238</v>
       </c>
       <c r="F37" s="7">
+        <f>'2018-Full'!H37</f>
         <v>9606348</v>
       </c>
     </row>
@@ -22949,18 +22897,23 @@
         <v>37</v>
       </c>
       <c r="B38" s="6">
+        <f>'2018-Full'!B38</f>
         <v>264684</v>
       </c>
       <c r="C38" s="6">
+        <f>'2018-Full'!C38</f>
         <v>1173427</v>
       </c>
       <c r="D38" s="6">
+        <f>'2018-Full'!D38</f>
         <v>49243</v>
       </c>
       <c r="E38" s="6">
+        <f>'2018-Full'!E38</f>
         <v>1222670</v>
       </c>
       <c r="F38" s="7">
+        <f>'2018-Full'!H38</f>
         <v>26399473</v>
       </c>
     </row>
@@ -22969,18 +22922,23 @@
         <v>38</v>
       </c>
       <c r="B39" s="6">
+        <f>'2018-Full'!B39</f>
         <v>975650</v>
       </c>
       <c r="C39" s="6">
+        <f>'2018-Full'!C39</f>
         <v>2468652</v>
       </c>
       <c r="D39" s="6">
+        <f>'2018-Full'!D39</f>
         <v>101278</v>
       </c>
       <c r="E39" s="6">
+        <f>'2018-Full'!E39</f>
         <v>2569930</v>
       </c>
       <c r="F39" s="7">
+        <f>'2018-Full'!H39</f>
         <v>36431816</v>
       </c>
     </row>
@@ -22989,18 +22947,23 @@
         <v>39</v>
       </c>
       <c r="B40" s="6">
+        <f>'2018-Full'!B40</f>
         <v>8209</v>
       </c>
       <c r="C40" s="6">
+        <f>'2018-Full'!C40</f>
         <v>26515</v>
       </c>
       <c r="D40" s="6">
+        <f>'2018-Full'!D40</f>
         <v>4388</v>
       </c>
       <c r="E40" s="6">
+        <f>'2018-Full'!E40</f>
         <v>30903</v>
       </c>
       <c r="F40" s="7">
+        <f>'2018-Full'!H40</f>
         <v>483576</v>
       </c>
     </row>
@@ -23009,18 +22972,23 @@
         <v>40</v>
       </c>
       <c r="B41" s="6">
+        <f>'2018-Full'!B41</f>
         <v>210369</v>
       </c>
       <c r="C41" s="6">
+        <f>'2018-Full'!C41</f>
         <v>722055</v>
       </c>
       <c r="D41" s="6">
+        <f>'2018-Full'!D41</f>
         <v>92230</v>
       </c>
       <c r="E41" s="6">
+        <f>'2018-Full'!E41</f>
         <v>814285</v>
       </c>
       <c r="F41" s="7">
+        <f>'2018-Full'!H41</f>
         <v>9717318</v>
       </c>
     </row>
@@ -23029,18 +22997,23 @@
         <v>41</v>
       </c>
       <c r="B42" s="6">
+        <f>'2018-Full'!B42</f>
         <v>233215</v>
       </c>
       <c r="C42" s="6">
+        <f>'2018-Full'!C42</f>
         <v>245474</v>
       </c>
       <c r="D42" s="6">
+        <f>'2018-Full'!D42</f>
         <v>128502</v>
       </c>
       <c r="E42" s="6">
+        <f>'2018-Full'!E42</f>
         <v>373976</v>
       </c>
       <c r="F42" s="7">
+        <f>'2018-Full'!H42</f>
         <v>22061719</v>
       </c>
     </row>
@@ -23049,18 +23022,23 @@
         <v>42</v>
       </c>
       <c r="B43" s="6">
+        <f>'2018-Full'!B43</f>
         <v>700600</v>
       </c>
       <c r="C43" s="6">
+        <f>'2018-Full'!C43</f>
         <v>696906</v>
       </c>
       <c r="D43" s="6">
+        <f>'2018-Full'!D43</f>
         <v>40267</v>
       </c>
       <c r="E43" s="6">
+        <f>'2018-Full'!E43</f>
         <v>737173</v>
       </c>
       <c r="F43" s="7">
+        <f>'2018-Full'!H43</f>
         <v>20720183</v>
       </c>
     </row>
@@ -23069,18 +23047,23 @@
         <v>43</v>
       </c>
       <c r="B44" s="6">
+        <f>'2018-Full'!B44</f>
         <v>1157779</v>
       </c>
       <c r="C44" s="6">
+        <f>'2018-Full'!C44</f>
         <v>1575985</v>
       </c>
       <c r="D44" s="6">
+        <f>'2018-Full'!D44</f>
         <v>79358</v>
       </c>
       <c r="E44" s="6">
+        <f>'2018-Full'!E44</f>
         <v>1655343</v>
       </c>
       <c r="F44" s="7">
+        <f>'2018-Full'!H44</f>
         <v>46217763</v>
       </c>
     </row>
@@ -23089,18 +23072,23 @@
         <v>44</v>
       </c>
       <c r="B45" s="6">
+        <f>'2018-Full'!B45</f>
         <v>236656</v>
       </c>
       <c r="C45" s="6">
+        <f>'2018-Full'!C45</f>
         <v>379805</v>
       </c>
       <c r="D45" s="6">
+        <f>'2018-Full'!D45</f>
         <v>41036</v>
       </c>
       <c r="E45" s="6">
+        <f>'2018-Full'!E45</f>
         <v>420841</v>
       </c>
       <c r="F45" s="7">
+        <f>'2018-Full'!H45</f>
         <v>16762036</v>
       </c>
     </row>
@@ -23109,18 +23097,23 @@
         <v>45</v>
       </c>
       <c r="B46" s="6">
+        <f>'2018-Full'!B46</f>
         <v>276019</v>
       </c>
       <c r="C46" s="6">
+        <f>'2018-Full'!C46</f>
         <v>815464</v>
       </c>
       <c r="D46" s="6">
+        <f>'2018-Full'!D46</f>
         <v>44611</v>
       </c>
       <c r="E46" s="6">
+        <f>'2018-Full'!E46</f>
         <v>860075</v>
       </c>
       <c r="F46" s="7">
+        <f>'2018-Full'!H46</f>
         <v>21304227</v>
       </c>
     </row>
@@ -23129,18 +23122,23 @@
         <v>46</v>
       </c>
       <c r="B47" s="6">
+        <f>'2018-Full'!B47</f>
         <v>69943</v>
       </c>
       <c r="C47" s="6">
+        <f>'2018-Full'!C47</f>
         <v>153476</v>
       </c>
       <c r="D47" s="6">
+        <f>'2018-Full'!D47</f>
         <v>15852</v>
       </c>
       <c r="E47" s="6">
+        <f>'2018-Full'!E47</f>
         <v>169328</v>
       </c>
       <c r="F47" s="7">
+        <f>'2018-Full'!H47</f>
         <v>3965555</v>
       </c>
     </row>
@@ -23149,18 +23147,23 @@
         <v>47</v>
       </c>
       <c r="B48" s="6">
+        <f>'2018-Full'!B48</f>
         <v>183063</v>
       </c>
       <c r="C48" s="6">
+        <f>'2018-Full'!C48</f>
         <v>681049</v>
       </c>
       <c r="D48" s="6">
+        <f>'2018-Full'!D48</f>
         <v>10683</v>
       </c>
       <c r="E48" s="6">
+        <f>'2018-Full'!E48</f>
         <v>691732</v>
       </c>
       <c r="F48" s="7">
+        <f>'2018-Full'!H48</f>
         <v>17191859</v>
       </c>
     </row>
@@ -23169,18 +23172,23 @@
         <v>48</v>
       </c>
       <c r="B49" s="6">
+        <f>'2018-Full'!B49</f>
         <v>706400</v>
       </c>
       <c r="C49" s="6">
+        <f>'2018-Full'!C49</f>
         <v>2716899</v>
       </c>
       <c r="D49" s="6">
+        <f>'2018-Full'!D49</f>
         <v>146777</v>
       </c>
       <c r="E49" s="6">
+        <f>'2018-Full'!E49</f>
         <v>2863676</v>
       </c>
       <c r="F49" s="7">
+        <f>'2018-Full'!H49</f>
         <v>41381372</v>
       </c>
     </row>
@@ -23189,18 +23197,23 @@
         <v>49</v>
       </c>
       <c r="B50" s="6">
+        <f>'2018-Full'!B50</f>
         <v>217123</v>
       </c>
       <c r="C50" s="6">
+        <f>'2018-Full'!C50</f>
         <v>537767</v>
       </c>
       <c r="D50" s="6">
+        <f>'2018-Full'!D50</f>
         <v>139943</v>
       </c>
       <c r="E50" s="6">
+        <f>'2018-Full'!E50</f>
         <v>677710</v>
       </c>
       <c r="F50" s="7">
+        <f>'2018-Full'!H50</f>
         <v>9222900</v>
       </c>
     </row>
@@ -23209,18 +23222,23 @@
         <v>50</v>
       </c>
       <c r="B51" s="6">
+        <f>'2018-Full'!B51</f>
         <v>130304</v>
       </c>
       <c r="C51" s="6">
+        <f>'2018-Full'!C51</f>
         <v>176549</v>
       </c>
       <c r="D51" s="6">
+        <f>'2018-Full'!D51</f>
         <v>71365</v>
       </c>
       <c r="E51" s="6">
+        <f>'2018-Full'!E51</f>
         <v>247914</v>
       </c>
       <c r="F51" s="7">
+        <f>'2018-Full'!H51</f>
         <v>24872972</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish writeup for residents vs non-residents
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="12" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="19" r:id="rId1"/>
@@ -1066,7 +1066,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1105,6 +1105,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -12099,10 +12100,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -13641,6 +13642,12 @@
         <f t="shared" si="0"/>
         <v>-2.8354934897694615</v>
       </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="I53" s="18"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="I54" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21959,7 +21966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Remove calculated cost factor for 2018
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D09F8E-D488-3A4E-8860-3577D810543C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A0284-9E48-C54E-9EA3-39746F45BC0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="156">
   <si>
     <r>
       <rPr>
@@ -949,19 +949,15 @@
   <si>
     <t>Total Licenses</t>
   </si>
-  <si>
-    <t>Non-resident Cost Factor</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1010,7 +1006,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1031,17 +1027,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1067,7 +1052,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1102,11 +1087,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1186,7 +1167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1238,7 +1219,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11058,9 +11039,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11068,7 +11051,7 @@
     <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -11088,7 +11071,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -11107,8 +11090,9 @@
       <c r="F2" s="9">
         <v>8684287.2599999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -11127,8 +11111,9 @@
       <c r="F3" s="9">
         <v>9111160</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -11147,8 +11132,9 @@
       <c r="F4" s="9">
         <v>12825689</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -11167,8 +11153,9 @@
       <c r="F5" s="9">
         <v>10892826</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -11187,8 +11174,9 @@
       <c r="F6" s="9">
         <v>15777132</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -11207,8 +11195,9 @@
       <c r="F7" s="9">
         <v>52158932</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -11227,8 +11216,9 @@
       <c r="F8" s="9">
         <v>1696858</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -11247,8 +11237,9 @@
       <c r="F9" s="9">
         <v>569656.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -11267,8 +11258,9 @@
       <c r="F10" s="9">
         <v>4816008</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -11287,8 +11279,9 @@
       <c r="F11" s="9">
         <v>13643071</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -11307,8 +11300,9 @@
       <c r="F12" s="9">
         <v>185605</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -11327,8 +11321,9 @@
       <c r="F13" s="9">
         <v>14380536</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -11347,8 +11342,9 @@
       <c r="F14" s="9">
         <v>20864108.460000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -11367,8 +11363,9 @@
       <c r="F15" s="9">
         <v>14403458</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -11387,6 +11384,7 @@
       <c r="F16" s="9">
         <v>7899606</v>
       </c>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
@@ -12101,18 +12099,16 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12137,11 +12133,8 @@
       <c r="H1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -12166,13 +12159,9 @@
       <c r="H2" s="7">
         <v>8491593</v>
       </c>
-      <c r="I2" s="17">
-        <f>IF(G2&gt;F2, -G2/F2, F2/G2)</f>
-        <v>-1.9054012533650484</v>
-      </c>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -12197,13 +12186,9 @@
       <c r="H3" s="7">
         <v>11801451</v>
       </c>
-      <c r="I3" s="17">
-        <f t="shared" ref="I3:I51" si="0">IF(G3&gt;F3, -G3/F3, F3/G3)</f>
-        <v>-1.0727085248450314</v>
-      </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -12228,13 +12213,9 @@
       <c r="H4" s="7">
         <v>18765517</v>
       </c>
-      <c r="I4" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.2923643587414124</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -12259,12 +12240,8 @@
       <c r="H5" s="7">
         <v>17874083</v>
       </c>
-      <c r="I5" s="17">
-        <f t="shared" si="0"/>
-        <v>2.9581385718524817</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -12289,12 +12266,8 @@
       <c r="H6" s="7">
         <v>21615994</v>
       </c>
-      <c r="I6" s="17">
-        <f t="shared" si="0"/>
-        <v>20.481050043625942</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -12319,12 +12292,8 @@
       <c r="H7" s="7">
         <v>57056595</v>
       </c>
-      <c r="I7" s="17">
-        <f t="shared" si="0"/>
-        <v>-3.4746332910939133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -12349,12 +12318,8 @@
       <c r="H8" s="7">
         <v>2480317</v>
       </c>
-      <c r="I8" s="17">
-        <f t="shared" si="0"/>
-        <v>5.2800784909482212</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -12379,12 +12344,8 @@
       <c r="H9" s="7">
         <v>1005204</v>
       </c>
-      <c r="I9" s="17">
-        <f t="shared" si="0"/>
-        <v>1.6988095429869357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -12409,12 +12370,8 @@
       <c r="H10" s="7">
         <v>8874919</v>
       </c>
-      <c r="I10" s="17">
-        <f t="shared" si="0"/>
-        <v>8.0189424926653725</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -12439,12 +12396,8 @@
       <c r="H11" s="7">
         <v>13759765</v>
       </c>
-      <c r="I11" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.0762163991606268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -12469,12 +12422,8 @@
       <c r="H12" s="7">
         <v>578355</v>
       </c>
-      <c r="I12" s="17">
-        <f t="shared" si="0"/>
-        <v>6.5042818217205136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -12499,12 +12448,8 @@
       <c r="H13" s="7">
         <v>17713256</v>
       </c>
-      <c r="I13" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5520389867198785</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -12529,12 +12474,8 @@
       <c r="H14" s="7">
         <v>25655741</v>
       </c>
-      <c r="I14" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.453953333286784</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -12559,12 +12500,8 @@
       <c r="H15" s="7">
         <v>31945215</v>
       </c>
-      <c r="I15" s="17">
-        <f t="shared" si="0"/>
-        <v>1.0582210736838185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -12589,12 +12526,8 @@
       <c r="H16" s="7">
         <v>11659245</v>
       </c>
-      <c r="I16" s="17">
-        <f t="shared" si="0"/>
-        <v>4.0671373991559152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -12619,12 +12552,8 @@
       <c r="H17" s="7">
         <v>19436612</v>
       </c>
-      <c r="I17" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.886999139393583</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -12649,12 +12578,8 @@
       <c r="H18" s="7">
         <v>19787571</v>
       </c>
-      <c r="I18" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5606429905148818</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -12679,12 +12604,8 @@
       <c r="H19" s="7">
         <v>9997994</v>
       </c>
-      <c r="I19" s="17">
-        <f t="shared" si="0"/>
-        <v>3.8917718078576637</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -12709,12 +12630,8 @@
       <c r="H20" s="7">
         <v>2406096</v>
       </c>
-      <c r="I20" s="17">
-        <f t="shared" si="0"/>
-        <v>5.0705273276364489</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -12739,12 +12656,8 @@
       <c r="H21" s="7">
         <v>6369051</v>
       </c>
-      <c r="I21" s="17">
-        <f t="shared" si="0"/>
-        <v>1.1412151878818075</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -12769,12 +12682,8 @@
       <c r="H22" s="7">
         <v>7871779</v>
       </c>
-      <c r="I22" s="17">
-        <f t="shared" si="0"/>
-        <v>1.4321151406507697</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -12799,12 +12708,8 @@
       <c r="H23" s="7">
         <v>37054782</v>
       </c>
-      <c r="I23" s="17">
-        <f t="shared" si="0"/>
-        <v>8.1590329408269362</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -12829,12 +12734,8 @@
       <c r="H24" s="7">
         <v>30725174</v>
       </c>
-      <c r="I24" s="17">
-        <f t="shared" si="0"/>
-        <v>7.7894849462507088</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -12859,12 +12760,8 @@
       <c r="H25" s="7">
         <v>21293840</v>
       </c>
-      <c r="I25" s="17">
-        <f t="shared" si="0"/>
-        <v>1.4451353280156349</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -12889,12 +12786,8 @@
       <c r="H26" s="7">
         <v>12272661</v>
       </c>
-      <c r="I26" s="17">
-        <f t="shared" si="0"/>
-        <v>-2.0501737998416343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -12919,12 +12812,8 @@
       <c r="H27" s="7">
         <v>32917709</v>
       </c>
-      <c r="I27" s="17">
-        <f t="shared" si="0"/>
-        <v>-2.4800065418527399</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -12949,12 +12838,8 @@
       <c r="H28" s="7">
         <v>10757714</v>
       </c>
-      <c r="I28" s="17">
-        <f t="shared" si="0"/>
-        <v>4.055471149259728</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -12979,12 +12864,8 @@
       <c r="H29" s="7">
         <v>11811245</v>
       </c>
-      <c r="I29" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.7739666830284484</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -13009,12 +12890,8 @@
       <c r="H30" s="7">
         <v>13501461</v>
       </c>
-      <c r="I30" s="17">
-        <f t="shared" si="0"/>
-        <v>1.2746171601799079</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -13039,12 +12916,8 @@
       <c r="H31" s="7">
         <v>4017347</v>
       </c>
-      <c r="I31" s="17">
-        <f t="shared" si="0"/>
-        <v>1.9304128994138952</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -13069,12 +12942,8 @@
       <c r="H32" s="7">
         <v>8128965</v>
       </c>
-      <c r="I32" s="17">
-        <f t="shared" si="0"/>
-        <v>6.0826087183812305</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -13099,12 +12968,8 @@
       <c r="H33" s="7">
         <v>16185652</v>
       </c>
-      <c r="I33" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.7591049779681089</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -13129,12 +12994,8 @@
       <c r="H34" s="7">
         <v>7750384</v>
       </c>
-      <c r="I34" s="17">
-        <f t="shared" si="0"/>
-        <v>1.0236095227651318</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -13159,12 +13020,8 @@
       <c r="H35" s="7">
         <v>21618296</v>
       </c>
-      <c r="I35" s="17">
-        <f t="shared" si="0"/>
-        <v>4.175289277664664</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -13189,12 +13046,8 @@
       <c r="H36" s="7">
         <v>22637955</v>
       </c>
-      <c r="I36" s="17">
-        <f t="shared" si="0"/>
-        <v>2.5488940371313067</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -13219,12 +13072,8 @@
       <c r="H37" s="7">
         <v>9606348</v>
       </c>
-      <c r="I37" s="17">
-        <f t="shared" si="0"/>
-        <v>1.4817968116034137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -13249,12 +13098,8 @@
       <c r="H38" s="7">
         <v>26399473</v>
       </c>
-      <c r="I38" s="17">
-        <f t="shared" si="0"/>
-        <v>3.8736558871799982</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -13279,12 +13124,8 @@
       <c r="H39" s="7">
         <v>36431816</v>
       </c>
-      <c r="I39" s="17">
-        <f t="shared" si="0"/>
-        <v>4.9926565242350822</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -13309,12 +13150,8 @@
       <c r="H40" s="7">
         <v>483576</v>
       </c>
-      <c r="I40" s="17">
-        <f t="shared" si="0"/>
-        <v>2.9806063399817257</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="41" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -13339,12 +13176,8 @@
       <c r="H41" s="7">
         <v>9717318</v>
       </c>
-      <c r="I41" s="17">
-        <f t="shared" si="0"/>
-        <v>1.2687200047067921</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -13369,12 +13202,8 @@
       <c r="H42" s="7">
         <v>22061719</v>
       </c>
-      <c r="I42" s="17">
-        <f t="shared" si="0"/>
-        <v>-2.0697790167871548</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -13399,12 +13228,8 @@
       <c r="H43" s="7">
         <v>20720183</v>
       </c>
-      <c r="I43" s="17">
-        <f t="shared" si="0"/>
-        <v>4.594964090746708</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="44" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -13429,12 +13254,8 @@
       <c r="H44" s="7">
         <v>46217763</v>
       </c>
-      <c r="I44" s="17">
-        <f t="shared" si="0"/>
-        <v>3.1949715087561334</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -13459,12 +13280,8 @@
       <c r="H45" s="7">
         <v>16762036</v>
       </c>
-      <c r="I45" s="17">
-        <f t="shared" si="0"/>
-        <v>2.0226009351252991</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -13489,12 +13306,8 @@
       <c r="H46" s="7">
         <v>21304227</v>
       </c>
-      <c r="I46" s="17">
-        <f t="shared" si="0"/>
-        <v>4.5835388524094345</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -13519,12 +13332,8 @@
       <c r="H47" s="7">
         <v>3965555</v>
       </c>
-      <c r="I47" s="17">
-        <f t="shared" si="0"/>
-        <v>3.0058741230484829</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -13549,12 +13358,8 @@
       <c r="H48" s="7">
         <v>17191859</v>
       </c>
-      <c r="I48" s="17">
-        <f t="shared" si="0"/>
-        <v>15.186865106154205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -13579,12 +13384,8 @@
       <c r="H49" s="7">
         <v>41381372</v>
       </c>
-      <c r="I49" s="17">
-        <f t="shared" si="0"/>
-        <v>4.4379389186482134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -13609,12 +13410,8 @@
       <c r="H50" s="7">
         <v>9222900</v>
       </c>
-      <c r="I50" s="17">
-        <f t="shared" si="0"/>
-        <v>-1.1181977737897342</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -13639,16 +13436,6 @@
       <c r="H51" s="7">
         <v>24872972</v>
       </c>
-      <c r="I51" s="17">
-        <f t="shared" si="0"/>
-        <v>-2.8354934897694615</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="I53" s="18"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="I54" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17151,7 +16938,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
feat: add 2019 data, save maps as HTML
</commit_message>
<xml_diff>
--- a/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
+++ b/Participation/Data/NatlHuntingLicenseReportAllYearsClean.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE751DF-4B0A-C042-97E9-07CAA4B2D535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E5E73F-C6BC-E341-BFD2-C33C9B0390E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="15900" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="19" r:id="rId1"/>
@@ -28,7 +28,8 @@
     <sheet name="2004" sheetId="15" r:id="rId18"/>
     <sheet name="2003" sheetId="21" r:id="rId19"/>
     <sheet name="2018-Full" sheetId="20" r:id="rId20"/>
-    <sheet name="Notes" sheetId="16" r:id="rId21"/>
+    <sheet name="2019-Full" sheetId="22" r:id="rId21"/>
+    <sheet name="Notes" sheetId="16" r:id="rId22"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="168">
   <si>
     <r>
       <rPr>
@@ -579,6 +580,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -596,6 +598,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -613,6 +616,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -630,6 +634,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -647,6 +652,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -664,6 +670,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Verdana"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Tags, Permits, and Stamps</t>
     </r>
@@ -965,6 +972,57 @@
   <si>
     <t>15-Year</t>
   </si>
+  <si>
+    <t>2019 Gross Cost - Hunting Licenses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2019 Cost - Non-Resident Hunting Licenses,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tags, Permits, and Stamps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2019 Cost - Resident Hunting Licenses,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tags, Permits, and Stamps</t>
+    </r>
+  </si>
+  <si>
+    <t>2019 Total Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <t>2019 Non-Resident Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <t>2019 Resident Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <t>2019 Paid Hunting License Holders</t>
+  </si>
 </sst>
 </file>
 
@@ -1006,12 +1064,14 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1068,7 +1128,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1105,6 +1165,16 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1464,7 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
@@ -18284,6 +18354,1407 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EEEDA-FD0F-E04C-8886-F0260FA19D46}">
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>124330</v>
+      </c>
+      <c r="C2" s="19">
+        <v>399020</v>
+      </c>
+      <c r="D2" s="19">
+        <v>64755</v>
+      </c>
+      <c r="E2" s="19">
+        <v>463775</v>
+      </c>
+      <c r="F2" s="19">
+        <v>3930940</v>
+      </c>
+      <c r="G2" s="19">
+        <v>7272195</v>
+      </c>
+      <c r="H2" s="19">
+        <v>11203135</v>
+      </c>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>535933</v>
+      </c>
+      <c r="C3" s="19">
+        <v>526677</v>
+      </c>
+      <c r="D3" s="19">
+        <v>37476</v>
+      </c>
+      <c r="E3" s="19">
+        <v>564153</v>
+      </c>
+      <c r="F3" s="19">
+        <v>5642231</v>
+      </c>
+      <c r="G3" s="19">
+        <v>6203532</v>
+      </c>
+      <c r="H3" s="19">
+        <v>11845763</v>
+      </c>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>301240</v>
+      </c>
+      <c r="C4" s="19">
+        <v>366964</v>
+      </c>
+      <c r="D4" s="19">
+        <v>146870</v>
+      </c>
+      <c r="E4" s="19">
+        <v>513834</v>
+      </c>
+      <c r="F4" s="19">
+        <v>7934870</v>
+      </c>
+      <c r="G4" s="19">
+        <v>11089040</v>
+      </c>
+      <c r="H4" s="19">
+        <v>19023910</v>
+      </c>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>310392</v>
+      </c>
+      <c r="C5" s="19">
+        <v>459282</v>
+      </c>
+      <c r="D5" s="19">
+        <v>66499</v>
+      </c>
+      <c r="E5" s="19">
+        <v>525781</v>
+      </c>
+      <c r="F5" s="19">
+        <v>13375848.5</v>
+      </c>
+      <c r="G5" s="19">
+        <v>4612812.5</v>
+      </c>
+      <c r="H5" s="19">
+        <v>17988661</v>
+      </c>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19">
+        <v>279248</v>
+      </c>
+      <c r="C6" s="19">
+        <v>984465</v>
+      </c>
+      <c r="D6" s="19">
+        <v>21309</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1005774</v>
+      </c>
+      <c r="F6" s="19">
+        <v>20531241</v>
+      </c>
+      <c r="G6" s="19">
+        <v>999698</v>
+      </c>
+      <c r="H6" s="19">
+        <v>21530939</v>
+      </c>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19">
+        <v>298901</v>
+      </c>
+      <c r="C7" s="19">
+        <v>466449</v>
+      </c>
+      <c r="D7" s="19">
+        <v>113156</v>
+      </c>
+      <c r="E7" s="19">
+        <v>579605</v>
+      </c>
+      <c r="F7" s="19">
+        <v>13018692</v>
+      </c>
+      <c r="G7" s="19">
+        <v>48693308</v>
+      </c>
+      <c r="H7" s="19">
+        <v>61712000</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <v>35681</v>
+      </c>
+      <c r="C8" s="19">
+        <v>117052</v>
+      </c>
+      <c r="D8" s="19">
+        <v>4255</v>
+      </c>
+      <c r="E8" s="19">
+        <v>121307</v>
+      </c>
+      <c r="F8" s="19">
+        <v>2016814</v>
+      </c>
+      <c r="G8" s="19">
+        <v>382127</v>
+      </c>
+      <c r="H8" s="19">
+        <v>2398941</v>
+      </c>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19">
+        <v>17839</v>
+      </c>
+      <c r="C9" s="19">
+        <v>52380</v>
+      </c>
+      <c r="D9" s="19">
+        <v>7759</v>
+      </c>
+      <c r="E9" s="19">
+        <v>60139</v>
+      </c>
+      <c r="F9" s="19">
+        <v>628831</v>
+      </c>
+      <c r="G9" s="19">
+        <v>407779</v>
+      </c>
+      <c r="H9" s="19">
+        <v>1036610</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19">
+        <v>189038</v>
+      </c>
+      <c r="C10" s="19">
+        <v>301085</v>
+      </c>
+      <c r="D10" s="19">
+        <v>18238</v>
+      </c>
+      <c r="E10" s="19">
+        <v>319323</v>
+      </c>
+      <c r="F10" s="19">
+        <v>5837701</v>
+      </c>
+      <c r="G10" s="19">
+        <v>1031692</v>
+      </c>
+      <c r="H10" s="19">
+        <v>6869393</v>
+      </c>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19">
+        <v>684277</v>
+      </c>
+      <c r="C11" s="19">
+        <v>1296488</v>
+      </c>
+      <c r="D11" s="19">
+        <v>179099</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1475587</v>
+      </c>
+      <c r="F11" s="19">
+        <v>6906445</v>
+      </c>
+      <c r="G11" s="19">
+        <v>7468044</v>
+      </c>
+      <c r="H11" s="19">
+        <v>14374489</v>
+      </c>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
+        <v>10585</v>
+      </c>
+      <c r="C12" s="19">
+        <v>10889</v>
+      </c>
+      <c r="D12" s="19">
+        <v>923</v>
+      </c>
+      <c r="E12" s="19">
+        <v>11812</v>
+      </c>
+      <c r="F12" s="19">
+        <v>510581</v>
+      </c>
+      <c r="G12" s="19">
+        <v>96915</v>
+      </c>
+      <c r="H12" s="19">
+        <v>607496</v>
+      </c>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19">
+        <v>227761</v>
+      </c>
+      <c r="C13" s="19">
+        <v>590834</v>
+      </c>
+      <c r="D13" s="19">
+        <v>79713</v>
+      </c>
+      <c r="E13" s="19">
+        <v>670547</v>
+      </c>
+      <c r="F13" s="19">
+        <v>13354833</v>
+      </c>
+      <c r="G13" s="19">
+        <v>7022157</v>
+      </c>
+      <c r="H13" s="19">
+        <v>20376990</v>
+      </c>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19">
+        <v>295281</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1077304</v>
+      </c>
+      <c r="D14" s="19">
+        <v>161667</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1238971</v>
+      </c>
+      <c r="F14" s="19">
+        <v>10977864</v>
+      </c>
+      <c r="G14" s="19">
+        <v>16824154</v>
+      </c>
+      <c r="H14" s="19">
+        <v>27802018</v>
+      </c>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19">
+        <v>299614</v>
+      </c>
+      <c r="C15" s="19">
+        <v>1172506</v>
+      </c>
+      <c r="D15" s="19">
+        <v>78414</v>
+      </c>
+      <c r="E15" s="19">
+        <v>1250920</v>
+      </c>
+      <c r="F15" s="19">
+        <v>16060492</v>
+      </c>
+      <c r="G15" s="19">
+        <v>14423073</v>
+      </c>
+      <c r="H15" s="19">
+        <v>30483565</v>
+      </c>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19">
+        <v>259453</v>
+      </c>
+      <c r="C16" s="19">
+        <v>366101</v>
+      </c>
+      <c r="D16" s="19">
+        <v>21395</v>
+      </c>
+      <c r="E16" s="19">
+        <v>387496</v>
+      </c>
+      <c r="F16" s="19">
+        <v>9152999</v>
+      </c>
+      <c r="G16" s="19">
+        <v>2404856</v>
+      </c>
+      <c r="H16" s="19">
+        <v>11557855</v>
+      </c>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19">
+        <v>250877</v>
+      </c>
+      <c r="C17" s="19">
+        <v>331050</v>
+      </c>
+      <c r="D17" s="19">
+        <v>156150</v>
+      </c>
+      <c r="E17" s="19">
+        <v>487200</v>
+      </c>
+      <c r="F17" s="19">
+        <v>8205661</v>
+      </c>
+      <c r="G17" s="19">
+        <v>16575650</v>
+      </c>
+      <c r="H17" s="19">
+        <v>24781311</v>
+      </c>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19">
+        <v>346161</v>
+      </c>
+      <c r="C18" s="19">
+        <v>494892</v>
+      </c>
+      <c r="D18" s="19">
+        <v>109815</v>
+      </c>
+      <c r="E18" s="19">
+        <v>604707</v>
+      </c>
+      <c r="F18" s="19">
+        <v>11643339</v>
+      </c>
+      <c r="G18" s="19">
+        <v>8191923</v>
+      </c>
+      <c r="H18" s="19">
+        <v>19835262</v>
+      </c>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19">
+        <v>396233</v>
+      </c>
+      <c r="C19" s="19">
+        <v>572812</v>
+      </c>
+      <c r="D19" s="19">
+        <v>54198</v>
+      </c>
+      <c r="E19" s="19">
+        <v>627010</v>
+      </c>
+      <c r="F19" s="19">
+        <v>7524678</v>
+      </c>
+      <c r="G19" s="19">
+        <v>2078804</v>
+      </c>
+      <c r="H19" s="19">
+        <v>9603482</v>
+      </c>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="19">
+        <v>57970</v>
+      </c>
+      <c r="C20" s="19">
+        <v>244831</v>
+      </c>
+      <c r="D20" s="19">
+        <v>16138</v>
+      </c>
+      <c r="E20" s="19">
+        <v>260969</v>
+      </c>
+      <c r="F20" s="19">
+        <v>1991508</v>
+      </c>
+      <c r="G20" s="19">
+        <v>417246</v>
+      </c>
+      <c r="H20" s="19">
+        <v>2408754</v>
+      </c>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19">
+        <v>120814</v>
+      </c>
+      <c r="C21" s="19">
+        <v>281145</v>
+      </c>
+      <c r="D21" s="19">
+        <v>63594</v>
+      </c>
+      <c r="E21" s="19">
+        <v>344739</v>
+      </c>
+      <c r="F21" s="19">
+        <v>3353366</v>
+      </c>
+      <c r="G21" s="19">
+        <v>3091028</v>
+      </c>
+      <c r="H21" s="19">
+        <v>6444394</v>
+      </c>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="19">
+        <v>162065</v>
+      </c>
+      <c r="C22" s="19">
+        <v>211305</v>
+      </c>
+      <c r="D22" s="19">
+        <v>34087</v>
+      </c>
+      <c r="E22" s="19">
+        <v>245392</v>
+      </c>
+      <c r="F22" s="19">
+        <v>4693267</v>
+      </c>
+      <c r="G22" s="19">
+        <v>3197139</v>
+      </c>
+      <c r="H22" s="19">
+        <v>7890406</v>
+      </c>
+      <c r="I22" s="18"/>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19">
+        <v>685185</v>
+      </c>
+      <c r="C23" s="19">
+        <v>2117282</v>
+      </c>
+      <c r="D23" s="19">
+        <v>53829</v>
+      </c>
+      <c r="E23" s="19">
+        <v>2171111</v>
+      </c>
+      <c r="F23" s="19">
+        <v>32049336</v>
+      </c>
+      <c r="G23" s="19">
+        <v>4091668</v>
+      </c>
+      <c r="H23" s="19">
+        <v>36141004</v>
+      </c>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="19">
+        <v>563127</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1389256</v>
+      </c>
+      <c r="D24" s="19">
+        <v>44442</v>
+      </c>
+      <c r="E24" s="19">
+        <v>1433698</v>
+      </c>
+      <c r="F24" s="19">
+        <v>26912777</v>
+      </c>
+      <c r="G24" s="19">
+        <v>3550726</v>
+      </c>
+      <c r="H24" s="19">
+        <v>30463503</v>
+      </c>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="19">
+        <v>494030</v>
+      </c>
+      <c r="C25" s="19">
+        <v>1711087</v>
+      </c>
+      <c r="D25" s="19">
+        <v>86067</v>
+      </c>
+      <c r="E25" s="19">
+        <v>1797154</v>
+      </c>
+      <c r="F25" s="19">
+        <v>12361151</v>
+      </c>
+      <c r="G25" s="19">
+        <v>9137209</v>
+      </c>
+      <c r="H25" s="19">
+        <v>21498360</v>
+      </c>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="19">
+        <v>288325</v>
+      </c>
+      <c r="C26" s="19">
+        <v>313758</v>
+      </c>
+      <c r="D26" s="19">
+        <v>88591</v>
+      </c>
+      <c r="E26" s="19">
+        <v>402349</v>
+      </c>
+      <c r="F26" s="19">
+        <v>4584194</v>
+      </c>
+      <c r="G26" s="19">
+        <v>8123862</v>
+      </c>
+      <c r="H26" s="19">
+        <v>12708056</v>
+      </c>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="19">
+        <v>227039</v>
+      </c>
+      <c r="C27" s="19">
+        <v>901421</v>
+      </c>
+      <c r="D27" s="19">
+        <v>143786</v>
+      </c>
+      <c r="E27" s="19">
+        <v>1045207</v>
+      </c>
+      <c r="F27" s="19">
+        <v>12644970</v>
+      </c>
+      <c r="G27" s="19">
+        <v>26660255</v>
+      </c>
+      <c r="H27" s="19">
+        <v>39305225</v>
+      </c>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="19">
+        <v>592564</v>
+      </c>
+      <c r="C28" s="19">
+        <v>302549</v>
+      </c>
+      <c r="D28" s="19">
+        <v>25920</v>
+      </c>
+      <c r="E28" s="19">
+        <v>328469</v>
+      </c>
+      <c r="F28" s="19">
+        <v>8216289</v>
+      </c>
+      <c r="G28" s="19">
+        <v>2144055</v>
+      </c>
+      <c r="H28" s="19">
+        <v>10360344</v>
+      </c>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="19">
+        <v>141328</v>
+      </c>
+      <c r="C29" s="19">
+        <v>367976</v>
+      </c>
+      <c r="D29" s="19">
+        <v>152420</v>
+      </c>
+      <c r="E29" s="19">
+        <v>520396</v>
+      </c>
+      <c r="F29" s="19">
+        <v>4437098</v>
+      </c>
+      <c r="G29" s="19">
+        <v>7272505</v>
+      </c>
+      <c r="H29" s="19">
+        <v>11709603</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="19">
+        <v>185231</v>
+      </c>
+      <c r="C30" s="19">
+        <v>335659</v>
+      </c>
+      <c r="D30" s="19">
+        <v>92534</v>
+      </c>
+      <c r="E30" s="19">
+        <v>428193</v>
+      </c>
+      <c r="F30" s="19">
+        <v>8044372</v>
+      </c>
+      <c r="G30" s="19">
+        <v>6263193</v>
+      </c>
+      <c r="H30" s="19">
+        <v>14307565</v>
+      </c>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="19">
+        <v>57632</v>
+      </c>
+      <c r="C31" s="19">
+        <v>47073</v>
+      </c>
+      <c r="D31" s="19">
+        <v>10559</v>
+      </c>
+      <c r="E31" s="19">
+        <v>57632</v>
+      </c>
+      <c r="F31" s="19">
+        <v>3360985</v>
+      </c>
+      <c r="G31" s="19">
+        <v>1511187</v>
+      </c>
+      <c r="H31" s="19">
+        <v>4872172</v>
+      </c>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="19">
+        <v>73009</v>
+      </c>
+      <c r="C32" s="19">
+        <v>300067</v>
+      </c>
+      <c r="D32" s="19">
+        <v>110494</v>
+      </c>
+      <c r="E32" s="19">
+        <v>410561</v>
+      </c>
+      <c r="F32" s="19">
+        <v>6898845</v>
+      </c>
+      <c r="G32" s="19">
+        <v>1147938</v>
+      </c>
+      <c r="H32" s="19">
+        <v>8046783</v>
+      </c>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="19">
+        <v>106661</v>
+      </c>
+      <c r="C33" s="19">
+        <v>270158</v>
+      </c>
+      <c r="D33" s="19">
+        <v>85107</v>
+      </c>
+      <c r="E33" s="19">
+        <v>355265</v>
+      </c>
+      <c r="F33" s="19">
+        <v>5440500</v>
+      </c>
+      <c r="G33" s="19">
+        <v>10191120</v>
+      </c>
+      <c r="H33" s="19">
+        <v>15631620</v>
+      </c>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="19">
+        <v>69780</v>
+      </c>
+      <c r="C34" s="19">
+        <v>118703</v>
+      </c>
+      <c r="D34" s="19">
+        <v>27372</v>
+      </c>
+      <c r="E34" s="19">
+        <v>146075</v>
+      </c>
+      <c r="F34" s="19">
+        <v>3766841</v>
+      </c>
+      <c r="G34" s="19">
+        <v>3921638</v>
+      </c>
+      <c r="H34" s="19">
+        <v>7688479</v>
+      </c>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="19">
+        <v>564612</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1366205</v>
+      </c>
+      <c r="D35" s="19">
+        <v>48657</v>
+      </c>
+      <c r="E35" s="19">
+        <v>1414862</v>
+      </c>
+      <c r="F35" s="19">
+        <v>20501860</v>
+      </c>
+      <c r="G35" s="19">
+        <v>4153540</v>
+      </c>
+      <c r="H35" s="19">
+        <v>24655400</v>
+      </c>
+      <c r="I35" s="18"/>
+    </row>
+    <row r="36" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="19">
+        <v>376435</v>
+      </c>
+      <c r="C36" s="19">
+        <v>852411</v>
+      </c>
+      <c r="D36" s="19">
+        <v>103254</v>
+      </c>
+      <c r="E36" s="19">
+        <v>955665</v>
+      </c>
+      <c r="F36" s="19">
+        <v>15471071</v>
+      </c>
+      <c r="G36" s="19">
+        <v>6564109</v>
+      </c>
+      <c r="H36" s="19">
+        <v>22035180</v>
+      </c>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="19">
+        <v>541553</v>
+      </c>
+      <c r="C37" s="19">
+        <v>399528</v>
+      </c>
+      <c r="D37" s="19">
+        <v>24877</v>
+      </c>
+      <c r="E37" s="19">
+        <v>424405</v>
+      </c>
+      <c r="F37" s="19">
+        <v>5512848</v>
+      </c>
+      <c r="G37" s="19">
+        <v>4476328</v>
+      </c>
+      <c r="H37" s="19">
+        <v>9989176</v>
+      </c>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="19">
+        <v>335543</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1263376</v>
+      </c>
+      <c r="D38" s="19">
+        <v>62274</v>
+      </c>
+      <c r="E38" s="19">
+        <v>1325650</v>
+      </c>
+      <c r="F38" s="19">
+        <v>23059651</v>
+      </c>
+      <c r="G38" s="19">
+        <v>5921203</v>
+      </c>
+      <c r="H38" s="19">
+        <v>28980854</v>
+      </c>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="19">
+        <v>956163</v>
+      </c>
+      <c r="C39" s="19">
+        <v>2526957</v>
+      </c>
+      <c r="D39" s="19">
+        <v>103431</v>
+      </c>
+      <c r="E39" s="19">
+        <v>2630388</v>
+      </c>
+      <c r="F39" s="19">
+        <v>30970695</v>
+      </c>
+      <c r="G39" s="19">
+        <v>6090417</v>
+      </c>
+      <c r="H39" s="19">
+        <v>37061112</v>
+      </c>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="19">
+        <v>7414</v>
+      </c>
+      <c r="C40" s="19">
+        <v>25962</v>
+      </c>
+      <c r="D40" s="19">
+        <v>3967</v>
+      </c>
+      <c r="E40" s="19">
+        <v>29929</v>
+      </c>
+      <c r="F40" s="19">
+        <v>327832</v>
+      </c>
+      <c r="G40" s="19">
+        <v>113394</v>
+      </c>
+      <c r="H40" s="19">
+        <v>441226</v>
+      </c>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="19">
+        <v>200912</v>
+      </c>
+      <c r="C41" s="19">
+        <v>703738</v>
+      </c>
+      <c r="D41" s="19">
+        <v>88971</v>
+      </c>
+      <c r="E41" s="19">
+        <v>792709</v>
+      </c>
+      <c r="F41" s="19">
+        <v>4599067</v>
+      </c>
+      <c r="G41" s="19">
+        <v>4072719</v>
+      </c>
+      <c r="H41" s="19">
+        <v>8671786</v>
+      </c>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="19">
+        <v>229323</v>
+      </c>
+      <c r="C42" s="19">
+        <v>244044</v>
+      </c>
+      <c r="D42" s="19">
+        <v>124596</v>
+      </c>
+      <c r="E42" s="19">
+        <v>368640</v>
+      </c>
+      <c r="F42" s="19">
+        <v>7431919</v>
+      </c>
+      <c r="G42" s="19">
+        <v>14459943</v>
+      </c>
+      <c r="H42" s="19">
+        <v>21891862</v>
+      </c>
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="19">
+        <v>679038</v>
+      </c>
+      <c r="C43" s="19">
+        <v>580955</v>
+      </c>
+      <c r="D43" s="19">
+        <v>43710</v>
+      </c>
+      <c r="E43" s="19">
+        <v>624665</v>
+      </c>
+      <c r="F43" s="19">
+        <v>15881299</v>
+      </c>
+      <c r="G43" s="19">
+        <v>4201071</v>
+      </c>
+      <c r="H43" s="19">
+        <v>20082370</v>
+      </c>
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="19">
+        <v>1162430</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1589078</v>
+      </c>
+      <c r="D44" s="19">
+        <v>85597</v>
+      </c>
+      <c r="E44" s="19">
+        <v>1674675</v>
+      </c>
+      <c r="F44" s="19">
+        <v>35414251</v>
+      </c>
+      <c r="G44" s="19">
+        <v>11507905</v>
+      </c>
+      <c r="H44" s="19">
+        <v>46922156</v>
+      </c>
+      <c r="I44" s="18"/>
+    </row>
+    <row r="45" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="19">
+        <v>244131</v>
+      </c>
+      <c r="C45" s="19">
+        <v>404413</v>
+      </c>
+      <c r="D45" s="19">
+        <v>44425</v>
+      </c>
+      <c r="E45" s="19">
+        <v>448838</v>
+      </c>
+      <c r="F45" s="19">
+        <v>11461931</v>
+      </c>
+      <c r="G45" s="19">
+        <v>5950216</v>
+      </c>
+      <c r="H45" s="19">
+        <v>17412147</v>
+      </c>
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="19">
+        <v>268300</v>
+      </c>
+      <c r="C46" s="19">
+        <v>789170</v>
+      </c>
+      <c r="D46" s="19">
+        <v>43029</v>
+      </c>
+      <c r="E46" s="19">
+        <v>832199</v>
+      </c>
+      <c r="F46" s="19">
+        <v>17441649</v>
+      </c>
+      <c r="G46" s="19">
+        <v>3780222</v>
+      </c>
+      <c r="H46" s="19">
+        <v>21221871</v>
+      </c>
+      <c r="I46" s="18"/>
+    </row>
+    <row r="47" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="19">
+        <v>67619</v>
+      </c>
+      <c r="C47" s="19">
+        <v>162299</v>
+      </c>
+      <c r="D47" s="19">
+        <v>16510</v>
+      </c>
+      <c r="E47" s="19">
+        <v>178809</v>
+      </c>
+      <c r="F47" s="19">
+        <v>3029366</v>
+      </c>
+      <c r="G47" s="19">
+        <v>1014738</v>
+      </c>
+      <c r="H47" s="19">
+        <v>4044104</v>
+      </c>
+      <c r="I47" s="18"/>
+    </row>
+    <row r="48" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="19">
+        <v>179316</v>
+      </c>
+      <c r="C48" s="19">
+        <v>702296</v>
+      </c>
+      <c r="D48" s="19">
+        <v>9506</v>
+      </c>
+      <c r="E48" s="19">
+        <v>711802</v>
+      </c>
+      <c r="F48" s="19">
+        <v>16200536</v>
+      </c>
+      <c r="G48" s="19">
+        <v>1032455</v>
+      </c>
+      <c r="H48" s="19">
+        <v>17232991</v>
+      </c>
+      <c r="I48" s="18"/>
+    </row>
+    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="19">
+        <v>692209</v>
+      </c>
+      <c r="C49" s="19">
+        <v>418349</v>
+      </c>
+      <c r="D49" s="19">
+        <v>1294207</v>
+      </c>
+      <c r="E49" s="19">
+        <v>1712556</v>
+      </c>
+      <c r="F49" s="19">
+        <v>11266763</v>
+      </c>
+      <c r="G49" s="19">
+        <v>27390894</v>
+      </c>
+      <c r="H49" s="19">
+        <v>38657657</v>
+      </c>
+      <c r="I49" s="18"/>
+    </row>
+    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="19">
+        <v>213656</v>
+      </c>
+      <c r="C50" s="19">
+        <v>519105</v>
+      </c>
+      <c r="D50" s="19">
+        <v>142397</v>
+      </c>
+      <c r="E50" s="19">
+        <v>661502</v>
+      </c>
+      <c r="F50" s="19">
+        <v>4103901</v>
+      </c>
+      <c r="G50" s="19">
+        <v>4920855</v>
+      </c>
+      <c r="H50" s="19">
+        <v>9024756</v>
+      </c>
+      <c r="I50" s="18"/>
+    </row>
+    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="19">
+        <v>132075</v>
+      </c>
+      <c r="C51" s="19">
+        <v>179864</v>
+      </c>
+      <c r="D51" s="19">
+        <v>74048</v>
+      </c>
+      <c r="E51" s="19">
+        <v>253912</v>
+      </c>
+      <c r="F51" s="19">
+        <v>6554885</v>
+      </c>
+      <c r="G51" s="19">
+        <v>19004047</v>
+      </c>
+      <c r="H51" s="19">
+        <v>25558932</v>
+      </c>
+      <c r="I51" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>

</xml_diff>